<commit_message>
New code for CUCD/NUCD
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skold\Dropbox\Projekt\MoCiS2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58596CDB-949F-46EA-958F-557DBB8BD977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519ED7C1-0279-428F-93C1-3F3F41A3E103}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29010" yWindow="-6690" windowWidth="26490" windowHeight="11385" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
     <sheet name="ARTER" sheetId="15" r:id="rId2"/>
     <sheet name="PARAMETRAR" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1111,12 +1111,6 @@
     <t>CH02/90</t>
   </si>
   <si>
-    <t>CUCD</t>
-  </si>
-  <si>
-    <t>NUCD</t>
-  </si>
-  <si>
     <t>D15NUCD</t>
   </si>
   <si>
@@ -1878,6 +1872,12 @@
   <si>
     <t>TOTVH</t>
   </si>
+  <si>
+    <t>CUCDTPRC</t>
+  </si>
+  <si>
+    <t>NUCDTPRC</t>
+  </si>
 </sst>
 </file>
 
@@ -2384,13 +2384,13 @@
         <v>108</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2401,10 +2401,10 @@
         <v>110</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2415,10 +2415,10 @@
         <v>110</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2429,10 +2429,10 @@
         <v>112</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2443,10 +2443,10 @@
         <v>112</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2457,10 +2457,10 @@
         <v>114</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2471,10 +2471,10 @@
         <v>114</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2485,10 +2485,10 @@
         <v>116</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2499,10 +2499,10 @@
         <v>116</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2530,7 +2530,7 @@
         <v>122</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2600,7 +2600,7 @@
         <v>134</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,7 +2726,7 @@
         <v>161</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2745,7 +2745,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>121</v>
@@ -2754,7 +2754,7 @@
         <v>122</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2801,7 +2801,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>160</v>
@@ -2810,7 +2810,7 @@
         <v>161</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2866,7 +2866,7 @@
         <v>173</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2930,7 +2930,7 @@
         <v>180</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>181</v>
@@ -2955,464 +2955,464 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>428</v>
-      </c>
       <c r="C42" s="10" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>435</v>
-      </c>
       <c r="C44" s="10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>438</v>
-      </c>
       <c r="C45" s="10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>441</v>
-      </c>
       <c r="C46" s="10" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="B47" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="B47" s="11" t="s">
-        <v>444</v>
-      </c>
       <c r="C47" s="10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>447</v>
-      </c>
       <c r="C48" s="10" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="B49" s="11" t="s">
         <v>448</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>450</v>
-      </c>
       <c r="C49" s="10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>453</v>
-      </c>
       <c r="C50" s="10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="B51" s="11" t="s">
-        <v>456</v>
-      </c>
       <c r="C51" s="10" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>459</v>
-      </c>
       <c r="C52" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="B53" s="11" t="s">
-        <v>462</v>
-      </c>
       <c r="C53" s="10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="B54" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>465</v>
-      </c>
       <c r="C54" s="10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="B55" s="11" t="s">
-        <v>468</v>
-      </c>
       <c r="C55" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="B56" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="B56" s="11" t="s">
-        <v>471</v>
-      </c>
       <c r="C56" s="10" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="B57" s="11" t="s">
-        <v>474</v>
-      </c>
       <c r="C57" s="10" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="B58" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="B58" s="11" t="s">
-        <v>477</v>
-      </c>
       <c r="C58" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="B59" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>477</v>
-      </c>
       <c r="C59" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="B60" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="B60" s="11" t="s">
-        <v>480</v>
-      </c>
       <c r="C60" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="B61" s="11" t="s">
         <v>481</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>483</v>
-      </c>
       <c r="C61" s="10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>486</v>
-      </c>
       <c r="C62" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>487</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>489</v>
-      </c>
       <c r="C63" s="10" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="B64" s="11" t="s">
         <v>490</v>
       </c>
-      <c r="B64" s="11" t="s">
-        <v>492</v>
-      </c>
       <c r="C64" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="B65" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="B65" s="11" t="s">
-        <v>495</v>
-      </c>
       <c r="C65" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>496</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>498</v>
-      </c>
       <c r="C66" s="10" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="B67" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>501</v>
-      </c>
       <c r="C67" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="B68" s="11" t="s">
         <v>502</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>504</v>
-      </c>
       <c r="C68" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="B69" s="11" t="s">
         <v>505</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>507</v>
-      </c>
       <c r="C69" s="10" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="B70" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>510</v>
-      </c>
       <c r="C70" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="B71" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="B71" s="11" t="s">
-        <v>513</v>
-      </c>
       <c r="C71" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="B72" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>516</v>
-      </c>
       <c r="C72" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="B73" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="B73" s="11" t="s">
-        <v>519</v>
-      </c>
       <c r="C73" s="10" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="B74" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="B74" s="11" t="s">
-        <v>522</v>
-      </c>
       <c r="C74" s="10" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -3439,10 +3439,10 @@
         <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3456,7 +3456,7 @@
         <v>206198</v>
       </c>
       <c r="D2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3470,7 +3470,7 @@
         <v>218387</v>
       </c>
       <c r="D3" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3484,12 +3484,12 @@
         <v>102618</v>
       </c>
       <c r="D4" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -3498,12 +3498,12 @@
         <v>206139</v>
       </c>
       <c r="D5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -3512,7 +3512,7 @@
         <v>206231</v>
       </c>
       <c r="D6" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3526,7 +3526,7 @@
         <v>100144</v>
       </c>
       <c r="D7" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3540,7 +3540,7 @@
         <v>102950</v>
       </c>
       <c r="D8" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3548,13 +3548,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C9">
         <v>206293</v>
       </c>
       <c r="D9" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3568,7 +3568,7 @@
         <v>206142</v>
       </c>
       <c r="D10" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3576,13 +3576,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C11">
         <v>206089</v>
       </c>
       <c r="D11" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -3599,7 +3599,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D121" sqref="D121"/>
+      <selection pane="bottomLeft" activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,7 +3625,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>16</v>
@@ -3634,51 +3634,51 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>573</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>396</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>408</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>397</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>575</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>398</v>
-      </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>399</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>18</v>
@@ -3687,22 +3687,22 @@
         <v>19</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -3716,22 +3716,22 @@
         <v>22</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -3745,22 +3745,22 @@
         <v>25</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3774,22 +3774,22 @@
         <v>28</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -3803,22 +3803,22 @@
         <v>31</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -3832,22 +3832,22 @@
         <v>34</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -3861,22 +3861,22 @@
         <v>37</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -3890,22 +3890,22 @@
         <v>40</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3919,22 +3919,22 @@
         <v>53</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -3948,22 +3948,22 @@
         <v>55</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -3977,22 +3977,22 @@
         <v>57</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -4006,51 +4006,51 @@
         <v>59</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>589</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>590</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>591</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>592</v>
-      </c>
       <c r="G14" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -4064,22 +4064,22 @@
         <v>61</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -4093,22 +4093,22 @@
         <v>63</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -4122,22 +4122,22 @@
         <v>65</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -4151,22 +4151,22 @@
         <v>67</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -4180,51 +4180,51 @@
         <v>69</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>524</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>525</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>526</v>
-      </c>
       <c r="G20" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -4238,22 +4238,22 @@
         <v>71</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -4267,22 +4267,22 @@
         <v>73</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -4296,80 +4296,80 @@
         <v>75</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>76</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>77</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -4377,28 +4377,28 @@
         <v>78</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>79</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -4406,28 +4406,28 @@
         <v>80</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>81</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -4435,178 +4435,178 @@
         <v>82</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>83</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>84</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>85</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>86</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>87</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>88</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>89</v>
@@ -4615,27 +4615,27 @@
         <v>90</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K34" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>91</v>
@@ -4644,56 +4644,56 @@
         <v>92</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>93</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>94</v>
@@ -4702,27 +4702,27 @@
         <v>95</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>96</v>
@@ -4731,27 +4731,27 @@
         <v>97</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>98</v>
@@ -4760,27 +4760,27 @@
         <v>99</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>100</v>
@@ -4789,27 +4789,27 @@
         <v>101</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>102</v>
@@ -4818,27 +4818,27 @@
         <v>103</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>104</v>
@@ -4847,22 +4847,22 @@
         <v>105</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -4876,22 +4876,22 @@
         <v>187</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K43" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -4905,22 +4905,22 @@
         <v>190</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -4934,22 +4934,22 @@
         <v>193</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -4963,22 +4963,22 @@
         <v>196</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -4992,22 +4992,22 @@
         <v>199</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -5021,22 +5021,22 @@
         <v>202</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K48" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L48" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -5050,22 +5050,22 @@
         <v>205</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L49" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -5079,22 +5079,22 @@
         <v>208</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J50" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -5108,22 +5108,22 @@
         <v>211</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -5137,22 +5137,22 @@
         <v>214</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J52" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K52" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L52" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -5166,22 +5166,22 @@
         <v>217</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K53" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -5195,22 +5195,22 @@
         <v>220</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I54" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K54" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L54" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -5224,22 +5224,22 @@
         <v>223</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I55" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K55" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L55" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -5253,22 +5253,22 @@
         <v>226</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I56" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K56" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L56" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -5282,22 +5282,22 @@
         <v>229</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I57" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K57" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L57" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -5311,22 +5311,22 @@
         <v>232</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I58" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K58" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L58" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -5340,22 +5340,22 @@
         <v>235</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I59" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K59" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -5369,22 +5369,22 @@
         <v>237</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J60" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L60" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -5398,22 +5398,22 @@
         <v>239</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J61" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K61" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -5427,22 +5427,22 @@
         <v>241</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J62" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K62" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L62" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -5456,22 +5456,22 @@
         <v>243</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J63" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K63" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L63" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -5485,22 +5485,22 @@
         <v>245</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L64" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -5514,22 +5514,22 @@
         <v>247</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I65" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J65" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K65" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L65" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -5543,22 +5543,22 @@
         <v>249</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I66" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J66" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K66" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L66" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -5572,22 +5572,22 @@
         <v>251</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J67" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L67" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -5601,22 +5601,22 @@
         <v>253</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I68" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J68" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K68" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L68" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -5630,22 +5630,22 @@
         <v>255</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I69" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J69" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K69" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L69" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -5659,22 +5659,22 @@
         <v>257</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J70" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K70" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L70" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -5688,22 +5688,22 @@
         <v>259</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J71" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K71" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L71" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -5717,22 +5717,22 @@
         <v>261</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J72" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K72" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L72" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -5746,22 +5746,22 @@
         <v>263</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J73" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K73" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L73" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -5775,27 +5775,27 @@
         <v>265</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J74" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K74" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="L74" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>266</v>
@@ -5807,22 +5807,22 @@
       <c r="E75" s="13"/>
       <c r="F75" s="9"/>
       <c r="G75" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I75" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J75" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K75" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L75" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H75" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I75" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J75" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K75" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L75" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M75" s="8"/>
       <c r="N75" s="8"/>
@@ -5832,7 +5832,7 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>268</v>
@@ -5844,22 +5844,22 @@
       <c r="E76" s="13"/>
       <c r="F76" s="9"/>
       <c r="G76" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I76" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J76" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K76" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L76" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H76" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I76" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J76" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K76" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L76" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M76" s="8"/>
       <c r="N76" s="8"/>
@@ -5869,7 +5869,7 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>270</v>
@@ -5881,22 +5881,22 @@
       <c r="E77" s="13"/>
       <c r="F77" s="9"/>
       <c r="G77" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I77" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J77" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K77" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L77" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H77" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I77" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J77" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K77" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L77" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M77" s="8"/>
       <c r="N77" s="8"/>
@@ -5906,7 +5906,7 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>272</v>
@@ -5918,22 +5918,22 @@
       <c r="E78" s="13"/>
       <c r="F78" s="9"/>
       <c r="G78" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H78" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I78" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J78" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K78" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L78" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H78" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I78" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J78" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K78" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L78" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M78" s="8"/>
       <c r="N78" s="8"/>
@@ -5955,22 +5955,22 @@
       <c r="E79" s="13"/>
       <c r="F79" s="9"/>
       <c r="G79" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I79" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J79" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K79" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L79" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H79" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I79" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J79" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K79" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L79" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M79" s="8"/>
       <c r="N79" s="8"/>
@@ -5992,22 +5992,22 @@
       <c r="E80" s="13"/>
       <c r="F80" s="9"/>
       <c r="G80" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I80" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J80" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K80" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L80" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H80" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I80" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J80" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K80" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L80" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M80" s="8"/>
       <c r="N80" s="8"/>
@@ -6029,22 +6029,22 @@
       <c r="E81" s="13"/>
       <c r="F81" s="9"/>
       <c r="G81" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J81" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K81" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L81" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H81" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I81" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J81" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K81" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L81" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M81" s="8"/>
       <c r="N81" s="8"/>
@@ -6066,22 +6066,22 @@
       <c r="E82" s="13"/>
       <c r="F82" s="9"/>
       <c r="G82" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J82" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K82" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L82" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H82" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I82" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J82" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K82" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L82" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M82" s="8"/>
       <c r="N82" s="8"/>
@@ -6103,22 +6103,22 @@
       <c r="E83" s="13"/>
       <c r="F83" s="9"/>
       <c r="G83" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I83" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J83" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K83" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L83" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H83" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I83" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J83" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K83" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L83" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M83" s="8"/>
       <c r="N83" s="8"/>
@@ -6140,22 +6140,22 @@
       <c r="E84" s="13"/>
       <c r="F84" s="9"/>
       <c r="G84" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H84" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I84" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J84" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K84" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L84" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H84" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I84" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J84" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K84" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L84" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M84" s="8"/>
       <c r="N84" s="8"/>
@@ -6177,22 +6177,22 @@
       <c r="E85" s="13"/>
       <c r="F85" s="9"/>
       <c r="G85" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I85" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J85" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K85" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L85" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H85" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I85" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J85" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K85" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L85" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M85" s="8"/>
       <c r="N85" s="8"/>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>288</v>
@@ -6214,22 +6214,22 @@
       <c r="E86" s="13"/>
       <c r="F86" s="9"/>
       <c r="G86" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H86" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I86" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J86" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K86" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L86" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H86" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I86" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J86" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K86" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L86" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M86" s="8"/>
       <c r="N86" s="8"/>
@@ -6239,7 +6239,7 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>290</v>
@@ -6251,22 +6251,22 @@
       <c r="E87" s="13"/>
       <c r="F87" s="9"/>
       <c r="G87" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I87" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J87" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K87" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L87" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H87" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I87" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J87" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K87" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L87" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M87" s="8"/>
       <c r="N87" s="8"/>
@@ -6288,22 +6288,22 @@
       <c r="E88" s="13"/>
       <c r="F88" s="9"/>
       <c r="G88" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="H88" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I88" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J88" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="K88" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="L88" s="13" t="s">
         <v>400</v>
-      </c>
-      <c r="H88" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I88" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="J88" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="K88" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="L88" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="M88" s="8"/>
       <c r="N88" s="8"/>
@@ -6322,22 +6322,22 @@
         <v>295</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J89" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K89" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L89" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
@@ -6351,22 +6351,22 @@
         <v>297</v>
       </c>
       <c r="G90" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J90" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K90" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L90" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
@@ -6380,22 +6380,22 @@
         <v>303</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J91" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K91" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L91" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
@@ -6409,27 +6409,27 @@
         <v>305</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J92" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K92" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L92" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>286</v>
@@ -6438,22 +6438,22 @@
         <v>287</v>
       </c>
       <c r="G93" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J93" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K93" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L93" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
@@ -6467,22 +6467,22 @@
         <v>307</v>
       </c>
       <c r="G94" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I94" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J94" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K94" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L94" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
@@ -6496,22 +6496,22 @@
         <v>299</v>
       </c>
       <c r="G95" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I95" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J95" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K95" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L95" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
@@ -6525,22 +6525,22 @@
         <v>309</v>
       </c>
       <c r="G96" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I96" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J96" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L96" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
@@ -6554,22 +6554,22 @@
         <v>311</v>
       </c>
       <c r="G97" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I97" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J97" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L97" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
@@ -6583,22 +6583,22 @@
         <v>313</v>
       </c>
       <c r="G98" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I98" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J98" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
@@ -6612,22 +6612,22 @@
         <v>301</v>
       </c>
       <c r="G99" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I99" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J99" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L99" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
@@ -6641,27 +6641,27 @@
         <v>315</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I100" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J100" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L100" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B101" s="15" t="s">
         <v>351</v>
@@ -6670,24 +6670,24 @@
         <v>352</v>
       </c>
       <c r="E101" s="22" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="J101" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="K101" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="L101" s="15" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="21" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B102" s="15" t="s">
         <v>353</v>
@@ -6696,24 +6696,24 @@
         <v>354</v>
       </c>
       <c r="E102" s="22" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J102" s="15" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="K102" s="15" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="L102" s="15" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
-        <v>359</v>
+        <v>613</v>
       </c>
       <c r="B103" s="15" t="s">
         <v>355</v>
@@ -6722,20 +6722,20 @@
         <v>356</v>
       </c>
       <c r="E103" s="22" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G103" s="16" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J103" s="23"/>
       <c r="K103" s="23"/>
       <c r="L103" s="15" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
-        <v>360</v>
+        <v>614</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>357</v>
@@ -6744,47 +6744,47 @@
         <v>358</v>
       </c>
       <c r="E104" s="22" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G104" s="16" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J104" s="23"/>
       <c r="K104" s="23"/>
       <c r="L104" s="15" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="13"/>
       <c r="F105" s="8"/>
       <c r="G105" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I105" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J105" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K105" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L105" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M105" s="8"/>
       <c r="N105" s="8"/>
@@ -6794,34 +6794,34 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D106" s="8"/>
       <c r="E106" s="13"/>
       <c r="F106" s="8"/>
       <c r="G106" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H106" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I106" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J106" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K106" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L106" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M106" s="8"/>
       <c r="N106" s="8"/>
@@ -6831,34 +6831,34 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D107" s="8"/>
       <c r="E107" s="13"/>
       <c r="F107" s="8"/>
       <c r="G107" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I107" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J107" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K107" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L107" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M107" s="8"/>
       <c r="N107" s="8"/>
@@ -6868,34 +6868,34 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D108" s="8"/>
       <c r="E108" s="13"/>
       <c r="F108" s="8"/>
       <c r="G108" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H108" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I108" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J108" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K108" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L108" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M108" s="8"/>
       <c r="N108" s="8"/>
@@ -6905,34 +6905,34 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D109" s="8"/>
       <c r="E109" s="13"/>
       <c r="F109" s="8"/>
       <c r="G109" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H109" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I109" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J109" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K109" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L109" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M109" s="8"/>
       <c r="N109" s="8"/>
@@ -6942,34 +6942,34 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D110" s="8"/>
       <c r="E110" s="13"/>
       <c r="F110" s="8"/>
       <c r="G110" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H110" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I110" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J110" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K110" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L110" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M110" s="8"/>
       <c r="N110" s="8"/>
@@ -6979,34 +6979,34 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D111" s="8"/>
       <c r="E111" s="13"/>
       <c r="F111" s="8"/>
       <c r="G111" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H111" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I111" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J111" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K111" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L111" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M111" s="8"/>
       <c r="N111" s="8"/>
@@ -7016,96 +7016,96 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B112" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="C112" s="13" t="s">
         <v>582</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="113" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B113" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="C113" s="13" t="s">
         <v>582</v>
-      </c>
-      <c r="C113" s="13" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="114" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B114" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="C114" s="13" t="s">
         <v>582</v>
-      </c>
-      <c r="C114" s="13" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="115" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B115" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="C115" s="13" t="s">
         <v>582</v>
-      </c>
-      <c r="C115" s="13" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="116" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B116" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="C116" s="13" t="s">
         <v>582</v>
-      </c>
-      <c r="C116" s="13" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="117" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="118" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="119" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A119" s="29" t="s">
+        <v>593</v>
+      </c>
+      <c r="B119" s="30" t="s">
+        <v>594</v>
+      </c>
+      <c r="C119" s="30" t="s">
         <v>595</v>
-      </c>
-      <c r="B119" s="30" t="s">
-        <v>596</v>
-      </c>
-      <c r="C119" s="30" t="s">
-        <v>597</v>
       </c>
       <c r="D119"/>
       <c r="E119"/>
       <c r="F119"/>
       <c r="G119" s="30" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="H119"/>
       <c r="I119"/>
@@ -23486,19 +23486,19 @@
     </row>
     <row r="120" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A120" s="29" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C120" s="30" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D120"/>
       <c r="E120"/>
       <c r="F120"/>
       <c r="G120" s="30" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="H120"/>
       <c r="I120"/>
@@ -39879,19 +39879,19 @@
     </row>
     <row r="121" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A121" s="29" t="s">
+        <v>599</v>
+      </c>
+      <c r="B121" s="30" t="s">
+        <v>600</v>
+      </c>
+      <c r="C121" s="30" t="s">
         <v>601</v>
-      </c>
-      <c r="B121" s="30" t="s">
-        <v>602</v>
-      </c>
-      <c r="C121" s="30" t="s">
-        <v>603</v>
       </c>
       <c r="D121"/>
       <c r="E121"/>
       <c r="F121"/>
       <c r="G121" s="30" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H121"/>
       <c r="I121"/>
@@ -56272,19 +56272,19 @@
     </row>
     <row r="122" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A122" s="29" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C122" s="30" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D122"/>
       <c r="E122"/>
       <c r="F122"/>
       <c r="G122" s="30" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H122"/>
       <c r="I122"/>
@@ -72665,24 +72665,24 @@
     </row>
     <row r="123" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A123" s="29" t="s">
+        <v>605</v>
+      </c>
+      <c r="B123" s="30" t="s">
+        <v>606</v>
+      </c>
+      <c r="C123" s="30" t="s">
         <v>607</v>
-      </c>
-      <c r="B123" s="30" t="s">
-        <v>608</v>
-      </c>
-      <c r="C123" s="30" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="124" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C124" s="30" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fixes and appending codelist
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skold\Dropbox\Projekt\MoCiS2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519ED7C1-0279-428F-93C1-3F3F41A3E103}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07186D08-1F43-4F43-909C-5F8CBCC12051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29010" yWindow="-6690" windowWidth="26490" windowHeight="11385" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-6870" windowWidth="16905" windowHeight="11385" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
     <sheet name="ARTER" sheetId="15" r:id="rId2"/>
     <sheet name="PARAMETRAR" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="617">
   <si>
     <t>PERC</t>
   </si>
@@ -1633,9 +1633,6 @@
     <t>LPFHXS</t>
   </si>
   <si>
-    <t>UC Davies Stable isotope facility</t>
-  </si>
-  <si>
     <t>Procent_av_tv</t>
   </si>
   <si>
@@ -1822,9 +1819,6 @@
     <t>CH12/161</t>
   </si>
   <si>
-    <t>mm</t>
-  </si>
-  <si>
     <t>Längd (medelvärde)</t>
   </si>
   <si>
@@ -1877,6 +1871,18 @@
   </si>
   <si>
     <t>NUCDTPRC</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Procent</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>UC Davies</t>
   </si>
 </sst>
 </file>
@@ -2002,7 +2008,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2073,6 +2079,9 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2384,13 +2393,13 @@
         <v>108</v>
       </c>
       <c r="B1" s="25" t="s">
+        <v>548</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>550</v>
-      </c>
       <c r="D1" s="24" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2401,10 +2410,10 @@
         <v>110</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2415,10 +2424,10 @@
         <v>110</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2429,10 +2438,10 @@
         <v>112</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2443,10 +2452,10 @@
         <v>112</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2457,10 +2466,10 @@
         <v>114</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2471,10 +2480,10 @@
         <v>114</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2485,10 +2494,10 @@
         <v>116</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2499,10 +2508,10 @@
         <v>116</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2530,7 +2539,7 @@
         <v>122</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2600,7 +2609,7 @@
         <v>134</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,7 +2735,7 @@
         <v>161</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2754,7 +2763,7 @@
         <v>122</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2810,7 +2819,7 @@
         <v>161</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2866,7 +2875,7 @@
         <v>173</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3202,7 +3211,7 @@
         <v>474</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3439,10 +3448,10 @@
         <v>107</v>
       </c>
       <c r="C1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D1" t="s">
         <v>562</v>
-      </c>
-      <c r="D1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3470,7 +3479,7 @@
         <v>218387</v>
       </c>
       <c r="D3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3484,7 +3493,7 @@
         <v>102618</v>
       </c>
       <c r="D4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,7 +3521,7 @@
         <v>206231</v>
       </c>
       <c r="D6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3526,7 +3535,7 @@
         <v>100144</v>
       </c>
       <c r="D7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3540,7 +3549,7 @@
         <v>102950</v>
       </c>
       <c r="D8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,7 +3563,7 @@
         <v>206293</v>
       </c>
       <c r="D9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3568,7 +3577,7 @@
         <v>206142</v>
       </c>
       <c r="D10" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3582,7 +3591,7 @@
         <v>206089</v>
       </c>
       <c r="D11" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
   </sheetData>
@@ -3598,8 +3607,8 @@
   <dimension ref="A1:XFC124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E97" sqref="E97"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,7 +3634,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>16</v>
@@ -3646,10 +3655,10 @@
         <v>395</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>396</v>
@@ -3687,19 +3696,19 @@
         <v>19</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>407</v>
@@ -3716,19 +3725,19 @@
         <v>22</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L3" s="13" t="s">
         <v>407</v>
@@ -3745,19 +3754,19 @@
         <v>25</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>407</v>
@@ -3774,19 +3783,19 @@
         <v>28</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L5" s="13" t="s">
         <v>407</v>
@@ -3803,19 +3812,19 @@
         <v>31</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L6" s="13" t="s">
         <v>407</v>
@@ -3832,19 +3841,19 @@
         <v>34</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L7" s="13" t="s">
         <v>407</v>
@@ -3861,19 +3870,19 @@
         <v>37</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L8" s="13" t="s">
         <v>407</v>
@@ -3890,19 +3899,19 @@
         <v>40</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L9" s="13" t="s">
         <v>407</v>
@@ -3919,19 +3928,19 @@
         <v>53</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L10" s="13" t="s">
         <v>407</v>
@@ -3948,19 +3957,19 @@
         <v>55</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L11" s="13" t="s">
         <v>407</v>
@@ -3977,19 +3986,19 @@
         <v>57</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L12" s="13" t="s">
         <v>407</v>
@@ -4006,19 +4015,19 @@
         <v>59</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L13" s="13" t="s">
         <v>407</v>
@@ -4026,28 +4035,28 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>588</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>589</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>590</v>
-      </c>
       <c r="G14" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>407</v>
@@ -4064,19 +4073,19 @@
         <v>61</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L15" s="13" t="s">
         <v>407</v>
@@ -4093,19 +4102,19 @@
         <v>63</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L16" s="13" t="s">
         <v>407</v>
@@ -4122,19 +4131,19 @@
         <v>65</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>407</v>
@@ -4151,19 +4160,19 @@
         <v>67</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L18" s="13" t="s">
         <v>407</v>
@@ -4180,19 +4189,19 @@
         <v>69</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L19" s="13" t="s">
         <v>407</v>
@@ -4209,19 +4218,19 @@
         <v>524</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L20" s="13" t="s">
         <v>407</v>
@@ -4238,19 +4247,19 @@
         <v>71</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L21" s="13" t="s">
         <v>407</v>
@@ -4267,19 +4276,19 @@
         <v>73</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L22" s="13" t="s">
         <v>407</v>
@@ -4296,19 +4305,19 @@
         <v>75</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L23" s="13" t="s">
         <v>407</v>
@@ -4319,25 +4328,25 @@
         <v>525</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>76</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L24" s="13" t="s">
         <v>407</v>
@@ -4348,25 +4357,25 @@
         <v>526</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>77</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L25" s="13" t="s">
         <v>407</v>
@@ -4383,19 +4392,19 @@
         <v>79</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L26" s="13" t="s">
         <v>407</v>
@@ -4412,19 +4421,19 @@
         <v>81</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L27" s="13" t="s">
         <v>407</v>
@@ -4435,25 +4444,25 @@
         <v>82</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>83</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L28" s="13" t="s">
         <v>407</v>
@@ -4470,19 +4479,19 @@
         <v>84</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L29" s="13" t="s">
         <v>407</v>
@@ -4499,19 +4508,19 @@
         <v>85</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L30" s="13" t="s">
         <v>407</v>
@@ -4528,19 +4537,19 @@
         <v>86</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L31" s="13" t="s">
         <v>407</v>
@@ -4557,19 +4566,19 @@
         <v>87</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L32" s="13" t="s">
         <v>407</v>
@@ -4586,19 +4595,19 @@
         <v>88</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L33" s="13" t="s">
         <v>407</v>
@@ -4615,19 +4624,19 @@
         <v>90</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K34" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L34" s="13" t="s">
         <v>407</v>
@@ -4644,19 +4653,19 @@
         <v>92</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L35" s="13" t="s">
         <v>407</v>
@@ -4664,7 +4673,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>414</v>
@@ -4673,19 +4682,19 @@
         <v>93</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L36" s="13" t="s">
         <v>407</v>
@@ -4702,19 +4711,19 @@
         <v>95</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L37" s="13" t="s">
         <v>407</v>
@@ -4722,7 +4731,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>96</v>
@@ -4731,19 +4740,19 @@
         <v>97</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L38" s="13" t="s">
         <v>407</v>
@@ -4760,19 +4769,19 @@
         <v>99</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L39" s="13" t="s">
         <v>407</v>
@@ -4789,19 +4798,19 @@
         <v>101</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L40" s="13" t="s">
         <v>407</v>
@@ -4818,19 +4827,19 @@
         <v>103</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L41" s="13" t="s">
         <v>407</v>
@@ -4847,19 +4856,19 @@
         <v>105</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L42" s="13" t="s">
         <v>407</v>
@@ -4876,19 +4885,19 @@
         <v>187</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K43" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L43" s="13" t="s">
         <v>407</v>
@@ -4905,19 +4914,19 @@
         <v>190</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L44" s="13" t="s">
         <v>407</v>
@@ -4934,19 +4943,19 @@
         <v>193</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L45" s="13" t="s">
         <v>407</v>
@@ -4963,19 +4972,19 @@
         <v>196</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L46" s="13" t="s">
         <v>407</v>
@@ -4992,19 +5001,19 @@
         <v>199</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L47" s="13" t="s">
         <v>407</v>
@@ -5021,19 +5030,19 @@
         <v>202</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K48" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L48" s="13" t="s">
         <v>407</v>
@@ -5050,19 +5059,19 @@
         <v>205</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L49" s="13" t="s">
         <v>407</v>
@@ -5079,19 +5088,19 @@
         <v>208</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J50" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L50" s="13" t="s">
         <v>407</v>
@@ -5108,19 +5117,19 @@
         <v>211</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L51" s="13" t="s">
         <v>407</v>
@@ -5137,19 +5146,19 @@
         <v>214</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J52" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K52" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L52" s="13" t="s">
         <v>407</v>
@@ -5166,19 +5175,19 @@
         <v>217</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K53" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L53" s="13" t="s">
         <v>407</v>
@@ -5195,19 +5204,19 @@
         <v>220</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I54" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K54" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L54" s="13" t="s">
         <v>407</v>
@@ -5224,19 +5233,19 @@
         <v>223</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I55" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K55" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L55" s="13" t="s">
         <v>407</v>
@@ -5253,19 +5262,19 @@
         <v>226</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I56" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K56" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L56" s="13" t="s">
         <v>407</v>
@@ -5282,19 +5291,19 @@
         <v>229</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I57" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K57" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L57" s="13" t="s">
         <v>407</v>
@@ -5311,19 +5320,19 @@
         <v>232</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I58" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K58" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L58" s="13" t="s">
         <v>407</v>
@@ -5340,19 +5349,19 @@
         <v>235</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I59" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K59" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L59" s="13" t="s">
         <v>407</v>
@@ -5369,19 +5378,19 @@
         <v>237</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J60" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L60" s="13" t="s">
         <v>407</v>
@@ -5398,19 +5407,19 @@
         <v>239</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J61" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K61" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L61" s="13" t="s">
         <v>407</v>
@@ -5427,19 +5436,19 @@
         <v>241</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J62" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K62" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L62" s="13" t="s">
         <v>407</v>
@@ -5456,19 +5465,19 @@
         <v>243</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J63" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K63" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L63" s="13" t="s">
         <v>407</v>
@@ -5485,19 +5494,19 @@
         <v>245</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L64" s="13" t="s">
         <v>407</v>
@@ -5514,19 +5523,19 @@
         <v>247</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I65" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J65" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K65" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L65" s="13" t="s">
         <v>407</v>
@@ -5543,19 +5552,19 @@
         <v>249</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I66" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J66" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K66" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L66" s="13" t="s">
         <v>407</v>
@@ -5572,19 +5581,19 @@
         <v>251</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J67" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L67" s="13" t="s">
         <v>407</v>
@@ -5601,19 +5610,19 @@
         <v>253</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I68" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J68" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K68" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L68" s="13" t="s">
         <v>407</v>
@@ -5630,19 +5639,19 @@
         <v>255</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I69" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J69" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K69" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L69" s="13" t="s">
         <v>407</v>
@@ -5659,19 +5668,19 @@
         <v>257</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J70" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K70" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L70" s="13" t="s">
         <v>407</v>
@@ -5688,19 +5697,19 @@
         <v>259</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J71" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K71" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L71" s="13" t="s">
         <v>407</v>
@@ -5717,19 +5726,19 @@
         <v>261</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J72" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K72" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L72" s="13" t="s">
         <v>407</v>
@@ -5746,19 +5755,19 @@
         <v>263</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J73" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K73" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L73" s="13" t="s">
         <v>407</v>
@@ -5775,19 +5784,19 @@
         <v>265</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J74" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K74" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L74" s="13" t="s">
         <v>407</v>
@@ -5906,7 +5915,7 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>272</v>
@@ -6322,19 +6331,19 @@
         <v>295</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J89" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K89" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L89" s="13" t="s">
         <v>400</v>
@@ -6351,19 +6360,19 @@
         <v>297</v>
       </c>
       <c r="G90" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J90" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K90" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L90" s="13" t="s">
         <v>400</v>
@@ -6380,19 +6389,19 @@
         <v>303</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J91" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K91" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L91" s="13" t="s">
         <v>400</v>
@@ -6409,19 +6418,19 @@
         <v>305</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J92" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K92" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L92" s="13" t="s">
         <v>400</v>
@@ -6438,19 +6447,19 @@
         <v>287</v>
       </c>
       <c r="G93" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J93" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K93" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L93" s="13" t="s">
         <v>400</v>
@@ -6467,19 +6476,19 @@
         <v>307</v>
       </c>
       <c r="G94" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I94" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J94" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K94" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L94" s="13" t="s">
         <v>400</v>
@@ -6496,19 +6505,19 @@
         <v>299</v>
       </c>
       <c r="G95" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I95" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J95" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K95" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L95" s="13" t="s">
         <v>400</v>
@@ -6525,19 +6534,19 @@
         <v>309</v>
       </c>
       <c r="G96" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I96" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J96" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L96" s="13" t="s">
         <v>400</v>
@@ -6554,19 +6563,19 @@
         <v>311</v>
       </c>
       <c r="G97" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I97" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J97" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L97" s="13" t="s">
         <v>400</v>
@@ -6583,19 +6592,19 @@
         <v>313</v>
       </c>
       <c r="G98" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I98" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J98" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L98" s="13" t="s">
         <v>400</v>
@@ -6612,19 +6621,19 @@
         <v>301</v>
       </c>
       <c r="G99" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I99" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J99" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L99" s="13" t="s">
         <v>400</v>
@@ -6641,19 +6650,19 @@
         <v>315</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I100" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J100" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L100" s="13" t="s">
         <v>400</v>
@@ -6670,19 +6679,19 @@
         <v>352</v>
       </c>
       <c r="E101" s="22" t="s">
-        <v>533</v>
+        <v>616</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="J101" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="K101" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L101" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
@@ -6696,24 +6705,24 @@
         <v>354</v>
       </c>
       <c r="E102" s="22" t="s">
-        <v>533</v>
+        <v>616</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J102" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="K102" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L102" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B103" s="15" t="s">
         <v>355</v>
@@ -6722,20 +6731,20 @@
         <v>356</v>
       </c>
       <c r="E103" s="22" t="s">
+        <v>616</v>
+      </c>
+      <c r="G103" s="16" t="s">
         <v>533</v>
-      </c>
-      <c r="G103" s="16" t="s">
-        <v>534</v>
       </c>
       <c r="J103" s="23"/>
       <c r="K103" s="23"/>
       <c r="L103" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>357</v>
@@ -6744,15 +6753,15 @@
         <v>358</v>
       </c>
       <c r="E104" s="22" t="s">
+        <v>616</v>
+      </c>
+      <c r="G104" s="16" t="s">
         <v>533</v>
-      </c>
-      <c r="G104" s="16" t="s">
-        <v>534</v>
       </c>
       <c r="J104" s="23"/>
       <c r="K104" s="23"/>
       <c r="L104" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
@@ -7016,102 +7025,146 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>582</v>
+        <v>581</v>
+      </c>
+      <c r="G112" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="L112" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="113" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>582</v>
+        <v>581</v>
+      </c>
+      <c r="G113" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="L113" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="114" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>582</v>
+        <v>581</v>
+      </c>
+      <c r="G114" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="L114" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="115" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>582</v>
+        <v>581</v>
+      </c>
+      <c r="G115" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="L115" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="116" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>579</v>
+      </c>
+      <c r="C116" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="B116" s="13" t="s">
-        <v>580</v>
-      </c>
-      <c r="C116" s="13" t="s">
-        <v>582</v>
+      <c r="G116" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="L116" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B117" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="C117" s="13" t="s">
         <v>583</v>
       </c>
-      <c r="C117" s="13" t="s">
-        <v>584</v>
+      <c r="G117" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="L117" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="118" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B118" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="C118" s="13" t="s">
         <v>583</v>
       </c>
-      <c r="C118" s="13" t="s">
-        <v>584</v>
+      <c r="G118" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="L118" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="119" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A119" s="29" t="s">
+        <v>592</v>
+      </c>
+      <c r="B119" s="30" t="s">
         <v>593</v>
       </c>
-      <c r="B119" s="30" t="s">
+      <c r="C119" s="30" t="s">
         <v>594</v>
-      </c>
-      <c r="C119" s="30" t="s">
-        <v>595</v>
       </c>
       <c r="D119"/>
       <c r="E119"/>
       <c r="F119"/>
       <c r="G119" s="30" t="s">
-        <v>596</v>
+        <v>613</v>
       </c>
       <c r="H119"/>
       <c r="I119"/>
       <c r="J119"/>
       <c r="K119"/>
-      <c r="L119"/>
+      <c r="L119" s="13" t="s">
+        <v>400</v>
+      </c>
       <c r="M119"/>
       <c r="N119"/>
       <c r="O119"/>
@@ -23486,25 +23539,27 @@
     </row>
     <row r="120" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A120" s="29" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C120" s="30" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D120"/>
       <c r="E120"/>
       <c r="F120"/>
       <c r="G120" s="30" t="s">
-        <v>596</v>
+        <v>613</v>
       </c>
       <c r="H120"/>
       <c r="I120"/>
       <c r="J120"/>
       <c r="K120"/>
-      <c r="L120"/>
+      <c r="L120" s="13" t="s">
+        <v>400</v>
+      </c>
       <c r="M120"/>
       <c r="N120"/>
       <c r="O120"/>
@@ -39879,25 +39934,27 @@
     </row>
     <row r="121" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A121" s="29" t="s">
+        <v>597</v>
+      </c>
+      <c r="B121" s="30" t="s">
+        <v>598</v>
+      </c>
+      <c r="C121" s="30" t="s">
         <v>599</v>
-      </c>
-      <c r="B121" s="30" t="s">
-        <v>600</v>
-      </c>
-      <c r="C121" s="30" t="s">
-        <v>601</v>
       </c>
       <c r="D121"/>
       <c r="E121"/>
       <c r="F121"/>
       <c r="G121" s="30" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="H121"/>
       <c r="I121"/>
       <c r="J121"/>
       <c r="K121"/>
-      <c r="L121"/>
+      <c r="L121" s="13" t="s">
+        <v>400</v>
+      </c>
       <c r="M121"/>
       <c r="N121"/>
       <c r="O121"/>
@@ -56272,25 +56329,27 @@
     </row>
     <row r="122" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A122" s="29" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C122" s="30" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D122"/>
       <c r="E122"/>
       <c r="F122"/>
       <c r="G122" s="30" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="H122"/>
       <c r="I122"/>
       <c r="J122"/>
       <c r="K122"/>
-      <c r="L122"/>
+      <c r="L122" s="13" t="s">
+        <v>400</v>
+      </c>
       <c r="M122"/>
       <c r="N122"/>
       <c r="O122"/>
@@ -72665,24 +72724,36 @@
     </row>
     <row r="123" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A123" s="29" t="s">
+        <v>603</v>
+      </c>
+      <c r="B123" s="30" t="s">
+        <v>604</v>
+      </c>
+      <c r="C123" s="30" t="s">
         <v>605</v>
       </c>
-      <c r="B123" s="30" t="s">
-        <v>606</v>
-      </c>
-      <c r="C123" s="30" t="s">
-        <v>607</v>
+      <c r="G123" s="31" t="s">
+        <v>615</v>
+      </c>
+      <c r="L123" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="124" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C124" s="30" t="s">
-        <v>609</v>
+        <v>607</v>
+      </c>
+      <c r="G124" s="31" t="s">
+        <v>615</v>
+      </c>
+      <c r="L124" s="13" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Bylsjön to codelist
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skold\Dropbox\Projekt\MoCiS2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C916B1D3-A184-4C14-B07D-A8FF1E567BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990ABF91-F150-49FB-BA1C-02ADBF02EB16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35970" yWindow="-7065" windowWidth="21600" windowHeight="11385" tabRatio="877" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8490" windowWidth="29040" windowHeight="15840" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="631">
   <si>
     <t>PERC</t>
   </si>
@@ -1917,6 +1917,15 @@
   <si>
     <t>Rutilus rutilus</t>
   </si>
+  <si>
+    <t>BYLS</t>
+  </si>
+  <si>
+    <t>00103932</t>
+  </si>
+  <si>
+    <t>Bylsjön</t>
+  </si>
 </sst>
 </file>
 
@@ -2041,7 +2050,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2113,6 +2122,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Bra" xfId="4" builtinId="26"/>
@@ -2405,15 +2418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="32" customWidth="1"/>
     <col min="3" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3451,6 +3464,20 @@
       </c>
       <c r="D74" s="10" t="s">
         <v>456</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="31" t="s">
+        <v>628</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>629</v>
+      </c>
+      <c r="C75" s="31" t="s">
+        <v>630</v>
+      </c>
+      <c r="D75" s="31" t="s">
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -3463,7 +3490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added additional names for six marine stations
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skold\Dropbox\Projekt\MoCiS2\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MFO_Privat\MG\Personliga mappar\Anne LS\temp\MoCiS2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990ABF91-F150-49FB-BA1C-02ADBF02EB16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8490" windowWidth="29040" windowHeight="15840" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8040" windowWidth="29040" windowHeight="15840" tabRatio="877"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="637">
   <si>
     <t>PERC</t>
   </si>
@@ -1926,11 +1925,29 @@
   <si>
     <t>Bylsjön</t>
   </si>
+  <si>
+    <t>Ålands_hav_49G9</t>
+  </si>
+  <si>
+    <t>Väderöarna/Fjällbacka</t>
+  </si>
+  <si>
+    <t>Hanöbukten</t>
+  </si>
+  <si>
+    <t>S_Eg_Ösjön_40G7</t>
+  </si>
+  <si>
+    <t>N_Eg_Ösjön_46H0</t>
+  </si>
+  <si>
+    <t>Bottenhavet_51G9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2050,7 +2067,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2126,21 +2143,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Bra" xfId="4" builtinId="26"/>
     <cellStyle name="Dålig" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 2 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 3 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 3 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 4" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 6" xfId="3" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 7" xfId="5" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="XLConnect.String 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 2" xfId="6"/>
+    <cellStyle name="Normal 2 2" xfId="12"/>
+    <cellStyle name="Normal 2 4" xfId="10"/>
+    <cellStyle name="Normal 3 2" xfId="7"/>
+    <cellStyle name="Normal 3 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="8"/>
+    <cellStyle name="Normal 5" xfId="9"/>
+    <cellStyle name="Normal 6" xfId="3"/>
+    <cellStyle name="Normal 7" xfId="5"/>
+    <cellStyle name="XLConnect.String 2" xfId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2417,11 +2444,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2474,16 +2501,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>478</v>
+        <v>481</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,456 +2523,456 @@
       <c r="C5" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>491</v>
+      <c r="D5" s="34" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>479</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>479</v>
+        <v>104</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>479</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>490</v>
+        <v>104</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>480</v>
+        <v>106</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>479</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>493</v>
+        <v>106</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>479</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>111</v>
+        <v>479</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>484</v>
+        <v>107</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>120</v>
+        <v>107</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>123</v>
+        <v>111</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>126</v>
+        <v>114</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>489</v>
+        <v>117</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>129</v>
+        <v>120</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>132</v>
+        <v>123</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>135</v>
+        <v>126</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>138</v>
+        <v>126</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>141</v>
+        <v>126</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>144</v>
+        <v>129</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>147</v>
+        <v>132</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>150</v>
+        <v>135</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>485</v>
+        <v>138</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>156</v>
+        <v>141</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>321</v>
+        <v>142</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>486</v>
+        <v>144</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>159</v>
+        <v>147</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>132</v>
+        <v>149</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>162</v>
+        <v>152</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>322</v>
+        <v>154</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>487</v>
+        <v>156</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>160</v>
+        <v>321</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>162</v>
+        <v>113</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>171</v>
+        <v>158</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>165</v>
+        <v>131</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>488</v>
+        <v>161</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>118</v>
+        <v>322</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>120</v>
+        <v>153</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2958,525 +2985,609 @@
       <c r="C38" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="36" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>162</v>
+        <v>171</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>360</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>173</v>
+        <v>163</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>176</v>
+        <v>164</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>362</v>
+      <c r="A42" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>365</v>
+      <c r="A43" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>369</v>
+      <c r="A44" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>372</v>
+      <c r="A45" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>376</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>375</v>
+      <c r="A46" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>378</v>
+      <c r="A47" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>383</v>
+        <v>458</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>402</v>
+        <v>385</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>524</v>
+        <v>396</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>417</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>417</v>
+        <v>403</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>419</v>
+      <c r="A62" s="10" t="s">
+        <v>404</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>420</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>420</v>
+        <v>406</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>427</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>426</v>
+        <v>412</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>429</v>
+        <v>524</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
-        <v>434</v>
+      <c r="A67" s="10" t="s">
+        <v>416</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>435</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>435</v>
+        <v>418</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
-        <v>437</v>
+      <c r="A68" s="12" t="s">
+        <v>419</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>439</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>438</v>
+        <v>421</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>444</v>
+        <v>427</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>447</v>
+        <v>430</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
-        <v>452</v>
+      <c r="A73" s="12" t="s">
+        <v>434</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>454</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>453</v>
+        <v>436</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="31" t="s">
+      <c r="A75" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="31" t="s">
         <v>628</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B81" s="11" t="s">
         <v>629</v>
       </c>
-      <c r="C75" s="31" t="s">
+      <c r="C81" s="31" t="s">
         <v>630</v>
       </c>
-      <c r="D75" s="31" t="s">
+      <c r="D81" s="31" t="s">
         <v>630</v>
       </c>
     </row>
@@ -3487,7 +3598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3671,7 +3782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>

</xml_diff>

<commit_message>
Changed dyntaxa_taxon_id for MYTI
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8040" windowWidth="29040" windowHeight="15840" tabRatio="877"/>
+    <workbookView xWindow="28680" yWindow="-7590" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
     <sheet name="ARTER" sheetId="15" r:id="rId2"/>
     <sheet name="PARAMETRAR" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2447,7 +2447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3601,8 +3601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3643,7 +3643,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>218387</v>
+        <v>106665</v>
       </c>
       <c r="D3" t="s">
         <v>497</v>

</xml_diff>

<commit_message>
Changed PARAMETRAR variable units
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7590" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-7130" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="641">
   <si>
     <t>PERC</t>
   </si>
@@ -1677,9 +1677,6 @@
     <t>cm</t>
   </si>
   <si>
-    <t>Procent</t>
-  </si>
-  <si>
     <t>ar</t>
   </si>
   <si>
@@ -1943,6 +1940,21 @@
   <si>
     <t>Bottenhavet_51G9</t>
   </si>
+  <si>
+    <t>Procent_av_vv</t>
+  </si>
+  <si>
+    <t>EJ_REL</t>
+  </si>
+  <si>
+    <t>Vet_ej</t>
+  </si>
+  <si>
+    <t>SAKNAS</t>
+  </si>
+  <si>
+    <t>Nej</t>
+  </si>
 </sst>
 </file>
 
@@ -2067,7 +2079,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2153,6 +2165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Bra" xfId="4" builtinId="26"/>
@@ -2451,13 +2464,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.140625" style="32" customWidth="1"/>
-    <col min="3" max="4" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" style="32" customWidth="1"/>
+    <col min="3" max="4" width="38.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>100</v>
       </c>
@@ -2471,7 +2484,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>101</v>
       </c>
@@ -2485,7 +2498,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>101</v>
       </c>
@@ -2499,7 +2512,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>101</v>
       </c>
@@ -2510,10 +2523,10 @@
         <v>481</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>103</v>
       </c>
@@ -2527,7 +2540,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
         <v>103</v>
       </c>
@@ -2541,7 +2554,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
         <v>103</v>
       </c>
@@ -2552,10 +2565,10 @@
         <v>478</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>105</v>
       </c>
@@ -2569,7 +2582,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>105</v>
       </c>
@@ -2583,7 +2596,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>105</v>
       </c>
@@ -2594,10 +2607,10 @@
         <v>479</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -2611,7 +2624,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
         <v>107</v>
       </c>
@@ -2625,7 +2638,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
         <v>107</v>
       </c>
@@ -2636,10 +2649,10 @@
         <v>480</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
         <v>109</v>
       </c>
@@ -2653,7 +2666,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
         <v>112</v>
       </c>
@@ -2667,7 +2680,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
         <v>115</v>
       </c>
@@ -2681,7 +2694,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="23" t="s">
         <v>118</v>
       </c>
@@ -2695,7 +2708,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>121</v>
       </c>
@@ -2709,7 +2722,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
         <v>124</v>
       </c>
@@ -2723,7 +2736,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
         <v>124</v>
       </c>
@@ -2737,7 +2750,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>124</v>
       </c>
@@ -2748,10 +2761,10 @@
         <v>126</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="23" t="s">
         <v>127</v>
       </c>
@@ -2765,7 +2778,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="23" t="s">
         <v>130</v>
       </c>
@@ -2779,7 +2792,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="23" t="s">
         <v>133</v>
       </c>
@@ -2793,7 +2806,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
         <v>136</v>
       </c>
@@ -2807,7 +2820,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="23" t="s">
         <v>139</v>
       </c>
@@ -2821,7 +2834,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>142</v>
       </c>
@@ -2835,7 +2848,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="23" t="s">
         <v>145</v>
       </c>
@@ -2849,7 +2862,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="23" t="s">
         <v>148</v>
       </c>
@@ -2863,7 +2876,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>151</v>
       </c>
@@ -2877,7 +2890,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="23" t="s">
         <v>154</v>
       </c>
@@ -2891,7 +2904,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>321</v>
       </c>
@@ -2905,7 +2918,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
         <v>157</v>
       </c>
@@ -2919,7 +2932,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
         <v>130</v>
       </c>
@@ -2933,7 +2946,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>160</v>
       </c>
@@ -2947,7 +2960,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="23" t="s">
         <v>322</v>
       </c>
@@ -2961,7 +2974,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="23" t="s">
         <v>160</v>
       </c>
@@ -2975,7 +2988,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="23" t="s">
         <v>169</v>
       </c>
@@ -2989,7 +3002,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="23" t="s">
         <v>169</v>
       </c>
@@ -3000,10 +3013,10 @@
         <v>171</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="23" t="s">
         <v>163</v>
       </c>
@@ -3017,7 +3030,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="23" t="s">
         <v>163</v>
       </c>
@@ -3031,7 +3044,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="23" t="s">
         <v>118</v>
       </c>
@@ -3045,7 +3058,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="23" t="s">
         <v>166</v>
       </c>
@@ -3059,7 +3072,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="23" t="s">
         <v>169</v>
       </c>
@@ -3073,7 +3086,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>160</v>
       </c>
@@ -3087,7 +3100,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="23" t="s">
         <v>172</v>
       </c>
@@ -3101,7 +3114,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="23" t="s">
         <v>174</v>
       </c>
@@ -3115,7 +3128,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>361</v>
       </c>
@@ -3129,7 +3142,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>458</v>
       </c>
@@ -3143,7 +3156,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>368</v>
       </c>
@@ -3157,7 +3170,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="s">
         <v>371</v>
       </c>
@@ -3171,7 +3184,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="10" t="s">
         <v>374</v>
       </c>
@@ -3185,7 +3198,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
         <v>377</v>
       </c>
@@ -3199,7 +3212,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>380</v>
       </c>
@@ -3213,7 +3226,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
         <v>383</v>
       </c>
@@ -3227,7 +3240,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>386</v>
       </c>
@@ -3241,7 +3254,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>389</v>
       </c>
@@ -3255,7 +3268,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>392</v>
       </c>
@@ -3269,7 +3282,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>395</v>
       </c>
@@ -3283,7 +3296,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
         <v>398</v>
       </c>
@@ -3297,7 +3310,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>401</v>
       </c>
@@ -3311,7 +3324,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
         <v>404</v>
       </c>
@@ -3325,7 +3338,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>407</v>
       </c>
@@ -3339,7 +3352,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>410</v>
       </c>
@@ -3353,7 +3366,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>410</v>
       </c>
@@ -3367,7 +3380,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>413</v>
       </c>
@@ -3381,7 +3394,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>416</v>
       </c>
@@ -3395,7 +3408,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="12" t="s">
         <v>419</v>
       </c>
@@ -3409,7 +3422,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>422</v>
       </c>
@@ -3423,7 +3436,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>425</v>
       </c>
@@ -3437,7 +3450,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
         <v>428</v>
       </c>
@@ -3451,7 +3464,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>431</v>
       </c>
@@ -3465,7 +3478,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="12" t="s">
         <v>434</v>
       </c>
@@ -3479,7 +3492,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>437</v>
       </c>
@@ -3493,7 +3506,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>440</v>
       </c>
@@ -3507,7 +3520,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
         <v>443</v>
       </c>
@@ -3521,7 +3534,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
         <v>446</v>
       </c>
@@ -3535,7 +3548,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="s">
         <v>449</v>
       </c>
@@ -3549,7 +3562,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
         <v>452</v>
       </c>
@@ -3563,7 +3576,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="s">
         <v>455</v>
       </c>
@@ -3577,18 +3590,18 @@
         <v>456</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="B81" s="11" t="s">
         <v>628</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="C81" s="31" t="s">
         <v>629</v>
       </c>
-      <c r="C81" s="31" t="s">
-        <v>630</v>
-      </c>
       <c r="D81" s="31" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>
@@ -3601,13 +3614,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -3621,7 +3634,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3635,7 +3648,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3649,7 +3662,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3663,7 +3676,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3677,7 +3690,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>313</v>
       </c>
@@ -3691,7 +3704,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3705,7 +3718,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3719,7 +3732,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3733,7 +3746,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3747,7 +3760,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3761,18 +3774,18 @@
         <v>503</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>624</v>
+      </c>
+      <c r="B12" t="s">
         <v>625</v>
-      </c>
-      <c r="B12" t="s">
-        <v>626</v>
       </c>
       <c r="C12">
         <v>206135</v>
       </c>
       <c r="D12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -3788,33 +3801,33 @@
   </sheetPr>
   <dimension ref="A1:XFC131"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L126" sqref="L126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="15" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="16" max="16" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>504</v>
       </c>
@@ -3867,7 +3880,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>337</v>
       </c>
@@ -3896,7 +3909,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -3925,7 +3938,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -3954,7 +3967,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -3983,7 +3996,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -4012,7 +4025,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -4041,7 +4054,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -4070,7 +4083,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
@@ -4099,9 +4112,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B10" t="s">
         <v>52</v>
@@ -4128,7 +4141,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -4157,7 +4170,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -4186,7 +4199,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>267</v>
       </c>
@@ -4215,7 +4228,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -4244,7 +4257,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>521</v>
       </c>
@@ -4273,9 +4286,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
@@ -4302,7 +4315,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -4331,9 +4344,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B18" t="s">
         <v>62</v>
@@ -4360,7 +4373,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -4389,9 +4402,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
@@ -4418,7 +4431,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -4447,9 +4460,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B22" t="s">
         <v>66</v>
@@ -4476,7 +4489,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -4505,9 +4518,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B24" t="s">
         <v>68</v>
@@ -4534,7 +4547,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -4563,7 +4576,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>459</v>
       </c>
@@ -4592,7 +4605,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -4621,7 +4634,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
@@ -4650,9 +4663,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B29" t="s">
         <v>74</v>
@@ -4679,7 +4692,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -4708,12 +4721,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>462</v>
       </c>
       <c r="B31" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>76</v>
@@ -4737,12 +4750,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>463</v>
       </c>
       <c r="B32" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>77</v>
@@ -4766,12 +4779,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>79</v>
@@ -4795,12 +4808,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>81</v>
@@ -4824,12 +4837,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>83</v>
@@ -4853,12 +4866,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>464</v>
       </c>
       <c r="B36" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>84</v>
@@ -4882,12 +4895,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>465</v>
       </c>
       <c r="B37" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>85</v>
@@ -4911,12 +4924,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>466</v>
       </c>
       <c r="B38" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>86</v>
@@ -4940,12 +4953,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>467</v>
       </c>
       <c r="B39" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>87</v>
@@ -4969,12 +4982,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>468</v>
       </c>
       <c r="B40" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>88</v>
@@ -4998,12 +5011,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>353</v>
       </c>
       <c r="B41" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>89</v>
@@ -5027,12 +5040,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>354</v>
       </c>
       <c r="B42" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>90</v>
@@ -5056,12 +5069,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>520</v>
       </c>
       <c r="B43" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>91</v>
@@ -5085,12 +5098,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>469</v>
       </c>
       <c r="B44" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>92</v>
@@ -5114,12 +5127,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>519</v>
       </c>
       <c r="B45" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>93</v>
@@ -5143,12 +5156,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>355</v>
       </c>
       <c r="B46" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>94</v>
@@ -5172,12 +5185,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>356</v>
       </c>
       <c r="B47" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>95</v>
@@ -5201,12 +5214,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>357</v>
       </c>
       <c r="B48" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>96</v>
@@ -5230,12 +5243,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>358</v>
       </c>
       <c r="B49" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>97</v>
@@ -5259,12 +5272,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>177</v>
       </c>
       <c r="B50" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>178</v>
@@ -5288,12 +5301,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B51" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>180</v>
@@ -5317,12 +5330,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>181</v>
       </c>
       <c r="B52" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>182</v>
@@ -5346,12 +5359,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B53" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>184</v>
@@ -5375,12 +5388,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B54" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>186</v>
@@ -5404,12 +5417,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>187</v>
       </c>
       <c r="B55" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>188</v>
@@ -5433,12 +5446,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B56" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>190</v>
@@ -5462,12 +5475,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B57" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>192</v>
@@ -5491,12 +5504,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B58" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>194</v>
@@ -5520,12 +5533,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B59" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>196</v>
@@ -5549,12 +5562,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>197</v>
       </c>
       <c r="B60" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>198</v>
@@ -5578,12 +5591,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>199</v>
       </c>
       <c r="B61" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>200</v>
@@ -5607,12 +5620,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>201</v>
       </c>
       <c r="B62" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>202</v>
@@ -5636,12 +5649,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B63" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>204</v>
@@ -5665,12 +5678,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>205</v>
       </c>
       <c r="B64" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>206</v>
@@ -5694,12 +5707,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B65" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>208</v>
@@ -5723,12 +5736,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B66" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>210</v>
@@ -5752,7 +5765,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>297</v>
       </c>
@@ -5781,7 +5794,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>296</v>
       </c>
@@ -5810,7 +5823,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>295</v>
       </c>
@@ -5839,7 +5852,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
         <v>294</v>
       </c>
@@ -5868,7 +5881,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>293</v>
       </c>
@@ -5897,7 +5910,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>292</v>
       </c>
@@ -5926,7 +5939,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>291</v>
       </c>
@@ -5955,7 +5968,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>290</v>
       </c>
@@ -5984,7 +5997,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>289</v>
       </c>
@@ -6013,7 +6026,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
         <v>287</v>
       </c>
@@ -6042,7 +6055,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>288</v>
       </c>
@@ -6071,7 +6084,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>298</v>
       </c>
@@ -6100,7 +6113,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>301</v>
       </c>
@@ -6129,7 +6142,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
         <v>300</v>
       </c>
@@ -6158,7 +6171,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
         <v>299</v>
       </c>
@@ -6187,12 +6200,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>316</v>
       </c>
       <c r="B82" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>241</v>
@@ -6224,12 +6237,12 @@
       <c r="P82" s="8"/>
       <c r="Q82" s="8"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>317</v>
       </c>
       <c r="B83" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>242</v>
@@ -6261,12 +6274,12 @@
       <c r="P83" s="8"/>
       <c r="Q83" s="8"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
         <v>318</v>
       </c>
       <c r="B84" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>243</v>
@@ -6298,12 +6311,12 @@
       <c r="P84" s="8"/>
       <c r="Q84" s="8"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="18" t="s">
         <v>518</v>
       </c>
       <c r="B85" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>244</v>
@@ -6335,12 +6348,12 @@
       <c r="P85" s="8"/>
       <c r="Q85" s="8"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="18" t="s">
         <v>280</v>
       </c>
       <c r="B86" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C86" s="13" t="s">
         <v>245</v>
@@ -6372,12 +6385,12 @@
       <c r="P86" s="8"/>
       <c r="Q86" s="8"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="18" t="s">
         <v>281</v>
       </c>
       <c r="B87" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>246</v>
@@ -6409,7 +6422,7 @@
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="18" t="s">
         <v>282</v>
       </c>
@@ -6446,12 +6459,12 @@
       <c r="P88" s="8"/>
       <c r="Q88" s="8"/>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="18" t="s">
         <v>283</v>
       </c>
       <c r="B89" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C89" s="13" t="s">
         <v>249</v>
@@ -6483,12 +6496,12 @@
       <c r="P89" s="8"/>
       <c r="Q89" s="8"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="18" t="s">
         <v>284</v>
       </c>
       <c r="B90" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C90" s="13" t="s">
         <v>250</v>
@@ -6520,12 +6533,12 @@
       <c r="P90" s="8"/>
       <c r="Q90" s="8"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="18" t="s">
         <v>286</v>
       </c>
       <c r="B91" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C91" s="13" t="s">
         <v>251</v>
@@ -6557,12 +6570,12 @@
       <c r="P91" s="8"/>
       <c r="Q91" s="8"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="17" t="s">
         <v>272</v>
       </c>
       <c r="B92" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C92" s="13" t="s">
         <v>252</v>
@@ -6594,12 +6607,12 @@
       <c r="P92" s="8"/>
       <c r="Q92" s="8"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="17" t="s">
         <v>314</v>
       </c>
       <c r="B93" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C93" s="13" t="s">
         <v>253</v>
@@ -6631,12 +6644,12 @@
       <c r="P93" s="8"/>
       <c r="Q93" s="8"/>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="17" t="s">
         <v>315</v>
       </c>
       <c r="B94" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C94" s="13" t="s">
         <v>254</v>
@@ -6668,12 +6681,12 @@
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="18" t="s">
         <v>285</v>
       </c>
       <c r="B95" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C95" s="13" t="s">
         <v>255</v>
@@ -6705,12 +6718,12 @@
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="14" t="s">
         <v>268</v>
       </c>
       <c r="B96" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C96" s="13" t="s">
         <v>256</v>
@@ -6734,12 +6747,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="14" t="s">
         <v>269</v>
       </c>
       <c r="B97" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C97" s="13" t="s">
         <v>257</v>
@@ -6763,12 +6776,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98" s="14" t="s">
         <v>270</v>
       </c>
       <c r="B98" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C98" s="13" t="s">
         <v>260</v>
@@ -6792,12 +6805,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
         <v>271</v>
       </c>
       <c r="B99" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C99" s="13" t="s">
         <v>261</v>
@@ -6821,12 +6834,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
         <v>319</v>
       </c>
       <c r="B100" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C100" s="19" t="s">
         <v>252</v>
@@ -6850,12 +6863,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
         <v>273</v>
       </c>
       <c r="B101" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C101" s="13" t="s">
         <v>262</v>
@@ -6879,12 +6892,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A102" s="14" t="s">
         <v>274</v>
       </c>
       <c r="B102" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C102" s="13" t="s">
         <v>258</v>
@@ -6908,12 +6921,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
         <v>275</v>
       </c>
       <c r="B103" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C103" s="13" t="s">
         <v>263</v>
@@ -6937,12 +6950,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104" s="14" t="s">
         <v>276</v>
       </c>
       <c r="B104" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C104" s="13" t="s">
         <v>264</v>
@@ -6966,12 +6979,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
         <v>277</v>
       </c>
       <c r="B105" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C105" s="13" t="s">
         <v>265</v>
@@ -6995,12 +7008,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
         <v>278</v>
       </c>
       <c r="B106" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C106" s="13" t="s">
         <v>259</v>
@@ -7024,12 +7037,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
         <v>279</v>
       </c>
       <c r="B107" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C107" s="13" t="s">
         <v>266</v>
@@ -7053,7 +7066,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="s">
         <v>311</v>
       </c>
@@ -7064,7 +7077,7 @@
         <v>303</v>
       </c>
       <c r="E108" s="21" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G108" s="15" t="s">
         <v>476</v>
@@ -7079,7 +7092,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A109" s="20" t="s">
         <v>310</v>
       </c>
@@ -7090,7 +7103,7 @@
         <v>305</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G109" s="15" t="s">
         <v>477</v>
@@ -7105,7 +7118,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="s">
         <v>545</v>
       </c>
@@ -7116,7 +7129,7 @@
         <v>307</v>
       </c>
       <c r="E110" s="21" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G110" s="16" t="s">
         <v>470</v>
@@ -7127,7 +7140,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111" s="20" t="s">
         <v>546</v>
       </c>
@@ -7138,7 +7151,7 @@
         <v>309</v>
       </c>
       <c r="E111" s="21" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G111" s="16" t="s">
         <v>470</v>
@@ -7149,12 +7162,12 @@
         <v>475</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A112" s="6" t="s">
         <v>323</v>
       </c>
       <c r="B112" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C112" s="13" t="s">
         <v>330</v>
@@ -7186,12 +7199,12 @@
       <c r="P112" s="8"/>
       <c r="Q112" s="8"/>
     </row>
-    <row r="113" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A113" s="6" t="s">
         <v>324</v>
       </c>
       <c r="B113" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C113" s="13" t="s">
         <v>331</v>
@@ -7223,12 +7236,12 @@
       <c r="P113" s="8"/>
       <c r="Q113" s="8"/>
     </row>
-    <row r="114" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
         <v>325</v>
       </c>
       <c r="B114" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C114" s="13" t="s">
         <v>332</v>
@@ -7260,12 +7273,12 @@
       <c r="P114" s="8"/>
       <c r="Q114" s="8"/>
     </row>
-    <row r="115" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
         <v>326</v>
       </c>
       <c r="B115" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C115" s="13" t="s">
         <v>333</v>
@@ -7297,12 +7310,12 @@
       <c r="P115" s="8"/>
       <c r="Q115" s="8"/>
     </row>
-    <row r="116" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
         <v>327</v>
       </c>
       <c r="B116" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C116" s="13" t="s">
         <v>334</v>
@@ -7334,12 +7347,12 @@
       <c r="P116" s="8"/>
       <c r="Q116" s="8"/>
     </row>
-    <row r="117" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
         <v>328</v>
       </c>
       <c r="B117" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C117" s="13" t="s">
         <v>335</v>
@@ -7371,12 +7384,12 @@
       <c r="P117" s="8"/>
       <c r="Q117" s="8"/>
     </row>
-    <row r="118" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
         <v>329</v>
       </c>
       <c r="B118" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C118" s="13" t="s">
         <v>336</v>
@@ -7408,7 +7421,7 @@
       <c r="P118" s="8"/>
       <c r="Q118" s="8"/>
     </row>
-    <row r="119" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
         <v>507</v>
       </c>
@@ -7419,13 +7432,13 @@
         <v>515</v>
       </c>
       <c r="G119" s="13" t="s">
-        <v>548</v>
+        <v>636</v>
       </c>
       <c r="L119" s="13" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="120" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
         <v>508</v>
       </c>
@@ -7436,13 +7449,13 @@
         <v>515</v>
       </c>
       <c r="G120" s="13" t="s">
-        <v>548</v>
+        <v>636</v>
       </c>
       <c r="L120" s="13" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="121" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
         <v>509</v>
       </c>
@@ -7453,13 +7466,13 @@
         <v>515</v>
       </c>
       <c r="G121" s="13" t="s">
-        <v>548</v>
+        <v>636</v>
       </c>
       <c r="L121" s="13" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="122" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
         <v>510</v>
       </c>
@@ -7470,13 +7483,13 @@
         <v>515</v>
       </c>
       <c r="G122" s="13" t="s">
-        <v>548</v>
+        <v>636</v>
       </c>
       <c r="L122" s="13" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="123" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A123" s="6" t="s">
         <v>514</v>
       </c>
@@ -7487,13 +7500,13 @@
         <v>515</v>
       </c>
       <c r="G123" s="13" t="s">
-        <v>548</v>
+        <v>636</v>
       </c>
       <c r="L123" s="13" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="124" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
         <v>511</v>
       </c>
@@ -7504,13 +7517,13 @@
         <v>517</v>
       </c>
       <c r="G124" s="13" t="s">
-        <v>548</v>
+        <v>636</v>
       </c>
       <c r="L124" s="13" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="125" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
         <v>512</v>
       </c>
@@ -7521,13 +7534,13 @@
         <v>517</v>
       </c>
       <c r="G125" s="13" t="s">
-        <v>548</v>
+        <v>636</v>
       </c>
       <c r="L125" s="13" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="126" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A126" s="28" t="s">
         <v>526</v>
       </c>
@@ -7550,10 +7563,18 @@
       <c r="L126" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="M126"/>
-      <c r="N126"/>
-      <c r="O126"/>
-      <c r="P126"/>
+      <c r="M126" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="N126" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="O126" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P126" s="37" t="s">
+        <v>638</v>
+      </c>
       <c r="Q126"/>
       <c r="R126"/>
       <c r="S126"/>
@@ -23922,7 +23943,7 @@
       <c r="XFB126"/>
       <c r="XFC126"/>
     </row>
-    <row r="127" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A127" s="28" t="s">
         <v>543</v>
       </c>
@@ -23945,10 +23966,10 @@
       <c r="L127" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="M127"/>
-      <c r="N127"/>
-      <c r="O127"/>
-      <c r="P127"/>
+      <c r="M127" s="37"/>
+      <c r="N127" s="37"/>
+      <c r="O127" s="37"/>
+      <c r="P127" s="37"/>
       <c r="Q127"/>
       <c r="R127"/>
       <c r="S127"/>
@@ -40317,7 +40338,7 @@
       <c r="XFB127"/>
       <c r="XFC127"/>
     </row>
-    <row r="128" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A128" s="28" t="s">
         <v>531</v>
       </c>
@@ -40340,10 +40361,18 @@
       <c r="L128" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="M128"/>
-      <c r="N128"/>
-      <c r="O128"/>
-      <c r="P128"/>
+      <c r="M128" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="N128" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="O128" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P128" s="37" t="s">
+        <v>638</v>
+      </c>
       <c r="Q128"/>
       <c r="R128"/>
       <c r="S128"/>
@@ -56712,7 +56741,7 @@
       <c r="XFB128"/>
       <c r="XFC128"/>
     </row>
-    <row r="129" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A129" s="28" t="s">
         <v>544</v>
       </c>
@@ -56735,10 +56764,10 @@
       <c r="L129" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="M129"/>
-      <c r="N129"/>
-      <c r="O129"/>
-      <c r="P129"/>
+      <c r="M129" s="37"/>
+      <c r="N129" s="37"/>
+      <c r="O129" s="37"/>
+      <c r="P129" s="37"/>
       <c r="Q129"/>
       <c r="R129"/>
       <c r="S129"/>
@@ -73107,7 +73136,7 @@
       <c r="XFB129"/>
       <c r="XFC129"/>
     </row>
-    <row r="130" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A130" s="28" t="s">
         <v>537</v>
       </c>
@@ -73118,13 +73147,25 @@
         <v>539</v>
       </c>
       <c r="G130" s="30" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L130" s="13" t="s">
         <v>345</v>
       </c>
+      <c r="M130" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="N130" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="O130" s="15" t="s">
+        <v>639</v>
+      </c>
+      <c r="P130" s="15" t="s">
+        <v>640</v>
+      </c>
     </row>
-    <row r="131" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A131" s="28" t="s">
         <v>542</v>
       </c>
@@ -73135,7 +73176,7 @@
         <v>541</v>
       </c>
       <c r="G131" s="30" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L131" s="13" t="s">
         <v>345</v>

</xml_diff>

<commit_message>
Changed bio PARAMETRAR variable info
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7130" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-6675" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="652">
   <si>
     <t>PERC</t>
   </si>
@@ -1955,6 +1955,39 @@
   <si>
     <t>Nej</t>
   </si>
+  <si>
+    <t>FRYSTO_TENNKAP</t>
+  </si>
+  <si>
+    <t>PLAST</t>
+  </si>
+  <si>
+    <t>UCD_SIA</t>
+  </si>
+  <si>
+    <t>EA-IRMS</t>
+  </si>
+  <si>
+    <t>ACHEXDEE</t>
+  </si>
+  <si>
+    <t>GLAS</t>
+  </si>
+  <si>
+    <t>VAG</t>
+  </si>
+  <si>
+    <t>LINJAL</t>
+  </si>
+  <si>
+    <t>Stereomikroskop</t>
+  </si>
+  <si>
+    <t>ACES</t>
+  </si>
+  <si>
+    <t>NRM</t>
+  </si>
 </sst>
 </file>
 
@@ -2464,13 +2497,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.1796875" style="32" customWidth="1"/>
-    <col min="3" max="4" width="38.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="32" customWidth="1"/>
+    <col min="3" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>100</v>
       </c>
@@ -2484,7 +2517,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>101</v>
       </c>
@@ -2498,7 +2531,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>101</v>
       </c>
@@ -2512,7 +2545,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>101</v>
       </c>
@@ -2526,7 +2559,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>103</v>
       </c>
@@ -2540,7 +2573,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>103</v>
       </c>
@@ -2554,7 +2587,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>103</v>
       </c>
@@ -2568,7 +2601,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>105</v>
       </c>
@@ -2582,7 +2615,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>105</v>
       </c>
@@ -2596,7 +2629,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>105</v>
       </c>
@@ -2610,7 +2643,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -2624,7 +2657,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>107</v>
       </c>
@@ -2638,7 +2671,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>107</v>
       </c>
@@ -2652,7 +2685,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>109</v>
       </c>
@@ -2666,7 +2699,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>112</v>
       </c>
@@ -2680,7 +2713,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>115</v>
       </c>
@@ -2694,7 +2727,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>118</v>
       </c>
@@ -2708,7 +2741,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>121</v>
       </c>
@@ -2722,7 +2755,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>124</v>
       </c>
@@ -2736,7 +2769,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>124</v>
       </c>
@@ -2750,7 +2783,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>124</v>
       </c>
@@ -2764,7 +2797,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>127</v>
       </c>
@@ -2778,7 +2811,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>130</v>
       </c>
@@ -2792,7 +2825,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>133</v>
       </c>
@@ -2806,7 +2839,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>136</v>
       </c>
@@ -2820,7 +2853,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>139</v>
       </c>
@@ -2834,7 +2867,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>142</v>
       </c>
@@ -2848,7 +2881,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>145</v>
       </c>
@@ -2862,7 +2895,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>148</v>
       </c>
@@ -2876,7 +2909,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>151</v>
       </c>
@@ -2890,7 +2923,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>154</v>
       </c>
@@ -2904,7 +2937,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>321</v>
       </c>
@@ -2918,7 +2951,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>157</v>
       </c>
@@ -2932,7 +2965,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>130</v>
       </c>
@@ -2946,7 +2979,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>160</v>
       </c>
@@ -2960,7 +2993,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>322</v>
       </c>
@@ -2974,7 +3007,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>160</v>
       </c>
@@ -2988,7 +3021,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>169</v>
       </c>
@@ -3002,7 +3035,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>169</v>
       </c>
@@ -3016,7 +3049,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>163</v>
       </c>
@@ -3030,7 +3063,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>163</v>
       </c>
@@ -3044,7 +3077,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>118</v>
       </c>
@@ -3058,7 +3091,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>166</v>
       </c>
@@ -3072,7 +3105,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>169</v>
       </c>
@@ -3086,7 +3119,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>160</v>
       </c>
@@ -3100,7 +3133,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>172</v>
       </c>
@@ -3114,7 +3147,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>174</v>
       </c>
@@ -3128,7 +3161,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>361</v>
       </c>
@@ -3142,7 +3175,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>458</v>
       </c>
@@ -3156,7 +3189,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>368</v>
       </c>
@@ -3170,7 +3203,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>371</v>
       </c>
@@ -3184,7 +3217,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>374</v>
       </c>
@@ -3198,7 +3231,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>377</v>
       </c>
@@ -3212,7 +3245,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>380</v>
       </c>
@@ -3226,7 +3259,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>383</v>
       </c>
@@ -3240,7 +3273,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>386</v>
       </c>
@@ -3254,7 +3287,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>389</v>
       </c>
@@ -3268,7 +3301,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>392</v>
       </c>
@@ -3282,7 +3315,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>395</v>
       </c>
@@ -3296,7 +3329,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>398</v>
       </c>
@@ -3310,7 +3343,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>401</v>
       </c>
@@ -3324,7 +3357,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>404</v>
       </c>
@@ -3338,7 +3371,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>407</v>
       </c>
@@ -3352,7 +3385,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>410</v>
       </c>
@@ -3366,7 +3399,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>410</v>
       </c>
@@ -3380,7 +3413,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>413</v>
       </c>
@@ -3394,7 +3427,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>416</v>
       </c>
@@ -3408,7 +3441,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>419</v>
       </c>
@@ -3422,7 +3455,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>422</v>
       </c>
@@ -3436,7 +3469,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>425</v>
       </c>
@@ -3450,7 +3483,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>428</v>
       </c>
@@ -3464,7 +3497,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>431</v>
       </c>
@@ -3478,7 +3511,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>434</v>
       </c>
@@ -3492,7 +3525,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>437</v>
       </c>
@@ -3506,7 +3539,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>440</v>
       </c>
@@ -3520,7 +3553,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>443</v>
       </c>
@@ -3534,7 +3567,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>446</v>
       </c>
@@ -3548,7 +3581,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>449</v>
       </c>
@@ -3562,7 +3595,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>452</v>
       </c>
@@ -3576,7 +3609,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>455</v>
       </c>
@@ -3590,7 +3623,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="31" t="s">
         <v>627</v>
       </c>
@@ -3618,9 +3651,9 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -3634,7 +3667,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3648,7 +3681,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3662,7 +3695,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3676,7 +3709,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3690,7 +3723,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>313</v>
       </c>
@@ -3704,7 +3737,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3718,7 +3751,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3732,7 +3765,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3746,7 +3779,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3760,7 +3793,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3774,7 +3807,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>624</v>
       </c>
@@ -3801,33 +3834,33 @@
   </sheetPr>
   <dimension ref="A1:XFC131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L126" sqref="L126"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="15" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.54296875" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.26953125" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26953125" style="1"/>
+    <col min="16" max="16" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>504</v>
       </c>
@@ -3880,7 +3913,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>337</v>
       </c>
@@ -3909,7 +3942,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -3938,7 +3971,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -3967,7 +4000,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -3996,7 +4029,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -4025,7 +4058,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -4054,7 +4087,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -4083,7 +4116,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
@@ -4112,7 +4145,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>550</v>
       </c>
@@ -4141,7 +4174,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -4170,7 +4203,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -4199,7 +4232,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>267</v>
       </c>
@@ -4228,7 +4261,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -4257,7 +4290,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>521</v>
       </c>
@@ -4286,7 +4319,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>552</v>
       </c>
@@ -4315,7 +4348,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -4344,7 +4377,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>556</v>
       </c>
@@ -4373,7 +4406,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -4402,7 +4435,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>553</v>
       </c>
@@ -4431,7 +4464,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -4460,7 +4493,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>555</v>
       </c>
@@ -4489,7 +4522,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -4518,7 +4551,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>551</v>
       </c>
@@ -4547,7 +4580,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -4576,7 +4609,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>459</v>
       </c>
@@ -4605,7 +4638,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -4634,7 +4667,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
@@ -4663,7 +4696,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>554</v>
       </c>
@@ -4692,7 +4725,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -4721,7 +4754,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>462</v>
       </c>
@@ -4750,7 +4783,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>463</v>
       </c>
@@ -4779,7 +4812,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
@@ -4808,7 +4841,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>80</v>
       </c>
@@ -4837,7 +4870,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>82</v>
       </c>
@@ -4866,7 +4899,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>464</v>
       </c>
@@ -4895,7 +4928,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>465</v>
       </c>
@@ -4924,7 +4957,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>466</v>
       </c>
@@ -4953,7 +4986,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>467</v>
       </c>
@@ -4982,7 +5015,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>468</v>
       </c>
@@ -5011,7 +5044,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>353</v>
       </c>
@@ -5040,7 +5073,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>354</v>
       </c>
@@ -5069,7 +5102,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>520</v>
       </c>
@@ -5098,7 +5131,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>469</v>
       </c>
@@ -5127,7 +5160,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>519</v>
       </c>
@@ -5156,7 +5189,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>355</v>
       </c>
@@ -5185,7 +5218,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>356</v>
       </c>
@@ -5214,7 +5247,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>357</v>
       </c>
@@ -5243,7 +5276,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>358</v>
       </c>
@@ -5272,7 +5305,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>177</v>
       </c>
@@ -5301,7 +5334,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>179</v>
       </c>
@@ -5330,7 +5363,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>181</v>
       </c>
@@ -5359,7 +5392,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>183</v>
       </c>
@@ -5388,7 +5421,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -5417,7 +5450,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>187</v>
       </c>
@@ -5446,7 +5479,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>189</v>
       </c>
@@ -5475,7 +5508,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>191</v>
       </c>
@@ -5504,7 +5537,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>193</v>
       </c>
@@ -5533,7 +5566,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>195</v>
       </c>
@@ -5562,7 +5595,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>197</v>
       </c>
@@ -5591,7 +5624,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>199</v>
       </c>
@@ -5620,7 +5653,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>201</v>
       </c>
@@ -5649,7 +5682,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>203</v>
       </c>
@@ -5678,7 +5711,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>205</v>
       </c>
@@ -5707,7 +5740,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>207</v>
       </c>
@@ -5736,7 +5769,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>209</v>
       </c>
@@ -5765,7 +5798,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>297</v>
       </c>
@@ -5794,7 +5827,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>296</v>
       </c>
@@ -5823,7 +5856,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>295</v>
       </c>
@@ -5852,7 +5885,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>294</v>
       </c>
@@ -5881,7 +5914,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>293</v>
       </c>
@@ -5910,7 +5943,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>292</v>
       </c>
@@ -5939,7 +5972,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>291</v>
       </c>
@@ -5968,7 +6001,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>290</v>
       </c>
@@ -5997,7 +6030,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>289</v>
       </c>
@@ -6026,7 +6059,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>287</v>
       </c>
@@ -6055,7 +6088,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>288</v>
       </c>
@@ -6084,7 +6117,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>298</v>
       </c>
@@ -6113,7 +6146,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>301</v>
       </c>
@@ -6142,7 +6175,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>300</v>
       </c>
@@ -6171,7 +6204,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>299</v>
       </c>
@@ -6200,7 +6233,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>316</v>
       </c>
@@ -6237,7 +6270,7 @@
       <c r="P82" s="8"/>
       <c r="Q82" s="8"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>317</v>
       </c>
@@ -6274,7 +6307,7 @@
       <c r="P83" s="8"/>
       <c r="Q83" s="8"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>318</v>
       </c>
@@ -6311,7 +6344,7 @@
       <c r="P84" s="8"/>
       <c r="Q84" s="8"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
         <v>518</v>
       </c>
@@ -6348,7 +6381,7 @@
       <c r="P85" s="8"/>
       <c r="Q85" s="8"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
         <v>280</v>
       </c>
@@ -6385,7 +6418,7 @@
       <c r="P86" s="8"/>
       <c r="Q86" s="8"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
         <v>281</v>
       </c>
@@ -6422,7 +6455,7 @@
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
         <v>282</v>
       </c>
@@ -6459,7 +6492,7 @@
       <c r="P88" s="8"/>
       <c r="Q88" s="8"/>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
         <v>283</v>
       </c>
@@ -6496,7 +6529,7 @@
       <c r="P89" s="8"/>
       <c r="Q89" s="8"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
         <v>284</v>
       </c>
@@ -6533,7 +6566,7 @@
       <c r="P90" s="8"/>
       <c r="Q90" s="8"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
         <v>286</v>
       </c>
@@ -6570,7 +6603,7 @@
       <c r="P91" s="8"/>
       <c r="Q91" s="8"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>272</v>
       </c>
@@ -6607,7 +6640,7 @@
       <c r="P92" s="8"/>
       <c r="Q92" s="8"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>314</v>
       </c>
@@ -6644,7 +6677,7 @@
       <c r="P93" s="8"/>
       <c r="Q93" s="8"/>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>315</v>
       </c>
@@ -6681,7 +6714,7 @@
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
         <v>285</v>
       </c>
@@ -6718,7 +6751,7 @@
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>268</v>
       </c>
@@ -6747,7 +6780,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>269</v>
       </c>
@@ -6776,7 +6809,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>270</v>
       </c>
@@ -6805,7 +6838,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>271</v>
       </c>
@@ -6834,7 +6867,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
         <v>319</v>
       </c>
@@ -6863,7 +6896,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
         <v>273</v>
       </c>
@@ -6892,7 +6925,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>274</v>
       </c>
@@ -6921,7 +6954,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
         <v>275</v>
       </c>
@@ -6950,7 +6983,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>276</v>
       </c>
@@ -6979,7 +7012,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
         <v>277</v>
       </c>
@@ -7008,7 +7041,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
         <v>278</v>
       </c>
@@ -7037,7 +7070,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
         <v>279</v>
       </c>
@@ -7066,7 +7099,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="s">
         <v>311</v>
       </c>
@@ -7092,7 +7125,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="s">
         <v>310</v>
       </c>
@@ -7118,7 +7151,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="s">
         <v>545</v>
       </c>
@@ -7127,6 +7160,9 @@
       </c>
       <c r="C110" s="15" t="s">
         <v>307</v>
+      </c>
+      <c r="D110" s="15" t="s">
+        <v>650</v>
       </c>
       <c r="E110" s="21" t="s">
         <v>549</v>
@@ -7139,8 +7175,23 @@
       <c r="L110" s="15" t="s">
         <v>475</v>
       </c>
+      <c r="M110" s="37" t="s">
+        <v>641</v>
+      </c>
+      <c r="N110" s="37" t="s">
+        <v>642</v>
+      </c>
+      <c r="O110" s="37" t="s">
+        <v>643</v>
+      </c>
+      <c r="P110" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q110" s="37" t="s">
+        <v>644</v>
+      </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="s">
         <v>546</v>
       </c>
@@ -7149,6 +7200,9 @@
       </c>
       <c r="C111" s="15" t="s">
         <v>309</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>650</v>
       </c>
       <c r="E111" s="21" t="s">
         <v>549</v>
@@ -7161,8 +7215,23 @@
       <c r="L111" s="15" t="s">
         <v>475</v>
       </c>
+      <c r="M111" s="37" t="s">
+        <v>641</v>
+      </c>
+      <c r="N111" s="37" t="s">
+        <v>642</v>
+      </c>
+      <c r="O111" s="37" t="s">
+        <v>643</v>
+      </c>
+      <c r="P111" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q111" s="37" t="s">
+        <v>644</v>
+      </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>323</v>
       </c>
@@ -7172,7 +7241,7 @@
       <c r="C112" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="D112" s="8"/>
+      <c r="D112" s="13"/>
       <c r="E112" s="13"/>
       <c r="F112" s="8"/>
       <c r="G112" s="13" t="s">
@@ -7193,13 +7262,13 @@
       <c r="L112" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="M112" s="8"/>
-      <c r="N112" s="8"/>
-      <c r="O112" s="8"/>
-      <c r="P112" s="8"/>
-      <c r="Q112" s="8"/>
+      <c r="M112" s="13"/>
+      <c r="N112" s="13"/>
+      <c r="O112" s="13"/>
+      <c r="P112" s="13"/>
+      <c r="Q112" s="13"/>
     </row>
-    <row r="113" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>324</v>
       </c>
@@ -7209,7 +7278,7 @@
       <c r="C113" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="D113" s="8"/>
+      <c r="D113" s="13"/>
       <c r="E113" s="13"/>
       <c r="F113" s="8"/>
       <c r="G113" s="13" t="s">
@@ -7230,13 +7299,13 @@
       <c r="L113" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="M113" s="8"/>
-      <c r="N113" s="8"/>
-      <c r="O113" s="8"/>
-      <c r="P113" s="8"/>
-      <c r="Q113" s="8"/>
+      <c r="M113" s="13"/>
+      <c r="N113" s="13"/>
+      <c r="O113" s="13"/>
+      <c r="P113" s="13"/>
+      <c r="Q113" s="13"/>
     </row>
-    <row r="114" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>325</v>
       </c>
@@ -7246,7 +7315,7 @@
       <c r="C114" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="D114" s="8"/>
+      <c r="D114" s="13"/>
       <c r="E114" s="13"/>
       <c r="F114" s="8"/>
       <c r="G114" s="13" t="s">
@@ -7267,13 +7336,13 @@
       <c r="L114" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="M114" s="8"/>
-      <c r="N114" s="8"/>
-      <c r="O114" s="8"/>
-      <c r="P114" s="8"/>
-      <c r="Q114" s="8"/>
+      <c r="M114" s="13"/>
+      <c r="N114" s="13"/>
+      <c r="O114" s="13"/>
+      <c r="P114" s="13"/>
+      <c r="Q114" s="13"/>
     </row>
-    <row r="115" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>326</v>
       </c>
@@ -7283,7 +7352,7 @@
       <c r="C115" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="D115" s="8"/>
+      <c r="D115" s="13"/>
       <c r="E115" s="13"/>
       <c r="F115" s="8"/>
       <c r="G115" s="13" t="s">
@@ -7304,13 +7373,13 @@
       <c r="L115" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="M115" s="8"/>
-      <c r="N115" s="8"/>
-      <c r="O115" s="8"/>
-      <c r="P115" s="8"/>
-      <c r="Q115" s="8"/>
+      <c r="M115" s="13"/>
+      <c r="N115" s="13"/>
+      <c r="O115" s="13"/>
+      <c r="P115" s="13"/>
+      <c r="Q115" s="13"/>
     </row>
-    <row r="116" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>327</v>
       </c>
@@ -7320,7 +7389,7 @@
       <c r="C116" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="D116" s="8"/>
+      <c r="D116" s="13"/>
       <c r="E116" s="13"/>
       <c r="F116" s="8"/>
       <c r="G116" s="13" t="s">
@@ -7341,13 +7410,13 @@
       <c r="L116" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="M116" s="8"/>
-      <c r="N116" s="8"/>
-      <c r="O116" s="8"/>
-      <c r="P116" s="8"/>
-      <c r="Q116" s="8"/>
+      <c r="M116" s="13"/>
+      <c r="N116" s="13"/>
+      <c r="O116" s="13"/>
+      <c r="P116" s="13"/>
+      <c r="Q116" s="13"/>
     </row>
-    <row r="117" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>328</v>
       </c>
@@ -7357,7 +7426,7 @@
       <c r="C117" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="D117" s="8"/>
+      <c r="D117" s="13"/>
       <c r="E117" s="13"/>
       <c r="F117" s="8"/>
       <c r="G117" s="13" t="s">
@@ -7378,13 +7447,13 @@
       <c r="L117" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="M117" s="8"/>
-      <c r="N117" s="8"/>
-      <c r="O117" s="8"/>
-      <c r="P117" s="8"/>
-      <c r="Q117" s="8"/>
+      <c r="M117" s="13"/>
+      <c r="N117" s="13"/>
+      <c r="O117" s="13"/>
+      <c r="P117" s="13"/>
+      <c r="Q117" s="13"/>
     </row>
-    <row r="118" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>329</v>
       </c>
@@ -7394,7 +7463,7 @@
       <c r="C118" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="D118" s="8"/>
+      <c r="D118" s="13"/>
       <c r="E118" s="13"/>
       <c r="F118" s="8"/>
       <c r="G118" s="13" t="s">
@@ -7415,13 +7484,13 @@
       <c r="L118" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="M118" s="8"/>
-      <c r="N118" s="8"/>
-      <c r="O118" s="8"/>
-      <c r="P118" s="8"/>
-      <c r="Q118" s="8"/>
+      <c r="M118" s="13"/>
+      <c r="N118" s="13"/>
+      <c r="O118" s="13"/>
+      <c r="P118" s="13"/>
+      <c r="Q118" s="13"/>
     </row>
-    <row r="119" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>507</v>
       </c>
@@ -7431,14 +7500,35 @@
       <c r="C119" s="13" t="s">
         <v>515</v>
       </c>
+      <c r="D119" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="E119" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G119" s="13" t="s">
         <v>636</v>
       </c>
       <c r="L119" s="13" t="s">
         <v>345</v>
       </c>
+      <c r="M119" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="N119" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="O119" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P119" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q119" s="37" t="s">
+        <v>647</v>
+      </c>
     </row>
-    <row r="120" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>508</v>
       </c>
@@ -7448,14 +7538,35 @@
       <c r="C120" s="13" t="s">
         <v>515</v>
       </c>
+      <c r="D120" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="E120" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G120" s="13" t="s">
         <v>636</v>
       </c>
       <c r="L120" s="13" t="s">
         <v>345</v>
       </c>
+      <c r="M120" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="N120" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="O120" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P120" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q120" s="37" t="s">
+        <v>647</v>
+      </c>
     </row>
-    <row r="121" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>509</v>
       </c>
@@ -7465,14 +7576,35 @@
       <c r="C121" s="13" t="s">
         <v>515</v>
       </c>
+      <c r="D121" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="E121" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G121" s="13" t="s">
         <v>636</v>
       </c>
       <c r="L121" s="13" t="s">
         <v>345</v>
       </c>
+      <c r="M121" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="N121" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="O121" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P121" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q121" s="37" t="s">
+        <v>647</v>
+      </c>
     </row>
-    <row r="122" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>510</v>
       </c>
@@ -7482,14 +7614,35 @@
       <c r="C122" s="13" t="s">
         <v>515</v>
       </c>
+      <c r="D122" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="E122" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G122" s="13" t="s">
         <v>636</v>
       </c>
       <c r="L122" s="13" t="s">
         <v>345</v>
       </c>
+      <c r="M122" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="N122" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="O122" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P122" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q122" s="37" t="s">
+        <v>647</v>
+      </c>
     </row>
-    <row r="123" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>514</v>
       </c>
@@ -7499,14 +7652,35 @@
       <c r="C123" s="13" t="s">
         <v>515</v>
       </c>
+      <c r="D123" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="E123" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G123" s="13" t="s">
         <v>636</v>
       </c>
       <c r="L123" s="13" t="s">
         <v>345</v>
       </c>
+      <c r="M123" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="N123" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="O123" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P123" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q123" s="37" t="s">
+        <v>647</v>
+      </c>
     </row>
-    <row r="124" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>511</v>
       </c>
@@ -7516,14 +7690,35 @@
       <c r="C124" s="13" t="s">
         <v>517</v>
       </c>
+      <c r="D124" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="E124" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G124" s="13" t="s">
         <v>636</v>
       </c>
       <c r="L124" s="13" t="s">
         <v>345</v>
       </c>
+      <c r="M124" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="N124" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="O124" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P124" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q124" s="37" t="s">
+        <v>647</v>
+      </c>
     </row>
-    <row r="125" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>512</v>
       </c>
@@ -7533,14 +7728,35 @@
       <c r="C125" s="13" t="s">
         <v>517</v>
       </c>
+      <c r="D125" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="E125" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G125" s="13" t="s">
         <v>636</v>
       </c>
       <c r="L125" s="13" t="s">
         <v>345</v>
       </c>
+      <c r="M125" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="N125" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="O125" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P125" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q125" s="37" t="s">
+        <v>647</v>
+      </c>
     </row>
-    <row r="126" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A126" s="28" t="s">
         <v>526</v>
       </c>
@@ -7550,8 +7766,12 @@
       <c r="C126" s="29" t="s">
         <v>528</v>
       </c>
-      <c r="D126"/>
-      <c r="E126"/>
+      <c r="D126" s="37" t="s">
+        <v>651</v>
+      </c>
+      <c r="E126" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="F126"/>
       <c r="G126" s="29" t="s">
         <v>547</v>
@@ -7575,7 +7795,9 @@
       <c r="P126" s="37" t="s">
         <v>638</v>
       </c>
-      <c r="Q126"/>
+      <c r="Q126" s="37" t="s">
+        <v>648</v>
+      </c>
       <c r="R126"/>
       <c r="S126"/>
       <c r="T126"/>
@@ -23943,7 +24165,7 @@
       <c r="XFB126"/>
       <c r="XFC126"/>
     </row>
-    <row r="127" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A127" s="28" t="s">
         <v>543</v>
       </c>
@@ -23953,8 +24175,12 @@
       <c r="C127" s="29" t="s">
         <v>530</v>
       </c>
-      <c r="D127"/>
-      <c r="E127"/>
+      <c r="D127" s="37" t="s">
+        <v>651</v>
+      </c>
+      <c r="E127" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="F127"/>
       <c r="G127" s="29" t="s">
         <v>547</v>
@@ -23966,11 +24192,21 @@
       <c r="L127" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="M127" s="37"/>
-      <c r="N127" s="37"/>
-      <c r="O127" s="37"/>
-      <c r="P127" s="37"/>
-      <c r="Q127"/>
+      <c r="M127" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="N127" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="O127" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P127" s="37" t="s">
+        <v>638</v>
+      </c>
+      <c r="Q127" s="37" t="s">
+        <v>648</v>
+      </c>
       <c r="R127"/>
       <c r="S127"/>
       <c r="T127"/>
@@ -40338,7 +40574,7 @@
       <c r="XFB127"/>
       <c r="XFC127"/>
     </row>
-    <row r="128" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A128" s="28" t="s">
         <v>531</v>
       </c>
@@ -40348,8 +40584,12 @@
       <c r="C128" s="29" t="s">
         <v>533</v>
       </c>
-      <c r="D128"/>
-      <c r="E128"/>
+      <c r="D128" s="37" t="s">
+        <v>651</v>
+      </c>
+      <c r="E128" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="F128"/>
       <c r="G128" s="29" t="s">
         <v>534</v>
@@ -40373,7 +40613,9 @@
       <c r="P128" s="37" t="s">
         <v>638</v>
       </c>
-      <c r="Q128"/>
+      <c r="Q128" s="37" t="s">
+        <v>647</v>
+      </c>
       <c r="R128"/>
       <c r="S128"/>
       <c r="T128"/>
@@ -56741,7 +56983,7 @@
       <c r="XFB128"/>
       <c r="XFC128"/>
     </row>
-    <row r="129" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A129" s="28" t="s">
         <v>544</v>
       </c>
@@ -56751,8 +56993,12 @@
       <c r="C129" s="29" t="s">
         <v>536</v>
       </c>
-      <c r="D129"/>
-      <c r="E129"/>
+      <c r="D129" s="37" t="s">
+        <v>651</v>
+      </c>
+      <c r="E129" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="F129"/>
       <c r="G129" s="29" t="s">
         <v>534</v>
@@ -56764,11 +57010,21 @@
       <c r="L129" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="M129" s="37"/>
-      <c r="N129" s="37"/>
-      <c r="O129" s="37"/>
-      <c r="P129" s="37"/>
-      <c r="Q129"/>
+      <c r="M129" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="N129" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="O129" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="P129" s="37" t="s">
+        <v>638</v>
+      </c>
+      <c r="Q129" s="37" t="s">
+        <v>647</v>
+      </c>
       <c r="R129"/>
       <c r="S129"/>
       <c r="T129"/>
@@ -73136,7 +73392,7 @@
       <c r="XFB129"/>
       <c r="XFC129"/>
     </row>
-    <row r="130" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A130" s="28" t="s">
         <v>537</v>
       </c>
@@ -73146,6 +73402,12 @@
       <c r="C130" s="29" t="s">
         <v>539</v>
       </c>
+      <c r="D130" s="37" t="s">
+        <v>651</v>
+      </c>
+      <c r="E130" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G130" s="30" t="s">
         <v>548</v>
       </c>
@@ -73164,8 +73426,11 @@
       <c r="P130" s="15" t="s">
         <v>640</v>
       </c>
+      <c r="Q130" s="15" t="s">
+        <v>649</v>
+      </c>
     </row>
-    <row r="131" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A131" s="28" t="s">
         <v>542</v>
       </c>
@@ -73175,11 +73440,32 @@
       <c r="C131" s="29" t="s">
         <v>541</v>
       </c>
+      <c r="D131" s="37" t="s">
+        <v>651</v>
+      </c>
+      <c r="E131" s="37" t="s">
+        <v>637</v>
+      </c>
       <c r="G131" s="30" t="s">
         <v>548</v>
       </c>
       <c r="L131" s="13" t="s">
         <v>345</v>
+      </c>
+      <c r="M131" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="N131" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="O131" s="15" t="s">
+        <v>639</v>
+      </c>
+      <c r="P131" s="15" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q131" s="15" t="s">
+        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added unit for lipid and dry weight
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6225" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-5775" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="652">
   <si>
     <t>PERC</t>
   </si>
@@ -3834,9 +3834,9 @@
   </sheetPr>
   <dimension ref="A1:XFC131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7509,6 +7509,9 @@
       <c r="G119" s="13" t="s">
         <v>635</v>
       </c>
+      <c r="J119" s="13" t="s">
+        <v>635</v>
+      </c>
       <c r="L119" s="13" t="s">
         <v>344</v>
       </c>
@@ -7547,6 +7550,9 @@
       <c r="G120" s="13" t="s">
         <v>635</v>
       </c>
+      <c r="J120" s="13" t="s">
+        <v>635</v>
+      </c>
       <c r="L120" s="13" t="s">
         <v>344</v>
       </c>
@@ -7585,6 +7591,9 @@
       <c r="G121" s="13" t="s">
         <v>635</v>
       </c>
+      <c r="J121" s="13" t="s">
+        <v>635</v>
+      </c>
       <c r="L121" s="13" t="s">
         <v>344</v>
       </c>
@@ -7623,6 +7632,9 @@
       <c r="G122" s="13" t="s">
         <v>635</v>
       </c>
+      <c r="J122" s="13" t="s">
+        <v>635</v>
+      </c>
       <c r="L122" s="13" t="s">
         <v>344</v>
       </c>
@@ -7661,6 +7673,9 @@
       <c r="G123" s="13" t="s">
         <v>635</v>
       </c>
+      <c r="J123" s="13" t="s">
+        <v>635</v>
+      </c>
       <c r="L123" s="13" t="s">
         <v>344</v>
       </c>
@@ -7699,6 +7714,9 @@
       <c r="G124" s="13" t="s">
         <v>635</v>
       </c>
+      <c r="J124" s="13" t="s">
+        <v>635</v>
+      </c>
       <c r="L124" s="13" t="s">
         <v>344</v>
       </c>
@@ -7735,6 +7753,9 @@
         <v>636</v>
       </c>
       <c r="G125" s="13" t="s">
+        <v>635</v>
+      </c>
+      <c r="J125" s="13" t="s">
         <v>635</v>
       </c>
       <c r="L125" s="13" t="s">

</xml_diff>

<commit_message>
Added kul/kväve mätosäkerhet enhet
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5325" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-4875" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="652">
   <si>
     <t>PERC</t>
   </si>
@@ -3835,8 +3835,8 @@
   <dimension ref="A1:XFC131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J110" sqref="J110:J111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7170,7 +7170,9 @@
       <c r="G110" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="J110" s="22"/>
+      <c r="J110" s="16" t="s">
+        <v>469</v>
+      </c>
       <c r="K110" s="22"/>
       <c r="L110" s="15" t="s">
         <v>474</v>
@@ -7210,7 +7212,9 @@
       <c r="G111" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="J111" s="22"/>
+      <c r="J111" s="16" t="s">
+        <v>469</v>
+      </c>
       <c r="K111" s="22"/>
       <c r="L111" s="15" t="s">
         <v>474</v>

</xml_diff>

<commit_message>
Removed "Bylsjön" from codelist
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4425" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-3970" windowWidth="29040" windowHeight="15840" tabRatio="877"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="649">
   <si>
     <t>PERC</t>
   </si>
@@ -1905,15 +1905,6 @@
     <t>Rutilus rutilus</t>
   </si>
   <si>
-    <t>BYLS</t>
-  </si>
-  <si>
-    <t>00103932</t>
-  </si>
-  <si>
-    <t>Bylsjön</t>
-  </si>
-  <si>
     <t>Ålands_hav_49G9</t>
   </si>
   <si>
@@ -2117,7 +2108,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2188,9 +2179,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -2497,19 +2485,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C13"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:XFD81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.140625" style="32" customWidth="1"/>
-    <col min="3" max="4" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" style="31" customWidth="1"/>
+    <col min="3" max="4" width="38.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>97</v>
       </c>
@@ -2523,7 +2511,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>98</v>
       </c>
@@ -2537,7 +2525,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>98</v>
       </c>
@@ -2551,7 +2539,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>98</v>
       </c>
@@ -2561,11 +2549,11 @@
       <c r="C4" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>630</v>
+      <c r="D4" s="32" t="s">
+        <v>627</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>100</v>
       </c>
@@ -2575,11 +2563,11 @@
       <c r="C5" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="33" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
         <v>100</v>
       </c>
@@ -2589,11 +2577,11 @@
       <c r="C6" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="33" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
         <v>100</v>
       </c>
@@ -2603,11 +2591,11 @@
       <c r="C7" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>631</v>
+      <c r="D7" s="32" t="s">
+        <v>628</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>102</v>
       </c>
@@ -2617,11 +2605,11 @@
       <c r="C8" s="25" t="s">
         <v>476</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="34" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>102</v>
       </c>
@@ -2631,11 +2619,11 @@
       <c r="C9" s="25" t="s">
         <v>476</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="34" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>102</v>
       </c>
@@ -2645,11 +2633,11 @@
       <c r="C10" s="25" t="s">
         <v>476</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>627</v>
+      <c r="D10" s="32" t="s">
+        <v>624</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
         <v>104</v>
       </c>
@@ -2659,11 +2647,11 @@
       <c r="C11" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="33" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
         <v>104</v>
       </c>
@@ -2673,11 +2661,11 @@
       <c r="C12" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="33" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
         <v>104</v>
       </c>
@@ -2687,11 +2675,11 @@
       <c r="C13" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>632</v>
+      <c r="D13" s="32" t="s">
+        <v>629</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
         <v>106</v>
       </c>
@@ -2701,11 +2689,11 @@
       <c r="C14" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="34" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
         <v>109</v>
       </c>
@@ -2715,11 +2703,11 @@
       <c r="C15" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="34" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
         <v>112</v>
       </c>
@@ -2729,11 +2717,11 @@
       <c r="C16" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="34" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="23" t="s">
         <v>115</v>
       </c>
@@ -2743,11 +2731,11 @@
       <c r="C17" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="34" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>118</v>
       </c>
@@ -2757,11 +2745,11 @@
       <c r="C18" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="34" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
         <v>121</v>
       </c>
@@ -2771,11 +2759,11 @@
       <c r="C19" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="34" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
         <v>121</v>
       </c>
@@ -2785,11 +2773,11 @@
       <c r="C20" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="34" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>121</v>
       </c>
@@ -2799,11 +2787,11 @@
       <c r="C21" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="33" t="s">
-        <v>629</v>
+      <c r="D21" s="32" t="s">
+        <v>626</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="23" t="s">
         <v>124</v>
       </c>
@@ -2813,11 +2801,11 @@
       <c r="C22" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="34" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="23" t="s">
         <v>127</v>
       </c>
@@ -2827,11 +2815,11 @@
       <c r="C23" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="23" t="s">
         <v>130</v>
       </c>
@@ -2841,11 +2829,11 @@
       <c r="C24" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="34" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
         <v>133</v>
       </c>
@@ -2855,11 +2843,11 @@
       <c r="C25" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="34" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="23" t="s">
         <v>136</v>
       </c>
@@ -2869,11 +2857,11 @@
       <c r="C26" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="34" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>139</v>
       </c>
@@ -2883,11 +2871,11 @@
       <c r="C27" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="34" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="23" t="s">
         <v>142</v>
       </c>
@@ -2897,11 +2885,11 @@
       <c r="C28" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="34" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="23" t="s">
         <v>145</v>
       </c>
@@ -2911,11 +2899,11 @@
       <c r="C29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="34" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>148</v>
       </c>
@@ -2925,11 +2913,11 @@
       <c r="C30" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="34" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="23" t="s">
         <v>151</v>
       </c>
@@ -2939,11 +2927,11 @@
       <c r="C31" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="34" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>318</v>
       </c>
@@ -2953,11 +2941,11 @@
       <c r="C32" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="34" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
         <v>154</v>
       </c>
@@ -2967,11 +2955,11 @@
       <c r="C33" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="34" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
         <v>127</v>
       </c>
@@ -2981,11 +2969,11 @@
       <c r="C34" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="36" t="s">
+      <c r="D34" s="35" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>157</v>
       </c>
@@ -2995,11 +2983,11 @@
       <c r="C35" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="D35" s="35" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="23" t="s">
         <v>319</v>
       </c>
@@ -3009,11 +2997,11 @@
       <c r="C36" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="34" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="23" t="s">
         <v>157</v>
       </c>
@@ -3023,11 +3011,11 @@
       <c r="C37" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="35" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="23" t="s">
         <v>166</v>
       </c>
@@ -3037,11 +3025,11 @@
       <c r="C38" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="35" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="23" t="s">
         <v>166</v>
       </c>
@@ -3051,11 +3039,11 @@
       <c r="C39" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="D39" s="33" t="s">
-        <v>628</v>
+      <c r="D39" s="32" t="s">
+        <v>625</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="23" t="s">
         <v>160</v>
       </c>
@@ -3069,7 +3057,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="23" t="s">
         <v>160</v>
       </c>
@@ -3083,7 +3071,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="23" t="s">
         <v>115</v>
       </c>
@@ -3097,7 +3085,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="23" t="s">
         <v>163</v>
       </c>
@@ -3111,7 +3099,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="23" t="s">
         <v>166</v>
       </c>
@@ -3125,7 +3113,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>157</v>
       </c>
@@ -3139,7 +3127,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="23" t="s">
         <v>169</v>
       </c>
@@ -3153,7 +3141,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="23" t="s">
         <v>171</v>
       </c>
@@ -3167,7 +3155,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>358</v>
       </c>
@@ -3181,7 +3169,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>455</v>
       </c>
@@ -3195,7 +3183,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>365</v>
       </c>
@@ -3209,7 +3197,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="s">
         <v>368</v>
       </c>
@@ -3223,7 +3211,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="10" t="s">
         <v>371</v>
       </c>
@@ -3237,7 +3225,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
         <v>374</v>
       </c>
@@ -3251,7 +3239,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>377</v>
       </c>
@@ -3265,7 +3253,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
         <v>380</v>
       </c>
@@ -3279,7 +3267,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>383</v>
       </c>
@@ -3293,7 +3281,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>386</v>
       </c>
@@ -3307,7 +3295,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>389</v>
       </c>
@@ -3321,7 +3309,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>392</v>
       </c>
@@ -3335,7 +3323,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
         <v>395</v>
       </c>
@@ -3349,7 +3337,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>398</v>
       </c>
@@ -3363,7 +3351,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
         <v>401</v>
       </c>
@@ -3377,7 +3365,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>404</v>
       </c>
@@ -3391,7 +3379,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>407</v>
       </c>
@@ -3405,7 +3393,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>407</v>
       </c>
@@ -3419,7 +3407,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>410</v>
       </c>
@@ -3433,7 +3421,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>413</v>
       </c>
@@ -3447,7 +3435,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="12" t="s">
         <v>416</v>
       </c>
@@ -3461,7 +3449,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>419</v>
       </c>
@@ -3475,7 +3463,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>422</v>
       </c>
@@ -3489,7 +3477,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
         <v>425</v>
       </c>
@@ -3503,7 +3491,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>428</v>
       </c>
@@ -3517,7 +3505,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="12" t="s">
         <v>431</v>
       </c>
@@ -3531,7 +3519,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>434</v>
       </c>
@@ -3545,7 +3533,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>437</v>
       </c>
@@ -3559,7 +3547,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
         <v>440</v>
       </c>
@@ -3573,7 +3561,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
         <v>443</v>
       </c>
@@ -3587,7 +3575,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="s">
         <v>446</v>
       </c>
@@ -3601,7 +3589,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
         <v>449</v>
       </c>
@@ -3615,7 +3603,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="s">
         <v>452</v>
       </c>
@@ -3627,20 +3615,6 @@
       </c>
       <c r="D80" s="10" t="s">
         <v>453</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="31" t="s">
-        <v>624</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>625</v>
-      </c>
-      <c r="C81" s="31" t="s">
-        <v>626</v>
-      </c>
-      <c r="D81" s="31" t="s">
-        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -3657,9 +3631,9 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -3673,7 +3647,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3687,7 +3661,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3701,7 +3675,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3715,7 +3689,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>309</v>
       </c>
@@ -3729,7 +3703,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>310</v>
       </c>
@@ -3743,7 +3717,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3757,7 +3731,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3771,7 +3745,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3785,7 +3759,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3799,7 +3773,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3813,7 +3787,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>621</v>
       </c>
@@ -3840,33 +3814,33 @@
   </sheetPr>
   <dimension ref="A1:XFC131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="15" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="16" max="16" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>501</v>
       </c>
@@ -3919,7 +3893,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>334</v>
       </c>
@@ -3948,15 +3922,15 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>651</v>
+      <c r="B3" s="37" t="s">
+        <v>648</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>468</v>
@@ -3977,7 +3951,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -4006,7 +3980,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
@@ -4035,7 +4009,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -4043,7 +4017,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>468</v>
@@ -4064,7 +4038,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -4093,7 +4067,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -4122,7 +4096,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -4151,7 +4125,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>547</v>
       </c>
@@ -4180,7 +4154,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -4209,7 +4183,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -4238,7 +4212,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>264</v>
       </c>
@@ -4267,7 +4241,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -4296,7 +4270,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>518</v>
       </c>
@@ -4325,7 +4299,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>549</v>
       </c>
@@ -4354,7 +4328,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -4383,7 +4357,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>553</v>
       </c>
@@ -4412,7 +4386,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -4441,7 +4415,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>550</v>
       </c>
@@ -4470,7 +4444,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -4499,7 +4473,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>552</v>
       </c>
@@ -4528,7 +4502,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -4557,7 +4531,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>548</v>
       </c>
@@ -4586,7 +4560,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -4615,7 +4589,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>456</v>
       </c>
@@ -4644,7 +4618,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -4673,7 +4647,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4702,7 +4676,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>551</v>
       </c>
@@ -4731,7 +4705,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
@@ -4760,7 +4734,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>459</v>
       </c>
@@ -4789,7 +4763,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>460</v>
       </c>
@@ -4818,7 +4792,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
@@ -4847,7 +4821,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>77</v>
       </c>
@@ -4876,7 +4850,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -4905,7 +4879,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>461</v>
       </c>
@@ -4934,7 +4908,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>462</v>
       </c>
@@ -4963,7 +4937,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>463</v>
       </c>
@@ -4992,7 +4966,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>464</v>
       </c>
@@ -5021,7 +4995,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>465</v>
       </c>
@@ -5050,7 +5024,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>350</v>
       </c>
@@ -5079,7 +5053,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>351</v>
       </c>
@@ -5108,7 +5082,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>517</v>
       </c>
@@ -5137,7 +5111,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>466</v>
       </c>
@@ -5166,7 +5140,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>516</v>
       </c>
@@ -5195,7 +5169,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>352</v>
       </c>
@@ -5224,7 +5198,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>353</v>
       </c>
@@ -5253,7 +5227,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>354</v>
       </c>
@@ -5282,7 +5256,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>355</v>
       </c>
@@ -5311,7 +5285,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>174</v>
       </c>
@@ -5340,7 +5314,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>176</v>
       </c>
@@ -5369,7 +5343,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>178</v>
       </c>
@@ -5398,7 +5372,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>180</v>
       </c>
@@ -5427,7 +5401,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>182</v>
       </c>
@@ -5456,7 +5430,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>184</v>
       </c>
@@ -5485,7 +5459,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>186</v>
       </c>
@@ -5514,7 +5488,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>188</v>
       </c>
@@ -5543,7 +5517,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>190</v>
       </c>
@@ -5572,7 +5546,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>192</v>
       </c>
@@ -5601,7 +5575,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>194</v>
       </c>
@@ -5630,7 +5604,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>196</v>
       </c>
@@ -5659,7 +5633,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>198</v>
       </c>
@@ -5688,7 +5662,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>200</v>
       </c>
@@ -5717,7 +5691,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>202</v>
       </c>
@@ -5746,7 +5720,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>204</v>
       </c>
@@ -5775,7 +5749,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>206</v>
       </c>
@@ -5804,7 +5778,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>294</v>
       </c>
@@ -5833,7 +5807,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>293</v>
       </c>
@@ -5862,7 +5836,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>292</v>
       </c>
@@ -5891,7 +5865,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
         <v>291</v>
       </c>
@@ -5920,7 +5894,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>290</v>
       </c>
@@ -5949,7 +5923,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>289</v>
       </c>
@@ -5978,7 +5952,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>288</v>
       </c>
@@ -6007,7 +5981,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>287</v>
       </c>
@@ -6036,7 +6010,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>286</v>
       </c>
@@ -6065,7 +6039,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
         <v>284</v>
       </c>
@@ -6094,7 +6068,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>285</v>
       </c>
@@ -6123,7 +6097,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>295</v>
       </c>
@@ -6152,7 +6126,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>298</v>
       </c>
@@ -6181,7 +6155,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
         <v>297</v>
       </c>
@@ -6210,7 +6184,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
         <v>296</v>
       </c>
@@ -6239,7 +6213,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>313</v>
       </c>
@@ -6276,7 +6250,7 @@
       <c r="P82" s="8"/>
       <c r="Q82" s="8"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>314</v>
       </c>
@@ -6313,7 +6287,7 @@
       <c r="P83" s="8"/>
       <c r="Q83" s="8"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
         <v>315</v>
       </c>
@@ -6350,7 +6324,7 @@
       <c r="P84" s="8"/>
       <c r="Q84" s="8"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="18" t="s">
         <v>515</v>
       </c>
@@ -6387,7 +6361,7 @@
       <c r="P85" s="8"/>
       <c r="Q85" s="8"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="18" t="s">
         <v>277</v>
       </c>
@@ -6424,7 +6398,7 @@
       <c r="P86" s="8"/>
       <c r="Q86" s="8"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="18" t="s">
         <v>278</v>
       </c>
@@ -6461,7 +6435,7 @@
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="18" t="s">
         <v>279</v>
       </c>
@@ -6498,7 +6472,7 @@
       <c r="P88" s="8"/>
       <c r="Q88" s="8"/>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="18" t="s">
         <v>280</v>
       </c>
@@ -6535,7 +6509,7 @@
       <c r="P89" s="8"/>
       <c r="Q89" s="8"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="18" t="s">
         <v>281</v>
       </c>
@@ -6572,7 +6546,7 @@
       <c r="P90" s="8"/>
       <c r="Q90" s="8"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="18" t="s">
         <v>283</v>
       </c>
@@ -6609,7 +6583,7 @@
       <c r="P91" s="8"/>
       <c r="Q91" s="8"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="17" t="s">
         <v>269</v>
       </c>
@@ -6646,7 +6620,7 @@
       <c r="P92" s="8"/>
       <c r="Q92" s="8"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="17" t="s">
         <v>311</v>
       </c>
@@ -6683,7 +6657,7 @@
       <c r="P93" s="8"/>
       <c r="Q93" s="8"/>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="17" t="s">
         <v>312</v>
       </c>
@@ -6720,7 +6694,7 @@
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="18" t="s">
         <v>282</v>
       </c>
@@ -6757,7 +6731,7 @@
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="14" t="s">
         <v>265</v>
       </c>
@@ -6786,7 +6760,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="14" t="s">
         <v>266</v>
       </c>
@@ -6815,7 +6789,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98" s="14" t="s">
         <v>267</v>
       </c>
@@ -6844,7 +6818,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
         <v>268</v>
       </c>
@@ -6873,7 +6847,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
         <v>316</v>
       </c>
@@ -6902,7 +6876,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
         <v>270</v>
       </c>
@@ -6931,7 +6905,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A102" s="14" t="s">
         <v>271</v>
       </c>
@@ -6960,7 +6934,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
         <v>272</v>
       </c>
@@ -6989,7 +6963,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104" s="14" t="s">
         <v>273</v>
       </c>
@@ -7018,7 +6992,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105" s="14" t="s">
         <v>274</v>
       </c>
@@ -7047,7 +7021,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A106" s="14" t="s">
         <v>275</v>
       </c>
@@ -7076,7 +7050,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
         <v>276</v>
       </c>
@@ -7105,7 +7079,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="s">
         <v>308</v>
       </c>
@@ -7131,7 +7105,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A109" s="20" t="s">
         <v>307</v>
       </c>
@@ -7157,7 +7131,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="s">
         <v>542</v>
       </c>
@@ -7168,7 +7142,7 @@
         <v>304</v>
       </c>
       <c r="D110" s="15" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E110" s="21" t="s">
         <v>546</v>
@@ -7183,23 +7157,23 @@
       <c r="L110" s="15" t="s">
         <v>472</v>
       </c>
-      <c r="M110" s="37" t="s">
+      <c r="M110" s="36" t="s">
+        <v>635</v>
+      </c>
+      <c r="N110" s="36" t="s">
+        <v>636</v>
+      </c>
+      <c r="O110" s="36" t="s">
+        <v>637</v>
+      </c>
+      <c r="P110" s="36" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q110" s="36" t="s">
         <v>638</v>
       </c>
-      <c r="N110" s="37" t="s">
-        <v>639</v>
-      </c>
-      <c r="O110" s="37" t="s">
-        <v>640</v>
-      </c>
-      <c r="P110" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q110" s="37" t="s">
-        <v>641</v>
-      </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111" s="20" t="s">
         <v>543</v>
       </c>
@@ -7210,7 +7184,7 @@
         <v>306</v>
       </c>
       <c r="D111" s="15" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E111" s="21" t="s">
         <v>546</v>
@@ -7225,23 +7199,23 @@
       <c r="L111" s="15" t="s">
         <v>472</v>
       </c>
-      <c r="M111" s="37" t="s">
+      <c r="M111" s="36" t="s">
+        <v>635</v>
+      </c>
+      <c r="N111" s="36" t="s">
+        <v>636</v>
+      </c>
+      <c r="O111" s="36" t="s">
+        <v>637</v>
+      </c>
+      <c r="P111" s="36" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q111" s="36" t="s">
         <v>638</v>
       </c>
-      <c r="N111" s="37" t="s">
-        <v>639</v>
-      </c>
-      <c r="O111" s="37" t="s">
-        <v>640</v>
-      </c>
-      <c r="P111" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q111" s="37" t="s">
-        <v>641</v>
-      </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A112" s="6" t="s">
         <v>320</v>
       </c>
@@ -7278,7 +7252,7 @@
       <c r="P112" s="13"/>
       <c r="Q112" s="13"/>
     </row>
-    <row r="113" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A113" s="6" t="s">
         <v>321</v>
       </c>
@@ -7315,7 +7289,7 @@
       <c r="P113" s="13"/>
       <c r="Q113" s="13"/>
     </row>
-    <row r="114" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
         <v>322</v>
       </c>
@@ -7352,7 +7326,7 @@
       <c r="P114" s="13"/>
       <c r="Q114" s="13"/>
     </row>
-    <row r="115" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
         <v>323</v>
       </c>
@@ -7389,7 +7363,7 @@
       <c r="P115" s="13"/>
       <c r="Q115" s="13"/>
     </row>
-    <row r="116" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
         <v>324</v>
       </c>
@@ -7426,7 +7400,7 @@
       <c r="P116" s="13"/>
       <c r="Q116" s="13"/>
     </row>
-    <row r="117" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
         <v>325</v>
       </c>
@@ -7463,7 +7437,7 @@
       <c r="P117" s="13"/>
       <c r="Q117" s="13"/>
     </row>
-    <row r="118" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
         <v>326</v>
       </c>
@@ -7500,7 +7474,7 @@
       <c r="P118" s="13"/>
       <c r="Q118" s="13"/>
     </row>
-    <row r="119" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
         <v>504</v>
       </c>
@@ -7511,37 +7485,37 @@
         <v>512</v>
       </c>
       <c r="D119" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="E119" s="37" t="s">
-        <v>634</v>
+        <v>644</v>
+      </c>
+      <c r="E119" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G119" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="J119" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L119" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M119" s="37" t="s">
-        <v>642</v>
-      </c>
-      <c r="N119" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="O119" s="37" t="s">
+      <c r="M119" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="N119" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="O119" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P119" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="P119" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q119" s="37" t="s">
-        <v>644</v>
+      <c r="Q119" s="36" t="s">
+        <v>641</v>
       </c>
     </row>
-    <row r="120" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
         <v>505</v>
       </c>
@@ -7552,37 +7526,37 @@
         <v>512</v>
       </c>
       <c r="D120" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="E120" s="37" t="s">
-        <v>634</v>
+        <v>644</v>
+      </c>
+      <c r="E120" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G120" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="J120" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L120" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M120" s="37" t="s">
-        <v>642</v>
-      </c>
-      <c r="N120" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="O120" s="37" t="s">
+      <c r="M120" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="N120" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="O120" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P120" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="P120" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q120" s="37" t="s">
-        <v>644</v>
+      <c r="Q120" s="36" t="s">
+        <v>641</v>
       </c>
     </row>
-    <row r="121" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
         <v>506</v>
       </c>
@@ -7593,37 +7567,37 @@
         <v>512</v>
       </c>
       <c r="D121" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="E121" s="37" t="s">
-        <v>634</v>
+        <v>644</v>
+      </c>
+      <c r="E121" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G121" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="J121" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L121" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M121" s="37" t="s">
-        <v>642</v>
-      </c>
-      <c r="N121" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="O121" s="37" t="s">
+      <c r="M121" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="N121" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="O121" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P121" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="P121" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q121" s="37" t="s">
-        <v>644</v>
+      <c r="Q121" s="36" t="s">
+        <v>641</v>
       </c>
     </row>
-    <row r="122" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
         <v>507</v>
       </c>
@@ -7634,37 +7608,37 @@
         <v>512</v>
       </c>
       <c r="D122" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="E122" s="37" t="s">
-        <v>634</v>
+        <v>644</v>
+      </c>
+      <c r="E122" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G122" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="J122" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L122" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M122" s="37" t="s">
-        <v>642</v>
-      </c>
-      <c r="N122" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="O122" s="37" t="s">
+      <c r="M122" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="N122" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="O122" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P122" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="P122" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q122" s="37" t="s">
-        <v>644</v>
+      <c r="Q122" s="36" t="s">
+        <v>641</v>
       </c>
     </row>
-    <row r="123" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A123" s="6" t="s">
         <v>511</v>
       </c>
@@ -7675,37 +7649,37 @@
         <v>512</v>
       </c>
       <c r="D123" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="E123" s="37" t="s">
-        <v>634</v>
+        <v>644</v>
+      </c>
+      <c r="E123" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G123" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="J123" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L123" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M123" s="37" t="s">
-        <v>642</v>
-      </c>
-      <c r="N123" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="O123" s="37" t="s">
+      <c r="M123" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="N123" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="O123" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P123" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="P123" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q123" s="37" t="s">
-        <v>644</v>
+      <c r="Q123" s="36" t="s">
+        <v>641</v>
       </c>
     </row>
-    <row r="124" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
         <v>508</v>
       </c>
@@ -7716,37 +7690,37 @@
         <v>514</v>
       </c>
       <c r="D124" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="E124" s="37" t="s">
-        <v>634</v>
+        <v>644</v>
+      </c>
+      <c r="E124" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G124" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="J124" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L124" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M124" s="37" t="s">
-        <v>642</v>
-      </c>
-      <c r="N124" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="O124" s="37" t="s">
+      <c r="M124" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="N124" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="O124" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P124" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="P124" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q124" s="37" t="s">
-        <v>644</v>
+      <c r="Q124" s="36" t="s">
+        <v>641</v>
       </c>
     </row>
-    <row r="125" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
         <v>509</v>
       </c>
@@ -7757,37 +7731,37 @@
         <v>514</v>
       </c>
       <c r="D125" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="E125" s="37" t="s">
-        <v>634</v>
+        <v>644</v>
+      </c>
+      <c r="E125" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G125" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="J125" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L125" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M125" s="37" t="s">
-        <v>642</v>
-      </c>
-      <c r="N125" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="O125" s="37" t="s">
+      <c r="M125" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="N125" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="O125" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P125" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="P125" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q125" s="37" t="s">
-        <v>644</v>
+      <c r="Q125" s="36" t="s">
+        <v>641</v>
       </c>
     </row>
-    <row r="126" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A126" s="28" t="s">
         <v>523</v>
       </c>
@@ -7797,11 +7771,11 @@
       <c r="C126" s="29" t="s">
         <v>525</v>
       </c>
-      <c r="D126" s="37" t="s">
-        <v>648</v>
-      </c>
-      <c r="E126" s="37" t="s">
-        <v>634</v>
+      <c r="D126" s="36" t="s">
+        <v>645</v>
+      </c>
+      <c r="E126" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="F126"/>
       <c r="G126" s="29" t="s">
@@ -7814,20 +7788,20 @@
       <c r="L126" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M126" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="N126" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="O126" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="P126" s="37" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q126" s="37" t="s">
-        <v>645</v>
+      <c r="M126" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="N126" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="O126" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P126" s="36" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q126" s="36" t="s">
+        <v>642</v>
       </c>
       <c r="R126"/>
       <c r="S126"/>
@@ -24196,7 +24170,7 @@
       <c r="XFB126"/>
       <c r="XFC126"/>
     </row>
-    <row r="127" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A127" s="28" t="s">
         <v>540</v>
       </c>
@@ -24206,11 +24180,11 @@
       <c r="C127" s="29" t="s">
         <v>527</v>
       </c>
-      <c r="D127" s="37" t="s">
-        <v>648</v>
-      </c>
-      <c r="E127" s="37" t="s">
-        <v>634</v>
+      <c r="D127" s="36" t="s">
+        <v>645</v>
+      </c>
+      <c r="E127" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="F127"/>
       <c r="G127" s="29" t="s">
@@ -24223,20 +24197,20 @@
       <c r="L127" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M127" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="N127" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="O127" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="P127" s="37" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q127" s="37" t="s">
-        <v>645</v>
+      <c r="M127" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="N127" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="O127" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P127" s="36" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q127" s="36" t="s">
+        <v>642</v>
       </c>
       <c r="R127"/>
       <c r="S127"/>
@@ -40605,7 +40579,7 @@
       <c r="XFB127"/>
       <c r="XFC127"/>
     </row>
-    <row r="128" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A128" s="28" t="s">
         <v>528</v>
       </c>
@@ -40615,11 +40589,11 @@
       <c r="C128" s="29" t="s">
         <v>530</v>
       </c>
-      <c r="D128" s="37" t="s">
-        <v>648</v>
-      </c>
-      <c r="E128" s="37" t="s">
-        <v>634</v>
+      <c r="D128" s="36" t="s">
+        <v>645</v>
+      </c>
+      <c r="E128" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="F128"/>
       <c r="G128" s="29" t="s">
@@ -40632,20 +40606,20 @@
       <c r="L128" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M128" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="N128" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="O128" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="P128" s="37" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q128" s="37" t="s">
-        <v>644</v>
+      <c r="M128" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="N128" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="O128" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P128" s="36" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q128" s="36" t="s">
+        <v>641</v>
       </c>
       <c r="R128"/>
       <c r="S128"/>
@@ -57014,7 +56988,7 @@
       <c r="XFB128"/>
       <c r="XFC128"/>
     </row>
-    <row r="129" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A129" s="28" t="s">
         <v>541</v>
       </c>
@@ -57024,11 +56998,11 @@
       <c r="C129" s="29" t="s">
         <v>533</v>
       </c>
-      <c r="D129" s="37" t="s">
-        <v>648</v>
-      </c>
-      <c r="E129" s="37" t="s">
-        <v>634</v>
+      <c r="D129" s="36" t="s">
+        <v>645</v>
+      </c>
+      <c r="E129" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="F129"/>
       <c r="G129" s="29" t="s">
@@ -57041,20 +57015,20 @@
       <c r="L129" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M129" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="N129" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="O129" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="P129" s="37" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q129" s="37" t="s">
-        <v>644</v>
+      <c r="M129" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="N129" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="O129" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="P129" s="36" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q129" s="36" t="s">
+        <v>641</v>
       </c>
       <c r="R129"/>
       <c r="S129"/>
@@ -73423,7 +73397,7 @@
       <c r="XFB129"/>
       <c r="XFC129"/>
     </row>
-    <row r="130" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A130" s="28" t="s">
         <v>534</v>
       </c>
@@ -73433,11 +73407,11 @@
       <c r="C130" s="29" t="s">
         <v>536</v>
       </c>
-      <c r="D130" s="37" t="s">
-        <v>648</v>
-      </c>
-      <c r="E130" s="37" t="s">
-        <v>634</v>
+      <c r="D130" s="36" t="s">
+        <v>645</v>
+      </c>
+      <c r="E130" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G130" s="30" t="s">
         <v>545</v>
@@ -73445,23 +73419,23 @@
       <c r="L130" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M130" s="37" t="s">
+      <c r="M130" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="N130" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="O130" s="15" t="s">
+        <v>633</v>
+      </c>
+      <c r="P130" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="N130" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="O130" s="15" t="s">
-        <v>636</v>
-      </c>
-      <c r="P130" s="15" t="s">
-        <v>637</v>
-      </c>
       <c r="Q130" s="15" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
-    <row r="131" spans="1:16383" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16383" x14ac:dyDescent="0.35">
       <c r="A131" s="28" t="s">
         <v>539</v>
       </c>
@@ -73471,11 +73445,11 @@
       <c r="C131" s="29" t="s">
         <v>538</v>
       </c>
-      <c r="D131" s="37" t="s">
-        <v>648</v>
-      </c>
-      <c r="E131" s="37" t="s">
-        <v>634</v>
+      <c r="D131" s="36" t="s">
+        <v>645</v>
+      </c>
+      <c r="E131" s="36" t="s">
+        <v>631</v>
       </c>
       <c r="G131" s="30" t="s">
         <v>545</v>
@@ -73483,20 +73457,20 @@
       <c r="L131" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="M131" s="37" t="s">
+      <c r="M131" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="N131" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="O131" s="15" t="s">
+        <v>633</v>
+      </c>
+      <c r="P131" s="15" t="s">
         <v>634</v>
       </c>
-      <c r="N131" s="37" t="s">
-        <v>634</v>
-      </c>
-      <c r="O131" s="15" t="s">
-        <v>636</v>
-      </c>
-      <c r="P131" s="15" t="s">
-        <v>637</v>
-      </c>
       <c r="Q131" s="15" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Codelist - Dioktyltenn-jon, CH01/172 korrigerad
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MFO_Privat\MG\Personliga mappar\Anne LS\temp\MoCiS2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3970" windowWidth="29040" windowHeight="15840" tabRatio="877"/>
+    <workbookView xWindow="28680" yWindow="-3525" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -1971,13 +1971,13 @@
     <t>NRM</t>
   </si>
   <si>
-    <t>CH01/171</t>
-  </si>
-  <si>
     <t>CH01/174</t>
   </si>
   <si>
-    <t>Dioktyltenn - opecificerade atomer/molekyler bundna till dioktyltenn</t>
+    <t>Dioktyltenn-jon</t>
+  </si>
+  <si>
+    <t>CH01/172</t>
   </si>
 </sst>
 </file>
@@ -2195,8 +2195,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Bra" xfId="4" builtinId="26"/>
-    <cellStyle name="Dålig" xfId="1" builtinId="27"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="6"/>
     <cellStyle name="Normal 2 2" xfId="12"/>
@@ -2487,17 +2487,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A81" sqref="A81:XFD81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.1796875" style="31" customWidth="1"/>
-    <col min="3" max="4" width="38.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="31" customWidth="1"/>
+    <col min="3" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>97</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>98</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>98</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>98</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>100</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>100</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>100</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>102</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>102</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>102</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>104</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>104</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>104</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>106</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>109</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>112</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>115</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>118</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>121</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>121</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>121</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>124</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>127</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>130</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>133</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>136</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>139</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>142</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>145</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>148</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>151</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>318</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>154</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>127</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>157</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>319</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>157</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>166</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>166</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>160</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>160</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>115</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>163</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>166</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>157</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>169</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>171</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>358</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>455</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>365</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>368</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>371</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>374</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>377</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>380</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>383</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>386</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>389</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>392</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>395</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>398</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>401</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>404</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>407</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>407</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>410</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>413</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>416</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>419</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>422</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>425</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>428</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>431</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>434</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>437</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>440</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>443</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>446</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>449</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>452</v>
       </c>
@@ -3631,9 +3631,9 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>309</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>310</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>621</v>
       </c>
@@ -3814,33 +3814,33 @@
   </sheetPr>
   <dimension ref="A1:XFC131"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="15" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.54296875" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.26953125" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26953125" style="1"/>
+    <col min="16" max="16" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>501</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>334</v>
       </c>
@@ -3922,15 +3922,15 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="37" t="s">
+        <v>647</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>648</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>646</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>468</v>
@@ -3951,7 +3951,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>468</v>
@@ -4038,7 +4038,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>547</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>264</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>518</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>549</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>553</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>550</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>552</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>548</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>456</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>551</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>459</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>460</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>77</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>461</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>462</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>463</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>464</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>465</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>350</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>351</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>517</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>466</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>516</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>352</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>353</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>354</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>355</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>174</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>176</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>178</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>180</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>182</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>184</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>186</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>188</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>190</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>192</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>194</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>196</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>198</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>200</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>202</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>204</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>206</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>294</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>293</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>292</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>291</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>290</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>289</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>288</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>287</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>286</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>284</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>285</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>295</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>298</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>297</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>296</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>313</v>
       </c>
@@ -6250,7 +6250,7 @@
       <c r="P82" s="8"/>
       <c r="Q82" s="8"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>314</v>
       </c>
@@ -6287,7 +6287,7 @@
       <c r="P83" s="8"/>
       <c r="Q83" s="8"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>315</v>
       </c>
@@ -6324,7 +6324,7 @@
       <c r="P84" s="8"/>
       <c r="Q84" s="8"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
         <v>515</v>
       </c>
@@ -6361,7 +6361,7 @@
       <c r="P85" s="8"/>
       <c r="Q85" s="8"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
         <v>277</v>
       </c>
@@ -6398,7 +6398,7 @@
       <c r="P86" s="8"/>
       <c r="Q86" s="8"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
         <v>278</v>
       </c>
@@ -6435,7 +6435,7 @@
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
         <v>279</v>
       </c>
@@ -6472,7 +6472,7 @@
       <c r="P88" s="8"/>
       <c r="Q88" s="8"/>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
         <v>280</v>
       </c>
@@ -6509,7 +6509,7 @@
       <c r="P89" s="8"/>
       <c r="Q89" s="8"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
         <v>281</v>
       </c>
@@ -6546,7 +6546,7 @@
       <c r="P90" s="8"/>
       <c r="Q90" s="8"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
         <v>283</v>
       </c>
@@ -6583,7 +6583,7 @@
       <c r="P91" s="8"/>
       <c r="Q91" s="8"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>269</v>
       </c>
@@ -6620,7 +6620,7 @@
       <c r="P92" s="8"/>
       <c r="Q92" s="8"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>311</v>
       </c>
@@ -6657,7 +6657,7 @@
       <c r="P93" s="8"/>
       <c r="Q93" s="8"/>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>312</v>
       </c>
@@ -6694,7 +6694,7 @@
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
         <v>282</v>
       </c>
@@ -6731,7 +6731,7 @@
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>265</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>266</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>267</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>268</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
         <v>316</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
         <v>270</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>271</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
         <v>272</v>
       </c>
@@ -6963,7 +6963,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>273</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
         <v>274</v>
       </c>
@@ -7021,7 +7021,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
         <v>275</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
         <v>276</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="s">
         <v>308</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="s">
         <v>307</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="s">
         <v>542</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="s">
         <v>543</v>
       </c>
@@ -7215,7 +7215,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>320</v>
       </c>
@@ -7252,7 +7252,7 @@
       <c r="P112" s="13"/>
       <c r="Q112" s="13"/>
     </row>
-    <row r="113" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>321</v>
       </c>
@@ -7289,7 +7289,7 @@
       <c r="P113" s="13"/>
       <c r="Q113" s="13"/>
     </row>
-    <row r="114" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>322</v>
       </c>
@@ -7326,7 +7326,7 @@
       <c r="P114" s="13"/>
       <c r="Q114" s="13"/>
     </row>
-    <row r="115" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>323</v>
       </c>
@@ -7363,7 +7363,7 @@
       <c r="P115" s="13"/>
       <c r="Q115" s="13"/>
     </row>
-    <row r="116" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>324</v>
       </c>
@@ -7400,7 +7400,7 @@
       <c r="P116" s="13"/>
       <c r="Q116" s="13"/>
     </row>
-    <row r="117" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>325</v>
       </c>
@@ -7437,7 +7437,7 @@
       <c r="P117" s="13"/>
       <c r="Q117" s="13"/>
     </row>
-    <row r="118" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>326</v>
       </c>
@@ -7474,7 +7474,7 @@
       <c r="P118" s="13"/>
       <c r="Q118" s="13"/>
     </row>
-    <row r="119" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>504</v>
       </c>
@@ -7515,7 +7515,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="120" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>505</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="121" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>506</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="122" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>507</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="123" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>511</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="124" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>508</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="125" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>509</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="126" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A126" s="28" t="s">
         <v>523</v>
       </c>
@@ -24170,7 +24170,7 @@
       <c r="XFB126"/>
       <c r="XFC126"/>
     </row>
-    <row r="127" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A127" s="28" t="s">
         <v>540</v>
       </c>
@@ -40579,7 +40579,7 @@
       <c r="XFB127"/>
       <c r="XFC127"/>
     </row>
-    <row r="128" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A128" s="28" t="s">
         <v>528</v>
       </c>
@@ -56988,7 +56988,7 @@
       <c r="XFB128"/>
       <c r="XFC128"/>
     </row>
-    <row r="129" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A129" s="28" t="s">
         <v>541</v>
       </c>
@@ -73397,7 +73397,7 @@
       <c r="XFB129"/>
       <c r="XFC129"/>
     </row>
-    <row r="130" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A130" s="28" t="s">
         <v>534</v>
       </c>
@@ -73435,7 +73435,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="131" spans="1:16383" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A131" s="28" t="s">
         <v>539</v>
       </c>

</xml_diff>

<commit_message>
Salvelinus changed to Salvelinus alpinus
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3525" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-3075" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -1599,9 +1599,6 @@
     <t>Limmingsjön</t>
   </si>
   <si>
-    <t>Salvelinus</t>
-  </si>
-  <si>
     <t>TOTL</t>
   </si>
   <si>
@@ -1978,6 +1975,9 @@
   </si>
   <si>
     <t>CH01/172</t>
+  </si>
+  <si>
+    <t>Salvelinus alpinus</t>
   </si>
 </sst>
 </file>
@@ -2550,7 +2550,7 @@
         <v>478</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
         <v>475</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2634,7 +2634,7 @@
         <v>476</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2676,7 +2676,7 @@
         <v>477</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
         <v>123</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
         <v>168</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3627,8 +3627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3714,7 +3714,7 @@
         <v>206231</v>
       </c>
       <c r="D6" t="s">
-        <v>522</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3789,16 +3789,16 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>620</v>
+      </c>
+      <c r="B12" t="s">
         <v>621</v>
-      </c>
-      <c r="B12" t="s">
-        <v>622</v>
       </c>
       <c r="C12">
         <v>206135</v>
       </c>
       <c r="D12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -3814,7 +3814,7 @@
   </sheetPr>
   <dimension ref="A1:XFC131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
@@ -3927,10 +3927,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>647</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>648</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>468</v>
@@ -4017,7 +4017,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>468</v>
@@ -4127,7 +4127,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>
@@ -4359,7 +4359,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B18" t="s">
         <v>59</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
@@ -4475,7 +4475,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B22" t="s">
         <v>63</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B24" t="s">
         <v>65</v>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B29" t="s">
         <v>71</v>
@@ -4739,7 +4739,7 @@
         <v>459</v>
       </c>
       <c r="B31" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>73</v>
@@ -4768,7 +4768,7 @@
         <v>460</v>
       </c>
       <c r="B32" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>74</v>
@@ -4797,7 +4797,7 @@
         <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>76</v>
@@ -4826,7 +4826,7 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>78</v>
@@ -4855,7 +4855,7 @@
         <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>80</v>
@@ -4884,7 +4884,7 @@
         <v>461</v>
       </c>
       <c r="B36" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>81</v>
@@ -4913,7 +4913,7 @@
         <v>462</v>
       </c>
       <c r="B37" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>82</v>
@@ -4942,7 +4942,7 @@
         <v>463</v>
       </c>
       <c r="B38" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>83</v>
@@ -4971,7 +4971,7 @@
         <v>464</v>
       </c>
       <c r="B39" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>84</v>
@@ -5000,7 +5000,7 @@
         <v>465</v>
       </c>
       <c r="B40" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>85</v>
@@ -5029,7 +5029,7 @@
         <v>350</v>
       </c>
       <c r="B41" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>86</v>
@@ -5058,7 +5058,7 @@
         <v>351</v>
       </c>
       <c r="B42" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>87</v>
@@ -5087,7 +5087,7 @@
         <v>517</v>
       </c>
       <c r="B43" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>88</v>
@@ -5116,7 +5116,7 @@
         <v>466</v>
       </c>
       <c r="B44" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>89</v>
@@ -5145,7 +5145,7 @@
         <v>516</v>
       </c>
       <c r="B45" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>90</v>
@@ -5174,7 +5174,7 @@
         <v>352</v>
       </c>
       <c r="B46" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>91</v>
@@ -5203,7 +5203,7 @@
         <v>353</v>
       </c>
       <c r="B47" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>92</v>
@@ -5232,7 +5232,7 @@
         <v>354</v>
       </c>
       <c r="B48" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>93</v>
@@ -5261,7 +5261,7 @@
         <v>355</v>
       </c>
       <c r="B49" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>94</v>
@@ -5290,7 +5290,7 @@
         <v>174</v>
       </c>
       <c r="B50" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>175</v>
@@ -5319,7 +5319,7 @@
         <v>176</v>
       </c>
       <c r="B51" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>177</v>
@@ -5348,7 +5348,7 @@
         <v>178</v>
       </c>
       <c r="B52" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>179</v>
@@ -5377,7 +5377,7 @@
         <v>180</v>
       </c>
       <c r="B53" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>181</v>
@@ -5406,7 +5406,7 @@
         <v>182</v>
       </c>
       <c r="B54" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>183</v>
@@ -5435,7 +5435,7 @@
         <v>184</v>
       </c>
       <c r="B55" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>185</v>
@@ -5464,7 +5464,7 @@
         <v>186</v>
       </c>
       <c r="B56" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>187</v>
@@ -5493,7 +5493,7 @@
         <v>188</v>
       </c>
       <c r="B57" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>189</v>
@@ -5522,7 +5522,7 @@
         <v>190</v>
       </c>
       <c r="B58" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>191</v>
@@ -5551,7 +5551,7 @@
         <v>192</v>
       </c>
       <c r="B59" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>193</v>
@@ -5580,7 +5580,7 @@
         <v>194</v>
       </c>
       <c r="B60" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>195</v>
@@ -5609,7 +5609,7 @@
         <v>196</v>
       </c>
       <c r="B61" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>197</v>
@@ -5638,7 +5638,7 @@
         <v>198</v>
       </c>
       <c r="B62" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>199</v>
@@ -5667,7 +5667,7 @@
         <v>200</v>
       </c>
       <c r="B63" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>201</v>
@@ -5696,7 +5696,7 @@
         <v>202</v>
       </c>
       <c r="B64" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>203</v>
@@ -5725,7 +5725,7 @@
         <v>204</v>
       </c>
       <c r="B65" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>205</v>
@@ -5754,7 +5754,7 @@
         <v>206</v>
       </c>
       <c r="B66" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>207</v>
@@ -6218,7 +6218,7 @@
         <v>313</v>
       </c>
       <c r="B82" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>238</v>
@@ -6255,7 +6255,7 @@
         <v>314</v>
       </c>
       <c r="B83" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>239</v>
@@ -6292,7 +6292,7 @@
         <v>315</v>
       </c>
       <c r="B84" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>240</v>
@@ -6329,7 +6329,7 @@
         <v>515</v>
       </c>
       <c r="B85" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>241</v>
@@ -6366,7 +6366,7 @@
         <v>277</v>
       </c>
       <c r="B86" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C86" s="13" t="s">
         <v>242</v>
@@ -6403,7 +6403,7 @@
         <v>278</v>
       </c>
       <c r="B87" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>243</v>
@@ -6477,7 +6477,7 @@
         <v>280</v>
       </c>
       <c r="B89" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C89" s="13" t="s">
         <v>246</v>
@@ -6514,7 +6514,7 @@
         <v>281</v>
       </c>
       <c r="B90" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C90" s="13" t="s">
         <v>247</v>
@@ -6551,7 +6551,7 @@
         <v>283</v>
       </c>
       <c r="B91" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C91" s="13" t="s">
         <v>248</v>
@@ -6588,7 +6588,7 @@
         <v>269</v>
       </c>
       <c r="B92" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C92" s="13" t="s">
         <v>249</v>
@@ -6625,7 +6625,7 @@
         <v>311</v>
       </c>
       <c r="B93" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C93" s="13" t="s">
         <v>250</v>
@@ -6662,7 +6662,7 @@
         <v>312</v>
       </c>
       <c r="B94" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C94" s="13" t="s">
         <v>251</v>
@@ -6699,7 +6699,7 @@
         <v>282</v>
       </c>
       <c r="B95" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C95" s="13" t="s">
         <v>252</v>
@@ -6736,7 +6736,7 @@
         <v>265</v>
       </c>
       <c r="B96" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C96" s="13" t="s">
         <v>253</v>
@@ -6765,7 +6765,7 @@
         <v>266</v>
       </c>
       <c r="B97" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C97" s="13" t="s">
         <v>254</v>
@@ -6794,7 +6794,7 @@
         <v>267</v>
       </c>
       <c r="B98" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C98" s="13" t="s">
         <v>257</v>
@@ -6823,7 +6823,7 @@
         <v>268</v>
       </c>
       <c r="B99" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C99" s="13" t="s">
         <v>258</v>
@@ -6852,7 +6852,7 @@
         <v>316</v>
       </c>
       <c r="B100" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C100" s="19" t="s">
         <v>249</v>
@@ -6881,7 +6881,7 @@
         <v>270</v>
       </c>
       <c r="B101" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C101" s="13" t="s">
         <v>259</v>
@@ -6910,7 +6910,7 @@
         <v>271</v>
       </c>
       <c r="B102" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C102" s="13" t="s">
         <v>255</v>
@@ -6939,7 +6939,7 @@
         <v>272</v>
       </c>
       <c r="B103" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C103" s="13" t="s">
         <v>260</v>
@@ -6968,7 +6968,7 @@
         <v>273</v>
       </c>
       <c r="B104" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C104" s="13" t="s">
         <v>261</v>
@@ -6997,7 +6997,7 @@
         <v>274</v>
       </c>
       <c r="B105" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C105" s="13" t="s">
         <v>262</v>
@@ -7026,7 +7026,7 @@
         <v>275</v>
       </c>
       <c r="B106" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C106" s="13" t="s">
         <v>256</v>
@@ -7055,7 +7055,7 @@
         <v>276</v>
       </c>
       <c r="B107" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C107" s="13" t="s">
         <v>263</v>
@@ -7090,7 +7090,7 @@
         <v>300</v>
       </c>
       <c r="E108" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G108" s="15" t="s">
         <v>473</v>
@@ -7116,7 +7116,7 @@
         <v>302</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G109" s="15" t="s">
         <v>474</v>
@@ -7133,7 +7133,7 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B110" t="s">
         <v>303</v>
@@ -7142,10 +7142,10 @@
         <v>304</v>
       </c>
       <c r="D110" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E110" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G110" s="16" t="s">
         <v>467</v>
@@ -7158,24 +7158,24 @@
         <v>472</v>
       </c>
       <c r="M110" s="36" t="s">
+        <v>634</v>
+      </c>
+      <c r="N110" s="36" t="s">
         <v>635</v>
       </c>
-      <c r="N110" s="36" t="s">
+      <c r="O110" s="36" t="s">
         <v>636</v>
       </c>
-      <c r="O110" s="36" t="s">
+      <c r="P110" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q110" s="36" t="s">
         <v>637</v>
-      </c>
-      <c r="P110" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q110" s="36" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B111" t="s">
         <v>305</v>
@@ -7184,10 +7184,10 @@
         <v>306</v>
       </c>
       <c r="D111" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E111" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G111" s="16" t="s">
         <v>467</v>
@@ -7200,19 +7200,19 @@
         <v>472</v>
       </c>
       <c r="M111" s="36" t="s">
+        <v>634</v>
+      </c>
+      <c r="N111" s="36" t="s">
         <v>635</v>
       </c>
-      <c r="N111" s="36" t="s">
+      <c r="O111" s="36" t="s">
         <v>636</v>
       </c>
-      <c r="O111" s="36" t="s">
+      <c r="P111" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q111" s="36" t="s">
         <v>637</v>
-      </c>
-      <c r="P111" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q111" s="36" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
@@ -7220,7 +7220,7 @@
         <v>320</v>
       </c>
       <c r="B112" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C112" s="13" t="s">
         <v>327</v>
@@ -7257,7 +7257,7 @@
         <v>321</v>
       </c>
       <c r="B113" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C113" s="13" t="s">
         <v>328</v>
@@ -7294,7 +7294,7 @@
         <v>322</v>
       </c>
       <c r="B114" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C114" s="13" t="s">
         <v>329</v>
@@ -7331,7 +7331,7 @@
         <v>323</v>
       </c>
       <c r="B115" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C115" s="13" t="s">
         <v>330</v>
@@ -7368,7 +7368,7 @@
         <v>324</v>
       </c>
       <c r="B116" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C116" s="13" t="s">
         <v>331</v>
@@ -7405,7 +7405,7 @@
         <v>325</v>
       </c>
       <c r="B117" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C117" s="13" t="s">
         <v>332</v>
@@ -7442,7 +7442,7 @@
         <v>326</v>
       </c>
       <c r="B118" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C118" s="13" t="s">
         <v>333</v>
@@ -7485,34 +7485,34 @@
         <v>512</v>
       </c>
       <c r="D119" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E119" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G119" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J119" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L119" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M119" s="36" t="s">
+        <v>638</v>
+      </c>
+      <c r="N119" s="36" t="s">
         <v>639</v>
       </c>
-      <c r="N119" s="36" t="s">
+      <c r="O119" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P119" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q119" s="36" t="s">
         <v>640</v>
-      </c>
-      <c r="O119" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P119" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q119" s="36" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="120" spans="1:16383" x14ac:dyDescent="0.25">
@@ -7526,34 +7526,34 @@
         <v>512</v>
       </c>
       <c r="D120" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E120" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G120" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J120" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L120" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M120" s="36" t="s">
+        <v>638</v>
+      </c>
+      <c r="N120" s="36" t="s">
         <v>639</v>
       </c>
-      <c r="N120" s="36" t="s">
+      <c r="O120" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P120" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q120" s="36" t="s">
         <v>640</v>
-      </c>
-      <c r="O120" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P120" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q120" s="36" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="121" spans="1:16383" x14ac:dyDescent="0.25">
@@ -7567,34 +7567,34 @@
         <v>512</v>
       </c>
       <c r="D121" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E121" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G121" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J121" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L121" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M121" s="36" t="s">
+        <v>638</v>
+      </c>
+      <c r="N121" s="36" t="s">
         <v>639</v>
       </c>
-      <c r="N121" s="36" t="s">
+      <c r="O121" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P121" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q121" s="36" t="s">
         <v>640</v>
-      </c>
-      <c r="O121" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P121" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q121" s="36" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="122" spans="1:16383" x14ac:dyDescent="0.25">
@@ -7608,34 +7608,34 @@
         <v>512</v>
       </c>
       <c r="D122" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E122" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G122" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J122" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L122" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M122" s="36" t="s">
+        <v>638</v>
+      </c>
+      <c r="N122" s="36" t="s">
         <v>639</v>
       </c>
-      <c r="N122" s="36" t="s">
+      <c r="O122" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P122" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q122" s="36" t="s">
         <v>640</v>
-      </c>
-      <c r="O122" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P122" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q122" s="36" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="123" spans="1:16383" x14ac:dyDescent="0.25">
@@ -7649,34 +7649,34 @@
         <v>512</v>
       </c>
       <c r="D123" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E123" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G123" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J123" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L123" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M123" s="36" t="s">
+        <v>638</v>
+      </c>
+      <c r="N123" s="36" t="s">
         <v>639</v>
       </c>
-      <c r="N123" s="36" t="s">
+      <c r="O123" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P123" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q123" s="36" t="s">
         <v>640</v>
-      </c>
-      <c r="O123" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P123" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q123" s="36" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="124" spans="1:16383" x14ac:dyDescent="0.25">
@@ -7690,34 +7690,34 @@
         <v>514</v>
       </c>
       <c r="D124" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E124" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G124" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J124" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L124" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M124" s="36" t="s">
+        <v>638</v>
+      </c>
+      <c r="N124" s="36" t="s">
         <v>639</v>
       </c>
-      <c r="N124" s="36" t="s">
+      <c r="O124" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P124" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q124" s="36" t="s">
         <v>640</v>
-      </c>
-      <c r="O124" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P124" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q124" s="36" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="125" spans="1:16383" x14ac:dyDescent="0.25">
@@ -7731,55 +7731,55 @@
         <v>514</v>
       </c>
       <c r="D125" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E125" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G125" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J125" s="13" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L125" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M125" s="36" t="s">
+        <v>638</v>
+      </c>
+      <c r="N125" s="36" t="s">
         <v>639</v>
       </c>
-      <c r="N125" s="36" t="s">
+      <c r="O125" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P125" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q125" s="36" t="s">
         <v>640</v>
-      </c>
-      <c r="O125" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P125" s="36" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q125" s="36" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="126" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A126" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="B126" t="s">
         <v>523</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" s="29" t="s">
         <v>524</v>
       </c>
-      <c r="C126" s="29" t="s">
-        <v>525</v>
-      </c>
       <c r="D126" s="36" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E126" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F126"/>
       <c r="G126" s="29" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H126"/>
       <c r="I126"/>
@@ -7789,19 +7789,19 @@
         <v>342</v>
       </c>
       <c r="M126" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="N126" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="O126" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P126" s="36" t="s">
         <v>631</v>
       </c>
-      <c r="N126" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="O126" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P126" s="36" t="s">
-        <v>632</v>
-      </c>
       <c r="Q126" s="36" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="R126"/>
       <c r="S126"/>
@@ -24172,23 +24172,23 @@
     </row>
     <row r="127" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A127" s="28" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B127" t="s">
+        <v>525</v>
+      </c>
+      <c r="C127" s="29" t="s">
         <v>526</v>
       </c>
-      <c r="C127" s="29" t="s">
-        <v>527</v>
-      </c>
       <c r="D127" s="36" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E127" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F127"/>
       <c r="G127" s="29" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H127"/>
       <c r="I127"/>
@@ -24198,19 +24198,19 @@
         <v>342</v>
       </c>
       <c r="M127" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="N127" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="O127" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P127" s="36" t="s">
         <v>631</v>
       </c>
-      <c r="N127" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="O127" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P127" s="36" t="s">
-        <v>632</v>
-      </c>
       <c r="Q127" s="36" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="R127"/>
       <c r="S127"/>
@@ -40581,23 +40581,23 @@
     </row>
     <row r="128" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A128" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="B128" t="s">
         <v>528</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" s="29" t="s">
         <v>529</v>
       </c>
-      <c r="C128" s="29" t="s">
-        <v>530</v>
-      </c>
       <c r="D128" s="36" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E128" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F128"/>
       <c r="G128" s="29" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="H128"/>
       <c r="I128"/>
@@ -40607,19 +40607,19 @@
         <v>342</v>
       </c>
       <c r="M128" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="N128" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="O128" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P128" s="36" t="s">
         <v>631</v>
       </c>
-      <c r="N128" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="O128" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P128" s="36" t="s">
-        <v>632</v>
-      </c>
       <c r="Q128" s="36" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R128"/>
       <c r="S128"/>
@@ -56990,23 +56990,23 @@
     </row>
     <row r="129" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A129" s="28" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B129" t="s">
+        <v>531</v>
+      </c>
+      <c r="C129" s="29" t="s">
         <v>532</v>
       </c>
-      <c r="C129" s="29" t="s">
-        <v>533</v>
-      </c>
       <c r="D129" s="36" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E129" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F129"/>
       <c r="G129" s="29" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="H129"/>
       <c r="I129"/>
@@ -57016,19 +57016,19 @@
         <v>342</v>
       </c>
       <c r="M129" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="N129" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="O129" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="P129" s="36" t="s">
         <v>631</v>
       </c>
-      <c r="N129" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="O129" s="36" t="s">
-        <v>631</v>
-      </c>
-      <c r="P129" s="36" t="s">
-        <v>632</v>
-      </c>
       <c r="Q129" s="36" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R129"/>
       <c r="S129"/>
@@ -73399,78 +73399,78 @@
     </row>
     <row r="130" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A130" s="28" t="s">
+        <v>533</v>
+      </c>
+      <c r="B130" t="s">
         <v>534</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" s="29" t="s">
         <v>535</v>
       </c>
-      <c r="C130" s="29" t="s">
-        <v>536</v>
-      </c>
       <c r="D130" s="36" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E130" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G130" s="30" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L130" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M130" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="N130" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="O130" s="15" t="s">
+        <v>632</v>
+      </c>
+      <c r="P130" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="P130" s="15" t="s">
-        <v>634</v>
-      </c>
       <c r="Q130" s="15" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="131" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A131" s="28" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B131" t="s">
+        <v>536</v>
+      </c>
+      <c r="C131" s="29" t="s">
         <v>537</v>
       </c>
-      <c r="C131" s="29" t="s">
-        <v>538</v>
-      </c>
       <c r="D131" s="36" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E131" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G131" s="30" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L131" s="13" t="s">
         <v>342</v>
       </c>
       <c r="M131" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="N131" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="O131" s="15" t="s">
+        <v>632</v>
+      </c>
+      <c r="P131" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="P131" s="15" t="s">
-        <v>634</v>
-      </c>
       <c r="Q131" s="15" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
codelist updated for dry weight
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martskol/ownCloud/Projects/MoCiS2/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MFO_Privat\MG\MOCIS\SGU\SGU_marina21\ny_codlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D685ED2-3ACD-A34D-9344-9F9311D1FC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39960" yWindow="2600" windowWidth="29040" windowHeight="15840" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39960" yWindow="3045" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
     <sheet name="ARTER" sheetId="15" r:id="rId2"/>
     <sheet name="PARAMETRAR" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="671">
   <si>
     <t>PERC</t>
   </si>
@@ -2042,12 +2041,15 @@
   </si>
   <si>
     <t>ORES</t>
+  </si>
+  <si>
+    <t>SS_EN_ISO_16720-2007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2232,19 +2234,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Bra" xfId="4" builtinId="26"/>
-    <cellStyle name="Dålig" xfId="1" builtinId="27"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 2 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 3 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 3 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 4" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 6" xfId="3" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 7" xfId="5" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="XLConnect.String 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 2" xfId="6"/>
+    <cellStyle name="Normal 2 2" xfId="12"/>
+    <cellStyle name="Normal 2 4" xfId="10"/>
+    <cellStyle name="Normal 3 2" xfId="7"/>
+    <cellStyle name="Normal 3 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="8"/>
+    <cellStyle name="Normal 5" xfId="9"/>
+    <cellStyle name="Normal 6" xfId="3"/>
+    <cellStyle name="Normal 7" xfId="5"/>
+    <cellStyle name="XLConnect.String 2" xfId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2521,20 +2523,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.1640625" style="16" customWidth="1"/>
-    <col min="3" max="4" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="16" customWidth="1"/>
+    <col min="3" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -2548,7 +2550,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -2562,7 +2564,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -2576,7 +2578,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>98</v>
       </c>
@@ -2590,7 +2592,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>100</v>
       </c>
@@ -2604,7 +2606,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>100</v>
       </c>
@@ -2618,7 +2620,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
@@ -2632,7 +2634,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>102</v>
       </c>
@@ -2646,7 +2648,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
@@ -2660,7 +2662,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>102</v>
       </c>
@@ -2674,7 +2676,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>104</v>
       </c>
@@ -2688,7 +2690,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>104</v>
       </c>
@@ -2702,7 +2704,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -2716,7 +2718,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>106</v>
       </c>
@@ -2730,7 +2732,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>109</v>
       </c>
@@ -2744,7 +2746,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>112</v>
       </c>
@@ -2758,7 +2760,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>115</v>
       </c>
@@ -2772,7 +2774,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>118</v>
       </c>
@@ -2786,7 +2788,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>121</v>
       </c>
@@ -2800,7 +2802,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>121</v>
       </c>
@@ -2814,7 +2816,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>121</v>
       </c>
@@ -2828,7 +2830,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>124</v>
       </c>
@@ -2842,7 +2844,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
@@ -2856,7 +2858,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>130</v>
       </c>
@@ -2870,7 +2872,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>133</v>
       </c>
@@ -2884,7 +2886,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>136</v>
       </c>
@@ -2898,7 +2900,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>139</v>
       </c>
@@ -2912,7 +2914,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>142</v>
       </c>
@@ -2926,7 +2928,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>145</v>
       </c>
@@ -2940,7 +2942,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>148</v>
       </c>
@@ -2954,7 +2956,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>151</v>
       </c>
@@ -2968,7 +2970,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>318</v>
       </c>
@@ -2982,7 +2984,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>154</v>
       </c>
@@ -2996,7 +2998,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>127</v>
       </c>
@@ -3010,7 +3012,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>157</v>
       </c>
@@ -3024,7 +3026,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>319</v>
       </c>
@@ -3038,7 +3040,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>157</v>
       </c>
@@ -3052,7 +3054,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>166</v>
       </c>
@@ -3066,7 +3068,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>166</v>
       </c>
@@ -3080,7 +3082,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>160</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>160</v>
       </c>
@@ -3108,7 +3110,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>115</v>
       </c>
@@ -3122,7 +3124,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>163</v>
       </c>
@@ -3136,7 +3138,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>166</v>
       </c>
@@ -3150,7 +3152,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>157</v>
       </c>
@@ -3164,7 +3166,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>169</v>
       </c>
@@ -3178,7 +3180,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>171</v>
       </c>
@@ -3192,7 +3194,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>358</v>
       </c>
@@ -3206,7 +3208,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>455</v>
       </c>
@@ -3220,7 +3222,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>365</v>
       </c>
@@ -3234,7 +3236,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>368</v>
       </c>
@@ -3248,7 +3250,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>371</v>
       </c>
@@ -3262,7 +3264,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>374</v>
       </c>
@@ -3276,7 +3278,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>377</v>
       </c>
@@ -3290,7 +3292,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>380</v>
       </c>
@@ -3304,7 +3306,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>383</v>
       </c>
@@ -3318,7 +3320,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>386</v>
       </c>
@@ -3332,7 +3334,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>389</v>
       </c>
@@ -3346,7 +3348,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>392</v>
       </c>
@@ -3360,7 +3362,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>395</v>
       </c>
@@ -3374,7 +3376,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>398</v>
       </c>
@@ -3388,7 +3390,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>401</v>
       </c>
@@ -3402,7 +3404,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>404</v>
       </c>
@@ -3416,7 +3418,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>407</v>
       </c>
@@ -3430,7 +3432,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>407</v>
       </c>
@@ -3444,7 +3446,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>410</v>
       </c>
@@ -3458,7 +3460,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>413</v>
       </c>
@@ -3472,7 +3474,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>416</v>
       </c>
@@ -3486,7 +3488,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>419</v>
       </c>
@@ -3500,7 +3502,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>422</v>
       </c>
@@ -3514,7 +3516,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>425</v>
       </c>
@@ -3528,7 +3530,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>428</v>
       </c>
@@ -3542,7 +3544,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>431</v>
       </c>
@@ -3556,7 +3558,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>434</v>
       </c>
@@ -3570,7 +3572,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>437</v>
       </c>
@@ -3584,7 +3586,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>440</v>
       </c>
@@ -3598,7 +3600,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>443</v>
       </c>
@@ -3612,7 +3614,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>446</v>
       </c>
@@ -3626,7 +3628,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>449</v>
       </c>
@@ -3640,7 +3642,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>452</v>
       </c>
@@ -3654,7 +3656,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
         <v>660</v>
       </c>
@@ -3668,7 +3670,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
         <v>663</v>
       </c>
@@ -3682,7 +3684,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
         <v>666</v>
       </c>
@@ -3696,7 +3698,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
         <v>669</v>
       </c>
@@ -3717,19 +3719,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -3743,7 +3745,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3757,7 +3759,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3771,7 +3773,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3785,7 +3787,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>309</v>
       </c>
@@ -3799,7 +3801,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>310</v>
       </c>
@@ -3813,7 +3815,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3827,7 +3829,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3841,7 +3843,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3855,7 +3857,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3869,7 +3871,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3883,7 +3885,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>620</v>
       </c>
@@ -3897,7 +3899,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>655</v>
       </c>
@@ -3911,7 +3913,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>656</v>
       </c>
@@ -3925,7 +3927,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>657</v>
       </c>
@@ -3946,37 +3948,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F135" sqref="F135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>501</v>
       </c>
@@ -4029,7 +4033,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>334</v>
       </c>
@@ -4058,7 +4062,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4087,7 +4091,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4116,7 +4120,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -4145,7 +4149,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -4174,7 +4178,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -4203,7 +4207,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -4232,7 +4236,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
@@ -4261,7 +4265,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>546</v>
       </c>
@@ -4290,7 +4294,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -4319,7 +4323,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -4348,7 +4352,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>264</v>
       </c>
@@ -4377,7 +4381,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -4406,7 +4410,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>518</v>
       </c>
@@ -4435,7 +4439,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>548</v>
       </c>
@@ -4464,7 +4468,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -4493,7 +4497,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>552</v>
       </c>
@@ -4522,7 +4526,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -4551,7 +4555,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>549</v>
       </c>
@@ -4580,7 +4584,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -4609,7 +4613,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>551</v>
       </c>
@@ -4638,7 +4642,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -4667,7 +4671,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>547</v>
       </c>
@@ -4696,7 +4700,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -4725,7 +4729,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>456</v>
       </c>
@@ -4754,7 +4758,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -4783,7 +4787,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -4812,7 +4816,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>550</v>
       </c>
@@ -4841,7 +4845,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -4870,7 +4874,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>459</v>
       </c>
@@ -4899,7 +4903,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>460</v>
       </c>
@@ -4928,7 +4932,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -4957,7 +4961,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -4986,7 +4990,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -5015,7 +5019,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>461</v>
       </c>
@@ -5044,7 +5048,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>462</v>
       </c>
@@ -5073,7 +5077,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>463</v>
       </c>
@@ -5102,7 +5106,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>464</v>
       </c>
@@ -5131,7 +5135,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>465</v>
       </c>
@@ -5160,7 +5164,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>350</v>
       </c>
@@ -5189,7 +5193,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>351</v>
       </c>
@@ -5218,7 +5222,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>517</v>
       </c>
@@ -5247,7 +5251,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>466</v>
       </c>
@@ -5276,7 +5280,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>516</v>
       </c>
@@ -5305,7 +5309,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>352</v>
       </c>
@@ -5334,7 +5338,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>353</v>
       </c>
@@ -5363,7 +5367,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>354</v>
       </c>
@@ -5392,7 +5396,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>355</v>
       </c>
@@ -5421,7 +5425,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -5450,7 +5454,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>176</v>
       </c>
@@ -5479,7 +5483,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>178</v>
       </c>
@@ -5508,7 +5512,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>180</v>
       </c>
@@ -5537,7 +5541,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>182</v>
       </c>
@@ -5566,7 +5570,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>184</v>
       </c>
@@ -5595,7 +5599,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>186</v>
       </c>
@@ -5624,7 +5628,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>188</v>
       </c>
@@ -5653,7 +5657,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -5682,7 +5686,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>192</v>
       </c>
@@ -5711,7 +5715,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>194</v>
       </c>
@@ -5740,7 +5744,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>196</v>
       </c>
@@ -5769,7 +5773,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>198</v>
       </c>
@@ -5798,7 +5802,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>200</v>
       </c>
@@ -5827,7 +5831,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>202</v>
       </c>
@@ -5856,7 +5860,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>204</v>
       </c>
@@ -5885,7 +5889,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>206</v>
       </c>
@@ -5914,7 +5918,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>294</v>
       </c>
@@ -5943,7 +5947,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>293</v>
       </c>
@@ -5972,7 +5976,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>292</v>
       </c>
@@ -6001,7 +6005,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>291</v>
       </c>
@@ -6030,7 +6034,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>290</v>
       </c>
@@ -6059,7 +6063,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>289</v>
       </c>
@@ -6088,7 +6092,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>288</v>
       </c>
@@ -6117,7 +6121,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>287</v>
       </c>
@@ -6146,7 +6150,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>286</v>
       </c>
@@ -6175,7 +6179,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>284</v>
       </c>
@@ -6204,7 +6208,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>285</v>
       </c>
@@ -6233,7 +6237,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>295</v>
       </c>
@@ -6262,7 +6266,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>298</v>
       </c>
@@ -6291,7 +6295,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>297</v>
       </c>
@@ -6320,7 +6324,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>296</v>
       </c>
@@ -6349,7 +6353,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>313</v>
       </c>
@@ -6386,7 +6390,7 @@
       <c r="P82" s="7"/>
       <c r="Q82" s="7"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
         <v>314</v>
       </c>
@@ -6423,7 +6427,7 @@
       <c r="P83" s="7"/>
       <c r="Q83" s="7"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
         <v>315</v>
       </c>
@@ -6460,7 +6464,7 @@
       <c r="P84" s="7"/>
       <c r="Q84" s="7"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
         <v>515</v>
       </c>
@@ -6497,7 +6501,7 @@
       <c r="P85" s="7"/>
       <c r="Q85" s="7"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
         <v>277</v>
       </c>
@@ -6534,7 +6538,7 @@
       <c r="P86" s="7"/>
       <c r="Q86" s="7"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
         <v>278</v>
       </c>
@@ -6571,7 +6575,7 @@
       <c r="P87" s="7"/>
       <c r="Q87" s="7"/>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
         <v>279</v>
       </c>
@@ -6608,7 +6612,7 @@
       <c r="P88" s="7"/>
       <c r="Q88" s="7"/>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
         <v>280</v>
       </c>
@@ -6645,7 +6649,7 @@
       <c r="P89" s="7"/>
       <c r="Q89" s="7"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
         <v>281</v>
       </c>
@@ -6682,7 +6686,7 @@
       <c r="P90" s="7"/>
       <c r="Q90" s="7"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
         <v>283</v>
       </c>
@@ -6719,7 +6723,7 @@
       <c r="P91" s="7"/>
       <c r="Q91" s="7"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
         <v>269</v>
       </c>
@@ -6756,7 +6760,7 @@
       <c r="P92" s="7"/>
       <c r="Q92" s="7"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
         <v>311</v>
       </c>
@@ -6793,7 +6797,7 @@
       <c r="P93" s="7"/>
       <c r="Q93" s="7"/>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
         <v>312</v>
       </c>
@@ -6830,7 +6834,7 @@
       <c r="P94" s="7"/>
       <c r="Q94" s="7"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
         <v>282</v>
       </c>
@@ -6867,7 +6871,7 @@
       <c r="P95" s="7"/>
       <c r="Q95" s="7"/>
     </row>
-    <row r="96" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
         <v>265</v>
       </c>
@@ -6896,7 +6900,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>266</v>
       </c>
@@ -6925,7 +6929,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>267</v>
       </c>
@@ -6954,7 +6958,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>268</v>
       </c>
@@ -6983,7 +6987,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>316</v>
       </c>
@@ -7012,7 +7016,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>270</v>
       </c>
@@ -7041,7 +7045,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
         <v>271</v>
       </c>
@@ -7070,7 +7074,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>272</v>
       </c>
@@ -7099,7 +7103,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>273</v>
       </c>
@@ -7128,7 +7132,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
         <v>274</v>
       </c>
@@ -7157,7 +7161,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
         <v>275</v>
       </c>
@@ -7186,7 +7190,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>276</v>
       </c>
@@ -7215,7 +7219,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>308</v>
       </c>
@@ -7241,7 +7245,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>307</v>
       </c>
@@ -7267,7 +7271,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>541</v>
       </c>
@@ -7309,7 +7313,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>542</v>
       </c>
@@ -7351,7 +7355,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>320</v>
       </c>
@@ -7388,7 +7392,7 @@
       <c r="P112" s="7"/>
       <c r="Q112" s="7"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>321</v>
       </c>
@@ -7425,7 +7429,7 @@
       <c r="P113" s="7"/>
       <c r="Q113" s="7"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>322</v>
       </c>
@@ -7462,7 +7466,7 @@
       <c r="P114" s="7"/>
       <c r="Q114" s="7"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>323</v>
       </c>
@@ -7499,7 +7503,7 @@
       <c r="P115" s="7"/>
       <c r="Q115" s="7"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>324</v>
       </c>
@@ -7536,7 +7540,7 @@
       <c r="P116" s="7"/>
       <c r="Q116" s="7"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>325</v>
       </c>
@@ -7573,7 +7577,7 @@
       <c r="P117" s="7"/>
       <c r="Q117" s="7"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>326</v>
       </c>
@@ -7610,7 +7614,7 @@
       <c r="P118" s="7"/>
       <c r="Q118" s="7"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>504</v>
       </c>
@@ -7636,13 +7640,13 @@
         <v>342</v>
       </c>
       <c r="M119" t="s">
-        <v>638</v>
+        <v>670</v>
       </c>
       <c r="N119" t="s">
         <v>639</v>
       </c>
       <c r="O119" t="s">
-        <v>630</v>
+        <v>670</v>
       </c>
       <c r="P119" t="s">
         <v>633</v>
@@ -7651,7 +7655,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>505</v>
       </c>
@@ -7677,13 +7681,13 @@
         <v>342</v>
       </c>
       <c r="M120" t="s">
-        <v>638</v>
+        <v>670</v>
       </c>
       <c r="N120" t="s">
         <v>639</v>
       </c>
       <c r="O120" t="s">
-        <v>630</v>
+        <v>670</v>
       </c>
       <c r="P120" t="s">
         <v>633</v>
@@ -7692,7 +7696,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>506</v>
       </c>
@@ -7718,13 +7722,13 @@
         <v>342</v>
       </c>
       <c r="M121" t="s">
-        <v>638</v>
+        <v>670</v>
       </c>
       <c r="N121" t="s">
         <v>639</v>
       </c>
       <c r="O121" t="s">
-        <v>630</v>
+        <v>670</v>
       </c>
       <c r="P121" t="s">
         <v>633</v>
@@ -7733,7 +7737,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>507</v>
       </c>
@@ -7759,13 +7763,13 @@
         <v>342</v>
       </c>
       <c r="M122" t="s">
-        <v>638</v>
+        <v>670</v>
       </c>
       <c r="N122" t="s">
         <v>639</v>
       </c>
       <c r="O122" t="s">
-        <v>630</v>
+        <v>670</v>
       </c>
       <c r="P122" t="s">
         <v>633</v>
@@ -7774,7 +7778,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>511</v>
       </c>
@@ -7800,13 +7804,13 @@
         <v>342</v>
       </c>
       <c r="M123" t="s">
-        <v>638</v>
+        <v>670</v>
       </c>
       <c r="N123" t="s">
         <v>639</v>
       </c>
       <c r="O123" t="s">
-        <v>630</v>
+        <v>670</v>
       </c>
       <c r="P123" t="s">
         <v>633</v>
@@ -7815,7 +7819,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>508</v>
       </c>
@@ -7856,7 +7860,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>509</v>
       </c>
@@ -7897,7 +7901,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>522</v>
       </c>
@@ -7935,7 +7939,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>539</v>
       </c>
@@ -7973,7 +7977,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>527</v>
       </c>
@@ -8011,7 +8015,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>540</v>
       </c>
@@ -8049,7 +8053,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>533</v>
       </c>
@@ -8087,7 +8091,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>538</v>
       </c>

</xml_diff>

<commit_message>
codlist PROV_BERED Umeå fat% corrected
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39960" yWindow="3045" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
+    <workbookView xWindow="39960" yWindow="3495" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="672">
   <si>
     <t>PERC</t>
   </si>
@@ -2044,6 +2044,9 @@
   </si>
   <si>
     <t>SS_EN_ISO_16720-2007</t>
+  </si>
+  <si>
+    <t>ACHEXHEXE</t>
   </si>
 </sst>
 </file>
@@ -3954,9 +3957,9 @@
   </sheetPr>
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F135" sqref="F135"/>
+      <selection pane="bottomLeft" activeCell="M126" sqref="M126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7886,7 +7889,7 @@
         <v>342</v>
       </c>
       <c r="M125" t="s">
-        <v>638</v>
+        <v>671</v>
       </c>
       <c r="N125" t="s">
         <v>639</v>

</xml_diff>

<commit_message>
Additional name for Utlängan for reading rawdata files
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MFO_Privat\MG\MOCIS\SGU\SGU_marina21\ny_codlist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annesore\Dropbox\SU_170821\Programmering\R\HARSAT\MoCiS2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39960" yWindow="3495" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2"/>
+    <workbookView xWindow="39960" yWindow="3945" windowWidth="29040" windowHeight="15840" tabRatio="877"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="672">
   <si>
     <t>PERC</t>
   </si>
@@ -2527,10 +2527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3713,6 +3713,20 @@
       </c>
       <c r="D84" s="21" t="s">
         <v>668</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3957,7 +3971,7 @@
   </sheetPr>
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M126" sqref="M126"/>
     </sheetView>

</xml_diff>

<commit_message>
Adding new PFAS codelist
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\NA\MAF\MAF_Privat\Miljogifter\mg_analys\SGU\Data SGU\MoCiS2_github_clone\MoCiS2\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\NA\MAF\MAF_Privat\Miljogifter\mg_analys\SGU\Mocis2_temp\MoCiS2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7CAC84-62B2-4A3F-955D-0702E152DC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8848E9BF-040B-4B87-B750-CD92AE9E1CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="1455" windowWidth="26505" windowHeight="16560" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="60" windowWidth="23475" windowHeight="15210" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -28,12 +28,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="732">
   <si>
     <t>PERC</t>
   </si>
@@ -2139,6 +2142,96 @@
   </si>
   <si>
     <t>CH07/118</t>
+  </si>
+  <si>
+    <t>HFPO-DA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NADONA </t>
+  </si>
+  <si>
+    <t>PFPRS</t>
+  </si>
+  <si>
+    <t>PFUNDS</t>
+  </si>
+  <si>
+    <t>PFDODS</t>
+  </si>
+  <si>
+    <t>PFTRDS</t>
+  </si>
+  <si>
+    <t>FBSA</t>
+  </si>
+  <si>
+    <t>FHXSA</t>
+  </si>
+  <si>
+    <t>PFODA</t>
+  </si>
+  <si>
+    <t>PFHXDA</t>
+  </si>
+  <si>
+    <t>2,3,3,3-Tetrafluor-2-(1,1,2,2,3,3,3-heptafluorpropoxy)propansyra</t>
+  </si>
+  <si>
+    <t>Dodekafluor-3H-4,8-dioxanonansyra</t>
+  </si>
+  <si>
+    <t>Perfluorpropansulfonsyra (PFPrS)</t>
+  </si>
+  <si>
+    <t>Perfluorundekansulfonsyra (PFUnDS), linjär</t>
+  </si>
+  <si>
+    <t>Perfluordodekansulfonsyra (PFDoDS), linjär</t>
+  </si>
+  <si>
+    <t>Perfluortridekansulfonsyra (PFTriDS), linjär</t>
+  </si>
+  <si>
+    <t>Perfluorbutansulfonamid (FBSA), linjär</t>
+  </si>
+  <si>
+    <t>Perfluorhexansulfonamid (FHxSA), linjär</t>
+  </si>
+  <si>
+    <t>Perfluoroktadekansyra (PFOcDA), linjär</t>
+  </si>
+  <si>
+    <t>Perfluorhexadekansyra (PFHxDA), linjär</t>
+  </si>
+  <si>
+    <t>CH07/813</t>
+  </si>
+  <si>
+    <t>CH07/814</t>
+  </si>
+  <si>
+    <t>CH07/931</t>
+  </si>
+  <si>
+    <t>CH07/808</t>
+  </si>
+  <si>
+    <t>CH07/774</t>
+  </si>
+  <si>
+    <t>CH07/890</t>
+  </si>
+  <si>
+    <t>CH07/970</t>
+  </si>
+  <si>
+    <t>CH07/971</t>
+  </si>
+  <si>
+    <t>CH07/562</t>
+  </si>
+  <si>
+    <t>CH07/558</t>
   </si>
 </sst>
 </file>
@@ -2250,12 +2343,23 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -2276,7 +2380,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2328,6 +2432,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -4202,11 +4307,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Q131"/>
+  <dimension ref="A1:Q141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A94" sqref="A94"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5677,28 +5782,28 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>702</v>
       </c>
       <c r="B50" t="s">
-        <v>571</v>
+        <v>712</v>
       </c>
       <c r="C50" t="s">
-        <v>175</v>
+        <v>722</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L50" s="7" t="s">
         <v>348</v>
@@ -5706,28 +5811,28 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>176</v>
+        <v>703</v>
       </c>
       <c r="B51" t="s">
-        <v>572</v>
+        <v>713</v>
       </c>
       <c r="C51" t="s">
-        <v>177</v>
+        <v>723</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L51" s="7" t="s">
         <v>348</v>
@@ -5735,28 +5840,28 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>178</v>
+        <v>704</v>
       </c>
       <c r="B52" t="s">
-        <v>573</v>
+        <v>714</v>
       </c>
       <c r="C52" t="s">
-        <v>179</v>
+        <v>724</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L52" s="7" t="s">
         <v>348</v>
@@ -5764,28 +5869,28 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>180</v>
+        <v>705</v>
       </c>
       <c r="B53" t="s">
-        <v>574</v>
+        <v>715</v>
       </c>
       <c r="C53" t="s">
-        <v>181</v>
+        <v>725</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L53" s="7" t="s">
         <v>348</v>
@@ -5793,28 +5898,28 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>182</v>
+        <v>706</v>
       </c>
       <c r="B54" t="s">
-        <v>575</v>
+        <v>716</v>
       </c>
       <c r="C54" t="s">
-        <v>183</v>
+        <v>726</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L54" s="7" t="s">
         <v>348</v>
@@ -5822,28 +5927,28 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>184</v>
+        <v>707</v>
       </c>
       <c r="B55" t="s">
-        <v>576</v>
+        <v>717</v>
       </c>
       <c r="C55" t="s">
-        <v>185</v>
+        <v>727</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K55" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L55" s="7" t="s">
         <v>348</v>
@@ -5851,28 +5956,28 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>708</v>
       </c>
       <c r="B56" t="s">
-        <v>577</v>
+        <v>718</v>
       </c>
       <c r="C56" t="s">
-        <v>187</v>
+        <v>728</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L56" s="7" t="s">
         <v>348</v>
@@ -5880,28 +5985,28 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>188</v>
+        <v>709</v>
       </c>
       <c r="B57" t="s">
-        <v>578</v>
+        <v>719</v>
       </c>
       <c r="C57" t="s">
-        <v>189</v>
+        <v>729</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K57" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L57" s="7" t="s">
         <v>348</v>
@@ -5909,28 +6014,28 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>190</v>
-      </c>
-      <c r="B58" t="s">
-        <v>579</v>
-      </c>
-      <c r="C58" t="s">
-        <v>191</v>
+        <v>710</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>730</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K58" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L58" s="7" t="s">
         <v>348</v>
@@ -5938,28 +6043,28 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>192</v>
-      </c>
-      <c r="B59" t="s">
-        <v>580</v>
-      </c>
-      <c r="C59" t="s">
-        <v>193</v>
+        <v>711</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="C59" s="23" t="s">
+        <v>731</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L59" s="7" t="s">
         <v>348</v>
@@ -5967,13 +6072,13 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B60" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="C60" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="G60" s="7" t="s">
         <v>469</v>
@@ -5996,13 +6101,13 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>582</v>
+        <v>572</v>
       </c>
       <c r="C61" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>469</v>
@@ -6025,13 +6130,13 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
-        <v>583</v>
+        <v>573</v>
       </c>
       <c r="C62" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>469</v>
@@ -6054,13 +6159,13 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B63" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="C63" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>469</v>
@@ -6083,13 +6188,13 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B64" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="C64" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>469</v>
@@ -6112,13 +6217,13 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B65" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="C65" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>469</v>
@@ -6141,318 +6246,318 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" t="s">
+        <v>577</v>
+      </c>
+      <c r="C66" t="s">
+        <v>187</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J66" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K66" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L66" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>188</v>
+      </c>
+      <c r="B67" t="s">
+        <v>578</v>
+      </c>
+      <c r="C67" t="s">
+        <v>189</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K67" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L67" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" t="s">
+        <v>579</v>
+      </c>
+      <c r="C68" t="s">
+        <v>191</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H68" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J68" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K68" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L68" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>192</v>
+      </c>
+      <c r="B69" t="s">
+        <v>580</v>
+      </c>
+      <c r="C69" t="s">
+        <v>193</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J69" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K69" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L69" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>194</v>
+      </c>
+      <c r="B70" t="s">
+        <v>581</v>
+      </c>
+      <c r="C70" t="s">
+        <v>195</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J70" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K70" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L70" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>196</v>
+      </c>
+      <c r="B71" t="s">
+        <v>582</v>
+      </c>
+      <c r="C71" t="s">
+        <v>197</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K71" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L71" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>198</v>
+      </c>
+      <c r="B72" t="s">
+        <v>583</v>
+      </c>
+      <c r="C72" t="s">
+        <v>199</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K72" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L72" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>200</v>
+      </c>
+      <c r="B73" t="s">
+        <v>584</v>
+      </c>
+      <c r="C73" t="s">
+        <v>201</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J73" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K73" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L73" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>202</v>
+      </c>
+      <c r="B74" t="s">
+        <v>585</v>
+      </c>
+      <c r="C74" t="s">
+        <v>203</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L74" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>204</v>
+      </c>
+      <c r="B75" t="s">
+        <v>586</v>
+      </c>
+      <c r="C75" t="s">
+        <v>205</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>206</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B76" t="s">
         <v>587</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C76" t="s">
         <v>207</v>
       </c>
-      <c r="G66" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="I66" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="J66" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="K66" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="L66" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B67" t="s">
-        <v>208</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="G67" t="s">
-        <v>470</v>
-      </c>
-      <c r="H67" t="s">
-        <v>470</v>
-      </c>
-      <c r="I67" t="s">
-        <v>470</v>
-      </c>
-      <c r="J67" t="s">
-        <v>470</v>
-      </c>
-      <c r="K67" t="s">
-        <v>470</v>
-      </c>
-      <c r="L67" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="B68" t="s">
-        <v>210</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G68" t="s">
-        <v>470</v>
-      </c>
-      <c r="H68" t="s">
-        <v>470</v>
-      </c>
-      <c r="I68" t="s">
-        <v>470</v>
-      </c>
-      <c r="J68" t="s">
-        <v>470</v>
-      </c>
-      <c r="K68" t="s">
-        <v>470</v>
-      </c>
-      <c r="L68" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="B69" t="s">
-        <v>212</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="G69" t="s">
-        <v>470</v>
-      </c>
-      <c r="H69" t="s">
-        <v>470</v>
-      </c>
-      <c r="I69" t="s">
-        <v>470</v>
-      </c>
-      <c r="J69" t="s">
-        <v>470</v>
-      </c>
-      <c r="K69" t="s">
-        <v>470</v>
-      </c>
-      <c r="L69" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="B70" t="s">
-        <v>214</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="G70" t="s">
-        <v>470</v>
-      </c>
-      <c r="H70" t="s">
-        <v>470</v>
-      </c>
-      <c r="I70" t="s">
-        <v>470</v>
-      </c>
-      <c r="J70" t="s">
-        <v>470</v>
-      </c>
-      <c r="K70" t="s">
-        <v>470</v>
-      </c>
-      <c r="L70" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B71" t="s">
-        <v>216</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="G71" t="s">
-        <v>470</v>
-      </c>
-      <c r="H71" t="s">
-        <v>470</v>
-      </c>
-      <c r="I71" t="s">
-        <v>470</v>
-      </c>
-      <c r="J71" t="s">
-        <v>470</v>
-      </c>
-      <c r="K71" t="s">
-        <v>470</v>
-      </c>
-      <c r="L71" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="B72" t="s">
-        <v>218</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="G72" t="s">
-        <v>470</v>
-      </c>
-      <c r="H72" t="s">
-        <v>470</v>
-      </c>
-      <c r="I72" t="s">
-        <v>470</v>
-      </c>
-      <c r="J72" t="s">
-        <v>470</v>
-      </c>
-      <c r="K72" t="s">
-        <v>470</v>
-      </c>
-      <c r="L72" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B73" t="s">
-        <v>220</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="G73" t="s">
-        <v>470</v>
-      </c>
-      <c r="H73" t="s">
-        <v>470</v>
-      </c>
-      <c r="I73" t="s">
-        <v>470</v>
-      </c>
-      <c r="J73" t="s">
-        <v>470</v>
-      </c>
-      <c r="K73" t="s">
-        <v>470</v>
-      </c>
-      <c r="L73" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B74" t="s">
-        <v>222</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="G74" t="s">
-        <v>470</v>
-      </c>
-      <c r="H74" t="s">
-        <v>470</v>
-      </c>
-      <c r="I74" t="s">
-        <v>470</v>
-      </c>
-      <c r="J74" t="s">
-        <v>470</v>
-      </c>
-      <c r="K74" t="s">
-        <v>470</v>
-      </c>
-      <c r="L74" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B75" t="s">
-        <v>224</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="G75" t="s">
-        <v>470</v>
-      </c>
-      <c r="H75" t="s">
-        <v>470</v>
-      </c>
-      <c r="I75" t="s">
-        <v>470</v>
-      </c>
-      <c r="J75" t="s">
-        <v>470</v>
-      </c>
-      <c r="K75" t="s">
-        <v>470</v>
-      </c>
-      <c r="L75" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="B76" t="s">
-        <v>226</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="G76" t="s">
-        <v>470</v>
-      </c>
-      <c r="H76" t="s">
-        <v>470</v>
-      </c>
-      <c r="I76" t="s">
-        <v>470</v>
-      </c>
-      <c r="J76" t="s">
-        <v>470</v>
-      </c>
-      <c r="K76" t="s">
-        <v>470</v>
+      <c r="G76" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J76" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K76" s="7" t="s">
+        <v>469</v>
       </c>
       <c r="L76" s="7" t="s">
         <v>348</v>
@@ -6460,13 +6565,13 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="B77" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="G77" t="s">
         <v>470</v>
@@ -6489,13 +6594,13 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B78" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="G78" t="s">
         <v>470</v>
@@ -6518,13 +6623,13 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B79" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="G79" t="s">
         <v>470</v>
@@ -6547,13 +6652,13 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B80" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="G80" t="s">
         <v>470</v>
@@ -6576,13 +6681,13 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B81" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="G81" t="s">
         <v>470</v>
@@ -6604,384 +6709,304 @@
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>312</v>
+      <c r="A82" s="5" t="s">
+        <v>288</v>
       </c>
       <c r="B82" t="s">
-        <v>588</v>
+        <v>218</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I82" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J82" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K82" s="7" t="s">
-        <v>339</v>
+        <v>219</v>
+      </c>
+      <c r="G82" t="s">
+        <v>470</v>
+      </c>
+      <c r="H82" t="s">
+        <v>470</v>
+      </c>
+      <c r="I82" t="s">
+        <v>470</v>
+      </c>
+      <c r="J82" t="s">
+        <v>470</v>
+      </c>
+      <c r="K82" t="s">
+        <v>470</v>
       </c>
       <c r="L82" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M82" s="7"/>
-      <c r="N82" s="7"/>
-      <c r="O82" s="6"/>
-      <c r="P82" s="7"/>
-      <c r="Q82" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>313</v>
+      <c r="A83" s="5" t="s">
+        <v>287</v>
       </c>
       <c r="B83" t="s">
-        <v>589</v>
+        <v>220</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I83" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J83" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K83" s="7" t="s">
-        <v>339</v>
+        <v>221</v>
+      </c>
+      <c r="G83" t="s">
+        <v>470</v>
+      </c>
+      <c r="H83" t="s">
+        <v>470</v>
+      </c>
+      <c r="I83" t="s">
+        <v>470</v>
+      </c>
+      <c r="J83" t="s">
+        <v>470</v>
+      </c>
+      <c r="K83" t="s">
+        <v>470</v>
       </c>
       <c r="L83" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M83" s="7"/>
-      <c r="N83" s="7"/>
-      <c r="O83" s="6"/>
-      <c r="P83" s="7"/>
-      <c r="Q83" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
-        <v>314</v>
+      <c r="A84" s="5" t="s">
+        <v>286</v>
       </c>
       <c r="B84" t="s">
-        <v>590</v>
+        <v>222</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H84" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I84" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J84" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K84" s="7" t="s">
-        <v>339</v>
+        <v>223</v>
+      </c>
+      <c r="G84" t="s">
+        <v>470</v>
+      </c>
+      <c r="H84" t="s">
+        <v>470</v>
+      </c>
+      <c r="I84" t="s">
+        <v>470</v>
+      </c>
+      <c r="J84" t="s">
+        <v>470</v>
+      </c>
+      <c r="K84" t="s">
+        <v>470</v>
       </c>
       <c r="L84" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M84" s="7"/>
-      <c r="N84" s="7"/>
-      <c r="O84" s="6"/>
-      <c r="P84" s="7"/>
-      <c r="Q84" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A85" s="15" t="s">
-        <v>514</v>
+      <c r="A85" s="5" t="s">
+        <v>285</v>
       </c>
       <c r="B85" t="s">
-        <v>591</v>
+        <v>224</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H85" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I85" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J85" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K85" s="7" t="s">
-        <v>339</v>
+        <v>225</v>
+      </c>
+      <c r="G85" t="s">
+        <v>470</v>
+      </c>
+      <c r="H85" t="s">
+        <v>470</v>
+      </c>
+      <c r="I85" t="s">
+        <v>470</v>
+      </c>
+      <c r="J85" t="s">
+        <v>470</v>
+      </c>
+      <c r="K85" t="s">
+        <v>470</v>
       </c>
       <c r="L85" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M85" s="7"/>
-      <c r="N85" s="7"/>
-      <c r="O85" s="6"/>
-      <c r="P85" s="7"/>
-      <c r="Q85" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A86" s="15" t="s">
-        <v>276</v>
+      <c r="A86" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="B86" t="s">
-        <v>592</v>
+        <v>226</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I86" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J86" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K86" s="7" t="s">
-        <v>339</v>
+        <v>227</v>
+      </c>
+      <c r="G86" t="s">
+        <v>470</v>
+      </c>
+      <c r="H86" t="s">
+        <v>470</v>
+      </c>
+      <c r="I86" t="s">
+        <v>470</v>
+      </c>
+      <c r="J86" t="s">
+        <v>470</v>
+      </c>
+      <c r="K86" t="s">
+        <v>470</v>
       </c>
       <c r="L86" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M86" s="7"/>
-      <c r="N86" s="7"/>
-      <c r="O86" s="6"/>
-      <c r="P86" s="7"/>
-      <c r="Q86" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
-        <v>277</v>
+      <c r="A87" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="B87" t="s">
-        <v>593</v>
+        <v>228</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I87" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J87" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K87" s="7" t="s">
-        <v>339</v>
+        <v>229</v>
+      </c>
+      <c r="G87" t="s">
+        <v>470</v>
+      </c>
+      <c r="H87" t="s">
+        <v>470</v>
+      </c>
+      <c r="I87" t="s">
+        <v>470</v>
+      </c>
+      <c r="J87" t="s">
+        <v>470</v>
+      </c>
+      <c r="K87" t="s">
+        <v>470</v>
       </c>
       <c r="L87" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M87" s="7"/>
-      <c r="N87" s="7"/>
-      <c r="O87" s="6"/>
-      <c r="P87" s="7"/>
-      <c r="Q87" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
-        <v>278</v>
+      <c r="A88" s="5" t="s">
+        <v>294</v>
       </c>
       <c r="B88" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H88" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I88" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J88" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K88" s="7" t="s">
-        <v>339</v>
+        <v>231</v>
+      </c>
+      <c r="G88" t="s">
+        <v>470</v>
+      </c>
+      <c r="H88" t="s">
+        <v>470</v>
+      </c>
+      <c r="I88" t="s">
+        <v>470</v>
+      </c>
+      <c r="J88" t="s">
+        <v>470</v>
+      </c>
+      <c r="K88" t="s">
+        <v>470</v>
       </c>
       <c r="L88" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M88" s="7"/>
-      <c r="N88" s="7"/>
-      <c r="O88" s="6"/>
-      <c r="P88" s="7"/>
-      <c r="Q88" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A89" s="15" t="s">
-        <v>279</v>
+      <c r="A89" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="B89" t="s">
-        <v>594</v>
+        <v>232</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H89" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I89" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J89" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K89" s="7" t="s">
-        <v>339</v>
+        <v>233</v>
+      </c>
+      <c r="G89" t="s">
+        <v>470</v>
+      </c>
+      <c r="H89" t="s">
+        <v>470</v>
+      </c>
+      <c r="I89" t="s">
+        <v>470</v>
+      </c>
+      <c r="J89" t="s">
+        <v>470</v>
+      </c>
+      <c r="K89" t="s">
+        <v>470</v>
       </c>
       <c r="L89" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M89" s="7"/>
-      <c r="N89" s="7"/>
-      <c r="O89" s="6"/>
-      <c r="P89" s="7"/>
-      <c r="Q89" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A90" s="15" t="s">
-        <v>280</v>
+      <c r="A90" s="5" t="s">
+        <v>296</v>
       </c>
       <c r="B90" t="s">
-        <v>595</v>
+        <v>234</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I90" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J90" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K90" s="7" t="s">
-        <v>339</v>
+        <v>235</v>
+      </c>
+      <c r="G90" t="s">
+        <v>470</v>
+      </c>
+      <c r="H90" t="s">
+        <v>470</v>
+      </c>
+      <c r="I90" t="s">
+        <v>470</v>
+      </c>
+      <c r="J90" t="s">
+        <v>470</v>
+      </c>
+      <c r="K90" t="s">
+        <v>470</v>
       </c>
       <c r="L90" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M90" s="7"/>
-      <c r="N90" s="7"/>
-      <c r="O90" s="6"/>
-      <c r="P90" s="7"/>
-      <c r="Q90" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A91" s="15" t="s">
-        <v>282</v>
+      <c r="A91" s="5" t="s">
+        <v>295</v>
       </c>
       <c r="B91" t="s">
-        <v>596</v>
+        <v>236</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H91" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I91" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J91" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K91" s="7" t="s">
-        <v>339</v>
+        <v>237</v>
+      </c>
+      <c r="G91" t="s">
+        <v>470</v>
+      </c>
+      <c r="H91" t="s">
+        <v>470</v>
+      </c>
+      <c r="I91" t="s">
+        <v>470</v>
+      </c>
+      <c r="J91" t="s">
+        <v>470</v>
+      </c>
+      <c r="K91" t="s">
+        <v>470</v>
       </c>
       <c r="L91" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M91" s="7"/>
-      <c r="N91" s="7"/>
-      <c r="O91" s="6"/>
-      <c r="P91" s="7"/>
-      <c r="Q91" s="7"/>
+        <v>348</v>
+      </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>268</v>
+        <v>312</v>
       </c>
       <c r="B92" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
@@ -7012,13 +7037,13 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B93" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
@@ -7049,13 +7074,13 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="B94" s="22" t="s">
-        <v>700</v>
+        <v>314</v>
+      </c>
+      <c r="B94" t="s">
+        <v>590</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>701</v>
+        <v>240</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
@@ -7086,13 +7111,13 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
-        <v>281</v>
+        <v>514</v>
       </c>
       <c r="B95" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
@@ -7122,304 +7147,384 @@
       <c r="Q95" s="7"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A96" s="12" t="s">
-        <v>264</v>
+      <c r="A96" s="15" t="s">
+        <v>276</v>
       </c>
       <c r="B96" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>252</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="8"/>
       <c r="G96" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J96" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K96" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L96" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M96" s="7"/>
+      <c r="N96" s="7"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="7"/>
+      <c r="Q96" s="7"/>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A97" s="12" t="s">
-        <v>265</v>
+      <c r="A97" s="15" t="s">
+        <v>277</v>
       </c>
       <c r="B97" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>253</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="8"/>
       <c r="G97" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I97" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J97" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K97" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L97" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M97" s="7"/>
+      <c r="N97" s="7"/>
+      <c r="O97" s="6"/>
+      <c r="P97" s="7"/>
+      <c r="Q97" s="7"/>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A98" s="12" t="s">
-        <v>266</v>
+      <c r="A98" s="15" t="s">
+        <v>278</v>
       </c>
       <c r="B98" t="s">
-        <v>602</v>
+        <v>244</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>256</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="8"/>
       <c r="G98" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I98" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J98" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K98" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L98" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M98" s="7"/>
+      <c r="N98" s="7"/>
+      <c r="O98" s="6"/>
+      <c r="P98" s="7"/>
+      <c r="Q98" s="7"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A99" s="12" t="s">
-        <v>267</v>
+      <c r="A99" s="15" t="s">
+        <v>279</v>
       </c>
       <c r="B99" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>257</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="8"/>
       <c r="G99" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I99" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J99" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K99" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L99" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M99" s="7"/>
+      <c r="N99" s="7"/>
+      <c r="O99" s="6"/>
+      <c r="P99" s="7"/>
+      <c r="Q99" s="7"/>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A100" s="12" t="s">
-        <v>315</v>
+      <c r="A100" s="15" t="s">
+        <v>280</v>
       </c>
       <c r="B100" t="s">
-        <v>597</v>
-      </c>
-      <c r="C100" s="16" t="s">
-        <v>249</v>
-      </c>
+        <v>595</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="8"/>
       <c r="G100" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I100" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J100" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K100" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L100" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M100" s="7"/>
+      <c r="N100" s="7"/>
+      <c r="O100" s="6"/>
+      <c r="P100" s="7"/>
+      <c r="Q100" s="7"/>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A101" s="12" t="s">
-        <v>269</v>
+      <c r="A101" s="15" t="s">
+        <v>282</v>
       </c>
       <c r="B101" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>258</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="8"/>
       <c r="G101" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I101" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K101" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L101" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M101" s="7"/>
+      <c r="N101" s="7"/>
+      <c r="O101" s="6"/>
+      <c r="P101" s="7"/>
+      <c r="Q101" s="7"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
-        <v>270</v>
+      <c r="A102" s="14" t="s">
+        <v>268</v>
       </c>
       <c r="B102" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>254</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="8"/>
       <c r="G102" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I102" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K102" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L102" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M102" s="7"/>
+      <c r="N102" s="7"/>
+      <c r="O102" s="6"/>
+      <c r="P102" s="7"/>
+      <c r="Q102" s="7"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
-        <v>271</v>
+      <c r="A103" s="14" t="s">
+        <v>310</v>
       </c>
       <c r="B103" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>259</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="8"/>
       <c r="G103" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I103" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K103" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L103" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M103" s="7"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="6"/>
+      <c r="P103" s="7"/>
+      <c r="Q103" s="7"/>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="B104" t="s">
-        <v>607</v>
+      <c r="A104" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B104" s="22" t="s">
+        <v>700</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>260</v>
-      </c>
+        <v>701</v>
+      </c>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="8"/>
       <c r="G104" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J104" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K104" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L104" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M104" s="7"/>
+      <c r="N104" s="7"/>
+      <c r="O104" s="6"/>
+      <c r="P104" s="7"/>
+      <c r="Q104" s="7"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
-        <v>273</v>
+      <c r="A105" s="15" t="s">
+        <v>281</v>
       </c>
       <c r="B105" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>261</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="8"/>
       <c r="G105" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="I105" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="J105" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="K105" s="7" t="s">
-        <v>469</v>
+        <v>339</v>
       </c>
       <c r="L105" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="M105" s="7"/>
+      <c r="N105" s="7"/>
+      <c r="O105" s="6"/>
+      <c r="P105" s="7"/>
+      <c r="Q105" s="7"/>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="B106" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G106" s="7" t="s">
         <v>469</v>
@@ -7442,13 +7547,13 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B107" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="G107" s="7" t="s">
         <v>469</v>
@@ -7470,834 +7575,726 @@
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>307</v>
+      <c r="A108" s="12" t="s">
+        <v>266</v>
       </c>
       <c r="B108" t="s">
-        <v>298</v>
-      </c>
-      <c r="C108" t="s">
-        <v>299</v>
-      </c>
-      <c r="E108" s="13" t="s">
-        <v>544</v>
-      </c>
-      <c r="G108" t="s">
-        <v>472</v>
-      </c>
-      <c r="J108" t="s">
-        <v>472</v>
-      </c>
-      <c r="K108" t="s">
-        <v>472</v>
-      </c>
-      <c r="L108" t="s">
-        <v>471</v>
+        <v>602</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G108" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H108" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I108" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J108" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K108" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L108" s="7" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>306</v>
+      <c r="A109" s="12" t="s">
+        <v>267</v>
       </c>
       <c r="B109" t="s">
-        <v>300</v>
-      </c>
-      <c r="C109" t="s">
-        <v>301</v>
-      </c>
-      <c r="E109" s="13" t="s">
-        <v>544</v>
-      </c>
-      <c r="G109" t="s">
-        <v>473</v>
-      </c>
-      <c r="J109" t="s">
-        <v>473</v>
-      </c>
-      <c r="K109" t="s">
-        <v>473</v>
-      </c>
-      <c r="L109" t="s">
-        <v>471</v>
+        <v>603</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I109" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K109" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L109" s="7" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>540</v>
+      <c r="A110" s="12" t="s">
+        <v>315</v>
       </c>
       <c r="B110" t="s">
-        <v>302</v>
-      </c>
-      <c r="C110" t="s">
-        <v>303</v>
-      </c>
-      <c r="D110" t="s">
-        <v>641</v>
-      </c>
-      <c r="E110" s="13" t="s">
-        <v>544</v>
-      </c>
-      <c r="G110" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="J110" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="K110" s="17"/>
-      <c r="L110" t="s">
-        <v>471</v>
-      </c>
-      <c r="M110" t="s">
-        <v>632</v>
-      </c>
-      <c r="N110" t="s">
-        <v>633</v>
-      </c>
-      <c r="O110" t="s">
-        <v>634</v>
-      </c>
-      <c r="P110" t="s">
-        <v>631</v>
-      </c>
-      <c r="Q110" t="s">
-        <v>635</v>
+        <v>597</v>
+      </c>
+      <c r="C110" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="G110" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H110" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I110" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J110" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K110" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L110" s="7" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>541</v>
+      <c r="A111" s="12" t="s">
+        <v>269</v>
       </c>
       <c r="B111" t="s">
-        <v>304</v>
-      </c>
-      <c r="C111" t="s">
-        <v>305</v>
-      </c>
-      <c r="D111" t="s">
-        <v>641</v>
-      </c>
-      <c r="E111" s="13" t="s">
-        <v>544</v>
-      </c>
-      <c r="G111" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="J111" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="K111" s="17"/>
-      <c r="L111" t="s">
-        <v>471</v>
-      </c>
-      <c r="M111" t="s">
-        <v>632</v>
-      </c>
-      <c r="N111" t="s">
-        <v>633</v>
-      </c>
-      <c r="O111" t="s">
-        <v>634</v>
-      </c>
-      <c r="P111" t="s">
-        <v>631</v>
-      </c>
-      <c r="Q111" t="s">
-        <v>635</v>
+        <v>604</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G111" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I111" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="L111" s="7" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
-        <v>319</v>
+      <c r="A112" s="12" t="s">
+        <v>270</v>
       </c>
       <c r="B112" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-      <c r="F112" s="7"/>
+        <v>254</v>
+      </c>
       <c r="G112" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="I112" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="J112" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="K112" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="L112" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="M112" s="7"/>
-      <c r="N112" s="7"/>
-      <c r="O112" s="7"/>
-      <c r="P112" s="7"/>
-      <c r="Q112" s="7"/>
+        <v>341</v>
+      </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>320</v>
+      <c r="A113" s="12" t="s">
+        <v>271</v>
       </c>
       <c r="B113" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-      <c r="F113" s="7"/>
+        <v>259</v>
+      </c>
       <c r="G113" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="I113" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="J113" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="K113" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="L113" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="M113" s="7"/>
-      <c r="N113" s="7"/>
-      <c r="O113" s="7"/>
-      <c r="P113" s="7"/>
-      <c r="Q113" s="7"/>
+        <v>341</v>
+      </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>321</v>
+      <c r="A114" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="B114" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-      <c r="F114" s="7"/>
+        <v>260</v>
+      </c>
       <c r="G114" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="I114" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="J114" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="K114" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="L114" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="M114" s="7"/>
-      <c r="N114" s="7"/>
-      <c r="O114" s="7"/>
-      <c r="P114" s="7"/>
-      <c r="Q114" s="7"/>
+        <v>341</v>
+      </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>322</v>
+      <c r="A115" s="12" t="s">
+        <v>273</v>
       </c>
       <c r="B115" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
-      <c r="F115" s="7"/>
+        <v>261</v>
+      </c>
       <c r="G115" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="I115" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="J115" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="K115" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="L115" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="M115" s="7"/>
-      <c r="N115" s="7"/>
-      <c r="O115" s="7"/>
-      <c r="P115" s="7"/>
-      <c r="Q115" s="7"/>
+        <v>341</v>
+      </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>323</v>
+      <c r="A116" s="12" t="s">
+        <v>274</v>
       </c>
       <c r="B116" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
-      <c r="F116" s="7"/>
+        <v>255</v>
+      </c>
       <c r="G116" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="I116" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="J116" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="K116" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="L116" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="M116" s="7"/>
-      <c r="N116" s="7"/>
-      <c r="O116" s="7"/>
-      <c r="P116" s="7"/>
-      <c r="Q116" s="7"/>
+        <v>341</v>
+      </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>324</v>
+      <c r="A117" s="12" t="s">
+        <v>275</v>
       </c>
       <c r="B117" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D117" s="7"/>
-      <c r="E117" s="7"/>
-      <c r="F117" s="7"/>
+        <v>262</v>
+      </c>
       <c r="G117" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="I117" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="J117" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="K117" s="7" t="s">
-        <v>339</v>
+        <v>469</v>
       </c>
       <c r="L117" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="M117" s="7"/>
-      <c r="N117" s="7"/>
-      <c r="O117" s="7"/>
-      <c r="P117" s="7"/>
-      <c r="Q117" s="7"/>
+        <v>341</v>
+      </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="B118" t="s">
-        <v>617</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
-      <c r="F118" s="7"/>
-      <c r="G118" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H118" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I118" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="J118" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="K118" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="L118" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="M118" s="7"/>
-      <c r="N118" s="7"/>
-      <c r="O118" s="7"/>
-      <c r="P118" s="7"/>
-      <c r="Q118" s="7"/>
+        <v>298</v>
+      </c>
+      <c r="C118" t="s">
+        <v>299</v>
+      </c>
+      <c r="E118" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="G118" t="s">
+        <v>472</v>
+      </c>
+      <c r="J118" t="s">
+        <v>472</v>
+      </c>
+      <c r="K118" t="s">
+        <v>472</v>
+      </c>
+      <c r="L118" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>503</v>
+        <v>306</v>
       </c>
       <c r="B119" t="s">
-        <v>509</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="D119" t="s">
-        <v>641</v>
-      </c>
-      <c r="E119" t="s">
-        <v>628</v>
-      </c>
-      <c r="G119" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="J119" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="L119" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M119" t="s">
-        <v>668</v>
-      </c>
-      <c r="N119" t="s">
-        <v>637</v>
-      </c>
-      <c r="O119" t="s">
-        <v>668</v>
-      </c>
-      <c r="P119" t="s">
-        <v>631</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>638</v>
+        <v>300</v>
+      </c>
+      <c r="C119" t="s">
+        <v>301</v>
+      </c>
+      <c r="E119" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="G119" t="s">
+        <v>473</v>
+      </c>
+      <c r="J119" t="s">
+        <v>473</v>
+      </c>
+      <c r="K119" t="s">
+        <v>473</v>
+      </c>
+      <c r="L119" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>504</v>
+        <v>540</v>
       </c>
       <c r="B120" t="s">
-        <v>509</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>511</v>
+        <v>302</v>
+      </c>
+      <c r="C120" t="s">
+        <v>303</v>
       </c>
       <c r="D120" t="s">
         <v>641</v>
       </c>
-      <c r="E120" t="s">
-        <v>628</v>
-      </c>
-      <c r="G120" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="J120" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="L120" s="7" t="s">
-        <v>341</v>
+      <c r="E120" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="G120" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="J120" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="K120" s="17"/>
+      <c r="L120" t="s">
+        <v>471</v>
       </c>
       <c r="M120" t="s">
-        <v>668</v>
+        <v>632</v>
       </c>
       <c r="N120" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="O120" t="s">
-        <v>668</v>
+        <v>634</v>
       </c>
       <c r="P120" t="s">
         <v>631</v>
       </c>
       <c r="Q120" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>505</v>
+        <v>541</v>
       </c>
       <c r="B121" t="s">
-        <v>509</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>511</v>
+        <v>304</v>
+      </c>
+      <c r="C121" t="s">
+        <v>305</v>
       </c>
       <c r="D121" t="s">
         <v>641</v>
       </c>
-      <c r="E121" t="s">
-        <v>628</v>
-      </c>
-      <c r="G121" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="J121" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="L121" s="7" t="s">
-        <v>341</v>
+      <c r="E121" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="G121" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="J121" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="K121" s="17"/>
+      <c r="L121" t="s">
+        <v>471</v>
       </c>
       <c r="M121" t="s">
-        <v>668</v>
+        <v>632</v>
       </c>
       <c r="N121" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="O121" t="s">
-        <v>668</v>
+        <v>634</v>
       </c>
       <c r="P121" t="s">
         <v>631</v>
       </c>
       <c r="Q121" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>506</v>
+        <v>319</v>
       </c>
       <c r="B122" t="s">
-        <v>509</v>
+        <v>611</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="D122" t="s">
-        <v>641</v>
-      </c>
-      <c r="E122" t="s">
-        <v>628</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="D122" s="7"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="7"/>
       <c r="G122" s="7" t="s">
-        <v>627</v>
+        <v>339</v>
+      </c>
+      <c r="H122" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I122" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="J122" s="7" t="s">
-        <v>627</v>
+        <v>339</v>
+      </c>
+      <c r="K122" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="L122" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M122" t="s">
-        <v>668</v>
-      </c>
-      <c r="N122" t="s">
-        <v>637</v>
-      </c>
-      <c r="O122" t="s">
-        <v>668</v>
-      </c>
-      <c r="P122" t="s">
-        <v>631</v>
-      </c>
-      <c r="Q122" t="s">
-        <v>638</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="M122" s="7"/>
+      <c r="N122" s="7"/>
+      <c r="O122" s="7"/>
+      <c r="P122" s="7"/>
+      <c r="Q122" s="7"/>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>510</v>
+        <v>320</v>
       </c>
       <c r="B123" t="s">
-        <v>509</v>
+        <v>612</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="D123" t="s">
-        <v>641</v>
-      </c>
-      <c r="E123" t="s">
-        <v>628</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7"/>
       <c r="G123" s="7" t="s">
-        <v>627</v>
+        <v>339</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I123" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="J123" s="7" t="s">
-        <v>627</v>
+        <v>339</v>
+      </c>
+      <c r="K123" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="L123" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M123" t="s">
-        <v>668</v>
-      </c>
-      <c r="N123" t="s">
-        <v>637</v>
-      </c>
-      <c r="O123" t="s">
-        <v>668</v>
-      </c>
-      <c r="P123" t="s">
-        <v>631</v>
-      </c>
-      <c r="Q123" t="s">
-        <v>638</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="M123" s="7"/>
+      <c r="N123" s="7"/>
+      <c r="O123" s="7"/>
+      <c r="P123" s="7"/>
+      <c r="Q123" s="7"/>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>507</v>
+        <v>321</v>
       </c>
       <c r="B124" t="s">
-        <v>512</v>
+        <v>613</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="D124" t="s">
-        <v>641</v>
-      </c>
-      <c r="E124" t="s">
-        <v>628</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
       <c r="G124" s="7" t="s">
-        <v>627</v>
+        <v>339</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I124" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="J124" s="7" t="s">
-        <v>627</v>
+        <v>339</v>
+      </c>
+      <c r="K124" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="L124" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M124" t="s">
-        <v>636</v>
-      </c>
-      <c r="N124" t="s">
-        <v>637</v>
-      </c>
-      <c r="O124" t="s">
-        <v>628</v>
-      </c>
-      <c r="P124" t="s">
-        <v>631</v>
-      </c>
-      <c r="Q124" t="s">
-        <v>638</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="M124" s="7"/>
+      <c r="N124" s="7"/>
+      <c r="O124" s="7"/>
+      <c r="P124" s="7"/>
+      <c r="Q124" s="7"/>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>508</v>
+        <v>322</v>
       </c>
       <c r="B125" t="s">
-        <v>512</v>
+        <v>614</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="D125" t="s">
-        <v>641</v>
-      </c>
-      <c r="E125" t="s">
-        <v>628</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
       <c r="G125" s="7" t="s">
-        <v>627</v>
+        <v>339</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I125" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>627</v>
+        <v>339</v>
+      </c>
+      <c r="K125" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="L125" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M125" t="s">
-        <v>669</v>
-      </c>
-      <c r="N125" t="s">
-        <v>637</v>
-      </c>
-      <c r="O125" t="s">
-        <v>628</v>
-      </c>
-      <c r="P125" t="s">
-        <v>631</v>
-      </c>
-      <c r="Q125" t="s">
-        <v>638</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="M125" s="7"/>
+      <c r="N125" s="7"/>
+      <c r="O125" s="7"/>
+      <c r="P125" s="7"/>
+      <c r="Q125" s="7"/>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>521</v>
+        <v>323</v>
       </c>
       <c r="B126" t="s">
-        <v>522</v>
+        <v>615</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>523</v>
-      </c>
-      <c r="D126" t="s">
-        <v>642</v>
-      </c>
-      <c r="E126" t="s">
-        <v>628</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="7"/>
       <c r="G126" s="7" t="s">
-        <v>542</v>
+        <v>339</v>
+      </c>
+      <c r="H126" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I126" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="J126" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="K126" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="L126" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M126" t="s">
-        <v>628</v>
-      </c>
-      <c r="N126" t="s">
-        <v>628</v>
-      </c>
-      <c r="O126" t="s">
-        <v>628</v>
-      </c>
-      <c r="P126" t="s">
-        <v>629</v>
-      </c>
-      <c r="Q126" t="s">
-        <v>639</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="M126" s="7"/>
+      <c r="N126" s="7"/>
+      <c r="O126" s="7"/>
+      <c r="P126" s="7"/>
+      <c r="Q126" s="7"/>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>538</v>
+        <v>324</v>
       </c>
       <c r="B127" t="s">
-        <v>524</v>
+        <v>616</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>525</v>
-      </c>
-      <c r="D127" t="s">
-        <v>642</v>
-      </c>
-      <c r="E127" t="s">
-        <v>628</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7"/>
       <c r="G127" s="7" t="s">
-        <v>542</v>
+        <v>339</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I127" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="J127" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="K127" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="L127" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M127" t="s">
-        <v>628</v>
-      </c>
-      <c r="N127" t="s">
-        <v>628</v>
-      </c>
-      <c r="O127" t="s">
-        <v>628</v>
-      </c>
-      <c r="P127" t="s">
-        <v>629</v>
-      </c>
-      <c r="Q127" t="s">
-        <v>639</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="M127" s="7"/>
+      <c r="N127" s="7"/>
+      <c r="O127" s="7"/>
+      <c r="P127" s="7"/>
+      <c r="Q127" s="7"/>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>526</v>
+        <v>325</v>
       </c>
       <c r="B128" t="s">
-        <v>527</v>
+        <v>617</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="D128" t="s">
-        <v>642</v>
-      </c>
-      <c r="E128" t="s">
-        <v>628</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="D128" s="7"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="7"/>
       <c r="G128" s="7" t="s">
-        <v>529</v>
+        <v>339</v>
+      </c>
+      <c r="H128" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I128" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="J128" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="K128" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="L128" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M128" t="s">
-        <v>628</v>
-      </c>
-      <c r="N128" t="s">
-        <v>628</v>
-      </c>
-      <c r="O128" t="s">
-        <v>628</v>
-      </c>
-      <c r="P128" t="s">
-        <v>629</v>
-      </c>
-      <c r="Q128" t="s">
-        <v>638</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="M128" s="7"/>
+      <c r="N128" s="7"/>
+      <c r="O128" s="7"/>
+      <c r="P128" s="7"/>
+      <c r="Q128" s="7"/>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>539</v>
+        <v>503</v>
       </c>
       <c r="B129" t="s">
-        <v>530</v>
+        <v>509</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>531</v>
+        <v>511</v>
       </c>
       <c r="D129" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E129" t="s">
         <v>628</v>
       </c>
       <c r="G129" s="7" t="s">
-        <v>529</v>
+        <v>627</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>627</v>
       </c>
       <c r="L129" s="7" t="s">
         <v>341</v>
       </c>
       <c r="M129" t="s">
-        <v>628</v>
+        <v>668</v>
       </c>
       <c r="N129" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="O129" t="s">
-        <v>628</v>
+        <v>668</v>
       </c>
       <c r="P129" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="Q129" t="s">
         <v>638</v>
@@ -8305,77 +8302,475 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>532</v>
+        <v>504</v>
       </c>
       <c r="B130" t="s">
-        <v>533</v>
+        <v>509</v>
       </c>
       <c r="C130" s="7" t="s">
-        <v>534</v>
+        <v>511</v>
       </c>
       <c r="D130" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E130" t="s">
         <v>628</v>
       </c>
       <c r="G130" s="7" t="s">
-        <v>543</v>
+        <v>627</v>
+      </c>
+      <c r="J130" s="7" t="s">
+        <v>627</v>
       </c>
       <c r="L130" s="7" t="s">
         <v>341</v>
       </c>
       <c r="M130" t="s">
-        <v>628</v>
+        <v>668</v>
       </c>
       <c r="N130" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="O130" t="s">
-        <v>630</v>
+        <v>668</v>
       </c>
       <c r="P130" t="s">
         <v>631</v>
       </c>
       <c r="Q130" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>537</v>
+        <v>505</v>
       </c>
       <c r="B131" t="s">
-        <v>535</v>
+        <v>509</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>536</v>
+        <v>511</v>
       </c>
       <c r="D131" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E131" t="s">
         <v>628</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>543</v>
+        <v>627</v>
+      </c>
+      <c r="J131" s="7" t="s">
+        <v>627</v>
       </c>
       <c r="L131" s="7" t="s">
         <v>341</v>
       </c>
       <c r="M131" t="s">
-        <v>628</v>
+        <v>668</v>
       </c>
       <c r="N131" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="O131" t="s">
-        <v>630</v>
+        <v>668</v>
       </c>
       <c r="P131" t="s">
         <v>631</v>
       </c>
       <c r="Q131" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B132" t="s">
+        <v>509</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="D132" t="s">
+        <v>641</v>
+      </c>
+      <c r="E132" t="s">
+        <v>628</v>
+      </c>
+      <c r="G132" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="J132" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="L132" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M132" t="s">
+        <v>668</v>
+      </c>
+      <c r="N132" t="s">
+        <v>637</v>
+      </c>
+      <c r="O132" t="s">
+        <v>668</v>
+      </c>
+      <c r="P132" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="B133" t="s">
+        <v>509</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="D133" t="s">
+        <v>641</v>
+      </c>
+      <c r="E133" t="s">
+        <v>628</v>
+      </c>
+      <c r="G133" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="J133" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="L133" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M133" t="s">
+        <v>668</v>
+      </c>
+      <c r="N133" t="s">
+        <v>637</v>
+      </c>
+      <c r="O133" t="s">
+        <v>668</v>
+      </c>
+      <c r="P133" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B134" t="s">
+        <v>512</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="D134" t="s">
+        <v>641</v>
+      </c>
+      <c r="E134" t="s">
+        <v>628</v>
+      </c>
+      <c r="G134" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="J134" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="L134" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M134" t="s">
+        <v>636</v>
+      </c>
+      <c r="N134" t="s">
+        <v>637</v>
+      </c>
+      <c r="O134" t="s">
+        <v>628</v>
+      </c>
+      <c r="P134" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B135" t="s">
+        <v>512</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="D135" t="s">
+        <v>641</v>
+      </c>
+      <c r="E135" t="s">
+        <v>628</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="J135" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="L135" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M135" t="s">
+        <v>669</v>
+      </c>
+      <c r="N135" t="s">
+        <v>637</v>
+      </c>
+      <c r="O135" t="s">
+        <v>628</v>
+      </c>
+      <c r="P135" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="B136" t="s">
+        <v>522</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="D136" t="s">
+        <v>642</v>
+      </c>
+      <c r="E136" t="s">
+        <v>628</v>
+      </c>
+      <c r="G136" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="L136" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M136" t="s">
+        <v>628</v>
+      </c>
+      <c r="N136" t="s">
+        <v>628</v>
+      </c>
+      <c r="O136" t="s">
+        <v>628</v>
+      </c>
+      <c r="P136" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="B137" t="s">
+        <v>524</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="D137" t="s">
+        <v>642</v>
+      </c>
+      <c r="E137" t="s">
+        <v>628</v>
+      </c>
+      <c r="G137" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="L137" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M137" t="s">
+        <v>628</v>
+      </c>
+      <c r="N137" t="s">
+        <v>628</v>
+      </c>
+      <c r="O137" t="s">
+        <v>628</v>
+      </c>
+      <c r="P137" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="B138" t="s">
+        <v>527</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="D138" t="s">
+        <v>642</v>
+      </c>
+      <c r="E138" t="s">
+        <v>628</v>
+      </c>
+      <c r="G138" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="L138" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M138" t="s">
+        <v>628</v>
+      </c>
+      <c r="N138" t="s">
+        <v>628</v>
+      </c>
+      <c r="O138" t="s">
+        <v>628</v>
+      </c>
+      <c r="P138" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="B139" t="s">
+        <v>530</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="D139" t="s">
+        <v>642</v>
+      </c>
+      <c r="E139" t="s">
+        <v>628</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="L139" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M139" t="s">
+        <v>628</v>
+      </c>
+      <c r="N139" t="s">
+        <v>628</v>
+      </c>
+      <c r="O139" t="s">
+        <v>628</v>
+      </c>
+      <c r="P139" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B140" t="s">
+        <v>533</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="D140" t="s">
+        <v>642</v>
+      </c>
+      <c r="E140" t="s">
+        <v>628</v>
+      </c>
+      <c r="G140" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="L140" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M140" t="s">
+        <v>628</v>
+      </c>
+      <c r="N140" t="s">
+        <v>628</v>
+      </c>
+      <c r="O140" t="s">
+        <v>630</v>
+      </c>
+      <c r="P140" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="B141" t="s">
+        <v>535</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="D141" t="s">
+        <v>642</v>
+      </c>
+      <c r="E141" t="s">
+        <v>628</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="L141" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M141" t="s">
+        <v>628</v>
+      </c>
+      <c r="N141" t="s">
+        <v>628</v>
+      </c>
+      <c r="O141" t="s">
+        <v>630</v>
+      </c>
+      <c r="P141" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q141" t="s">
         <v>640</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected unik_parameterkod in codelist
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist.xlsx
+++ b/inst/extdata/codelist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\NA\MAF\MAF_Privat\Miljogifter\mg_analys\SGU\Mocis2_temp\MoCiS2\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\NA\MAF\MAF_Privat\Miljogifter\mg_analys\SGU\MoCiS2_temp\MoCiS2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8848E9BF-040B-4B87-B750-CD92AE9E1CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB86AA4-C9D0-4864-941D-8F50854E7060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="60" windowWidth="23475" windowHeight="15210" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="120" windowWidth="27435" windowHeight="16635" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -2174,9 +2174,6 @@
     <t>PFHXDA</t>
   </si>
   <si>
-    <t>2,3,3,3-Tetrafluor-2-(1,1,2,2,3,3,3-heptafluorpropoxy)propansyra</t>
-  </si>
-  <si>
     <t>Dodekafluor-3H-4,8-dioxanonansyra</t>
   </si>
   <si>
@@ -2204,9 +2201,6 @@
     <t>Perfluorhexadekansyra (PFHxDA), linjär</t>
   </si>
   <si>
-    <t>CH07/813</t>
-  </si>
-  <si>
     <t>CH07/814</t>
   </si>
   <si>
@@ -2232,6 +2226,12 @@
   </si>
   <si>
     <t>CH07/558</t>
+  </si>
+  <si>
+    <t>Hexafluorpropylenoxiddimersyra (HFPO-DA/FRD-903)</t>
+  </si>
+  <si>
+    <t>CH07/895</t>
   </si>
 </sst>
 </file>
@@ -2380,7 +2380,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2433,6 +2433,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -4311,7 +4312,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5784,11 +5785,11 @@
       <c r="A50" t="s">
         <v>702</v>
       </c>
-      <c r="B50" t="s">
-        <v>712</v>
+      <c r="B50" s="24" t="s">
+        <v>730</v>
       </c>
       <c r="C50" t="s">
-        <v>722</v>
+        <v>731</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>467</v>
@@ -5814,10 +5815,10 @@
         <v>703</v>
       </c>
       <c r="B51" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C51" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>467</v>
@@ -5843,10 +5844,10 @@
         <v>704</v>
       </c>
       <c r="B52" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C52" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>467</v>
@@ -5872,10 +5873,10 @@
         <v>705</v>
       </c>
       <c r="B53" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C53" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>467</v>
@@ -5901,10 +5902,10 @@
         <v>706</v>
       </c>
       <c r="B54" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C54" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="G54" s="7" t="s">
         <v>467</v>
@@ -5930,10 +5931,10 @@
         <v>707</v>
       </c>
       <c r="B55" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C55" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="G55" s="7" t="s">
         <v>467</v>
@@ -5959,10 +5960,10 @@
         <v>708</v>
       </c>
       <c r="B56" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C56" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>467</v>
@@ -5988,10 +5989,10 @@
         <v>709</v>
       </c>
       <c r="B57" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C57" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>467</v>
@@ -6017,10 +6018,10 @@
         <v>710</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G58" s="7" t="s">
         <v>467</v>
@@ -6046,10 +6047,10 @@
         <v>711</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>467</v>

</xml_diff>